<commit_message>
add comments on the differences from using different numbers of CPUs. The reason is caused by MPI_ALLREDUCE with operator MPI_SUM
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0DC66B-4CEF-49D9-BE4A-AEB4AF2C0C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581998FF-803A-4426-BD32-6DBA496B91D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" activeTab="1" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
     <sheet name="CHA_RETAU1000" sheetId="4" r:id="rId2"/>
     <sheet name="main" sheetId="2" r:id="rId3"/>
     <sheet name="initsolver" sheetId="3" r:id="rId4"/>
+    <sheet name="note" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="48">
   <si>
     <t>nompi</t>
   </si>
@@ -180,28 +181,7 @@
     <t>dz</t>
   </si>
   <si>
-    <t>CPU1</t>
-  </si>
-  <si>
-    <t>CPU4</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>cans-main-dns</t>
-  </si>
-  <si>
-    <t>cans-dns</t>
-  </si>
-  <si>
-    <t>uni-noise</t>
-  </si>
-  <si>
-    <t>uni</t>
-  </si>
-  <si>
-    <t>deal with Pedro's updates</t>
+    <t>avoid MPI_ALLREDUCE(MPI_SUM) and use -O0 when comparing the results from different numbers of MPI tasks</t>
   </si>
 </sst>
 </file>
@@ -262,7 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -276,9 +256,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -599,7 +576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760F17C5-A88B-45BD-B60F-0BA67AB143DF}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -871,10 +848,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BFF680-E330-4D55-9962-B9A4D02270CE}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -924,7 +901,7 @@
       <c r="J1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="5" t="s">
         <v>35</v>
       </c>
       <c r="L1" s="5" t="s">
@@ -964,7 +941,7 @@
         <f t="shared" ref="J2:J7" si="1">8*(C2/A2)^2</f>
         <v>5.3388888888888887E-3</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="7">
         <f t="shared" ref="K2:K7" si="2">(J2-I2)/I2</f>
         <v>5.7073306229640679E-2</v>
       </c>
@@ -1007,7 +984,7 @@
         <f t="shared" si="1"/>
         <v>5.3180338740944797E-3</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="7">
         <f t="shared" si="2"/>
         <v>5.2944117572788538E-2</v>
       </c>
@@ -1050,7 +1027,7 @@
         <f t="shared" si="1"/>
         <v>5.6137179879604121E-3</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="7">
         <f t="shared" si="2"/>
         <v>0.11148809373500673</v>
       </c>
@@ -1093,7 +1070,7 @@
         <f t="shared" si="1"/>
         <v>4.9496224875012753E-3</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="7">
         <f t="shared" si="2"/>
         <v>-1.9999494962248385E-2</v>
       </c>
@@ -1136,7 +1113,7 @@
         <f t="shared" si="1"/>
         <v>5.1321752882358945E-3</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="7">
         <f t="shared" si="2"/>
         <v>1.6145046842251543E-2</v>
       </c>
@@ -1179,7 +1156,7 @@
         <f t="shared" si="1"/>
         <v>4.9496224875012753E-3</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="7">
         <f t="shared" si="2"/>
         <v>-1.9999494962248385E-2</v>
       </c>
@@ -1251,54 +1228,6 @@
       <c r="G13">
         <f t="shared" si="5"/>
         <v>15.546875</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6">
-      <c r="D17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6">
-      <c r="D18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6">
-      <c r="D20" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6">
-      <c r="D21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="4:6">
-      <c r="D22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="4:6">
-      <c r="D26" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1356,7 +1285,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1384,4 +1313,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B65B28-909F-4DCB-A7FC-99B4B3E29597}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="95.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
natural griding modified and wall model grid added
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D540A5-1107-4090-A985-3B5FE25BF61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7420D354-1F9D-4DCC-B860-81105E0EDF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="2" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" activeTab="4" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
-    <sheet name="CHA_RETAU1000" sheetId="4" r:id="rId2"/>
-    <sheet name="CHA_RETAU5200" sheetId="6" r:id="rId3"/>
-    <sheet name="main" sheetId="2" r:id="rId4"/>
-    <sheet name="initsolver" sheetId="3" r:id="rId5"/>
-    <sheet name="notes" sheetId="5" r:id="rId6"/>
+    <sheet name="CHA_RETAU550" sheetId="7" r:id="rId2"/>
+    <sheet name="CHA_RETAU1000" sheetId="4" r:id="rId3"/>
+    <sheet name="CHA_RETAU5200" sheetId="6" r:id="rId4"/>
+    <sheet name="CHA_RETAU180" sheetId="9" r:id="rId5"/>
+    <sheet name="main" sheetId="2" r:id="rId6"/>
+    <sheet name="initsolver" sheetId="3" r:id="rId7"/>
+    <sheet name="notes" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="73">
   <si>
     <t>nompi</t>
   </si>
@@ -183,24 +185,6 @@
   </si>
   <si>
     <t>avoid MPI_ALLREDUCE(MPI_SUM) and use -O0 when comparing the results from different numbers of MPI tasks</t>
-  </si>
-  <si>
-    <t>opt</t>
-  </si>
-  <si>
-    <t>debug</t>
-  </si>
-  <si>
-    <t>CPG</t>
-  </si>
-  <si>
-    <t>different in force</t>
-  </si>
-  <si>
-    <t>different in mean velocity</t>
-  </si>
-  <si>
-    <t>exactly the same</t>
   </si>
   <si>
     <t>debug, CFR, different in force
@@ -252,6 +236,33 @@
   </si>
   <si>
     <t>#cells</t>
+  </si>
+  <si>
+    <t>dx+</t>
+  </si>
+  <si>
+    <t>dy+</t>
+  </si>
+  <si>
+    <t>dz_w+</t>
+  </si>
+  <si>
+    <t>dz_c+</t>
+  </si>
+  <si>
+    <t>896×512×384</t>
+  </si>
+  <si>
+    <t>using accurate mean bc</t>
+  </si>
+  <si>
+    <t>if correct, wall model prob</t>
+  </si>
+  <si>
+    <t>if incorrect, sgs prob, try dns grids, RETAU180</t>
+  </si>
+  <si>
+    <t>328×192×104</t>
   </si>
 </sst>
 </file>
@@ -316,7 +327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -336,6 +347,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,15 +671,15 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:D30"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="16.453125" customWidth="1"/>
-    <col min="2" max="2" width="27.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.1796875" customWidth="1"/>
-    <col min="4" max="4" width="22.54296875" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" customWidth="1"/>
+    <col min="4" max="4" width="38.26953125" customWidth="1"/>
     <col min="5" max="5" width="28.54296875" customWidth="1"/>
     <col min="6" max="6" width="14.90625" customWidth="1"/>
   </cols>
@@ -917,48 +934,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="B27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" t="s">
-        <v>51</v>
-      </c>
-    </row>
     <row r="29" spans="1:5">
       <c r="B29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
       <c r="B30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -968,11 +954,599 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3643DFC1-43AF-4E64-819A-C97D29654F85}">
+  <dimension ref="A1:R15"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="14.08984375" customWidth="1"/>
+    <col min="13" max="13" width="10.81640625" customWidth="1"/>
+    <col min="15" max="15" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.08984375" customWidth="1"/>
+    <col min="18" max="18" width="13.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F2">
+        <f>E2</f>
+        <v>0.1</v>
+      </c>
+      <c r="G2" s="5">
+        <f>0.25*F2</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2">
+        <v>0.1</v>
+      </c>
+      <c r="L2" s="8">
+        <f>K2/G2</f>
+        <v>4</v>
+      </c>
+      <c r="M2" s="5">
+        <v>544</v>
+      </c>
+      <c r="O2" s="9">
+        <f>8*(M2/A2)^2</f>
+        <v>5.9187199999999997E-3</v>
+      </c>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="10">
+        <f>(P2-O2)/O2</f>
+        <v>-1</v>
+      </c>
+      <c r="R2" s="8"/>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F3">
+        <f>E3</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G3" s="5">
+        <f>0.25*F3</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3">
+        <v>0.1</v>
+      </c>
+      <c r="L3" s="8">
+        <f t="shared" ref="L3:L10" si="0">K3/G3</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="M3" s="5">
+        <v>544</v>
+      </c>
+      <c r="O3" s="9">
+        <f>8*(M3/A3)^2</f>
+        <v>5.9187199999999997E-3</v>
+      </c>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F4">
+        <f>E4</f>
+        <v>0.05</v>
+      </c>
+      <c r="G4" s="5">
+        <f>0.25*F4</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4">
+        <v>0.1</v>
+      </c>
+      <c r="L4" s="8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M4" s="5">
+        <v>544</v>
+      </c>
+      <c r="O4" s="9">
+        <f>8*(M4/A4)^2</f>
+        <v>5.9187199999999997E-3</v>
+      </c>
+      <c r="P4" s="4"/>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F5">
+        <f>E5</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G5" s="5">
+        <f>0.25*F5</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5">
+        <v>0.1</v>
+      </c>
+      <c r="L5" s="8">
+        <f t="shared" si="0"/>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="M5" s="5">
+        <v>544</v>
+      </c>
+      <c r="O5" s="9">
+        <f>8*(M5/A5)^2</f>
+        <v>5.9187199999999997E-3</v>
+      </c>
+      <c r="P5" s="4"/>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="5"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F7">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="5">
+        <f>0.25*F7</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H7" s="5">
+        <v>2</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7">
+        <v>0.1</v>
+      </c>
+      <c r="L7" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M7" s="5">
+        <v>544</v>
+      </c>
+      <c r="O7" s="9">
+        <f>8*(M7/A7)^2</f>
+        <v>5.9187199999999997E-3</v>
+      </c>
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F8">
+        <f>E8</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G8" s="5">
+        <f>0.25*F8</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8">
+        <v>0.1</v>
+      </c>
+      <c r="L8" s="8">
+        <f t="shared" si="0"/>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="M8" s="5">
+        <v>544</v>
+      </c>
+      <c r="O8" s="9">
+        <f>8*(M8/A8)^2</f>
+        <v>5.9187199999999997E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F9">
+        <f>E9</f>
+        <v>0.05</v>
+      </c>
+      <c r="G9" s="5">
+        <f>0.25*F9</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="H9" s="5">
+        <v>2</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9">
+        <v>0.1</v>
+      </c>
+      <c r="L9" s="8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M9" s="5">
+        <v>544</v>
+      </c>
+      <c r="O9" s="9">
+        <f>8*(M9/A9)^2</f>
+        <v>5.9187199999999997E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F10">
+        <f>E10</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G10" s="5">
+        <f>0.25*F10</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="H10" s="5">
+        <v>2</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10">
+        <v>0.1</v>
+      </c>
+      <c r="L10" s="8">
+        <f t="shared" si="0"/>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="M10" s="5">
+        <v>544</v>
+      </c>
+      <c r="O10" s="9">
+        <f>8*(M10/A10)^2</f>
+        <v>5.9187199999999997E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="12">
+        <f>12.8*M15/880</f>
+        <v>7.9127272727272739</v>
+      </c>
+      <c r="E15">
+        <f>4.8*M15/512</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F15">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="G15">
+        <v>0.06</v>
+      </c>
+      <c r="H15" s="4">
+        <f>D15/E15</f>
+        <v>1.551515151515152</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15">
+        <v>0.1</v>
+      </c>
+      <c r="M15">
+        <v>544</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BFF680-E330-4D55-9962-B9A4D02270CE}">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1102,7 +1676,7 @@
         <v>5.0506325885113761E-3</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J2:J7" si="3">8*(C3/A3)^2</f>
+        <f t="shared" ref="J3:J7" si="3">8*(C3/A3)^2</f>
         <v>5.3180338740944797E-3</v>
       </c>
       <c r="K3" s="7">
@@ -1360,12 +1934,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42F51E-90FA-449F-904F-669D9897EDC7}">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1384,7 +1958,7 @@
     <col min="15" max="15" width="8.6328125" customWidth="1"/>
     <col min="16" max="16" width="10.90625" customWidth="1"/>
     <col min="17" max="17" width="15.453125" customWidth="1"/>
-    <col min="18" max="18" width="18.08984375" customWidth="1"/>
+    <col min="18" max="18" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -1404,16 +1978,16 @@
         <v>45</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>31</v>
@@ -1422,7 +1996,7 @@
         <v>23</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>32</v>
@@ -1448,10 +2022,10 @@
         <v>250000</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D2" s="5">
         <v>0.1</v>
@@ -1471,7 +2045,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>30</v>
@@ -1502,7 +2076,7 @@
         <v>0.1543849482248521</v>
       </c>
       <c r="R2" s="8">
-        <f>100*(2*N2/A2)</f>
+        <f>100*2*N2/A2</f>
         <v>4.4695999999999998</v>
       </c>
       <c r="T2" s="6"/>
@@ -1512,10 +2086,10 @@
         <v>250000</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D3" s="5">
         <v>6.7000000000000004E-2</v>
@@ -1535,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>30</v>
@@ -1550,11 +2124,25 @@
       <c r="M3" s="5">
         <v>5200</v>
       </c>
+      <c r="N3">
+        <v>4998</v>
+      </c>
       <c r="O3">
         <f>8*(M3/A3)^2</f>
         <v>3.4611199999999998E-3</v>
       </c>
-      <c r="P3" s="4"/>
+      <c r="P3" s="9">
+        <f t="shared" ref="P3:P5" si="1">8*(N3/A3)^2</f>
+        <v>3.1974405119999999E-3</v>
+      </c>
+      <c r="Q3" s="10">
+        <f t="shared" ref="Q3:Q5" si="2">(P3-O3)/O3</f>
+        <v>-7.6183284023668627E-2</v>
+      </c>
+      <c r="R3" s="8">
+        <f t="shared" ref="R3:R5" si="3">100*2*N3/A3</f>
+        <v>3.9984000000000002</v>
+      </c>
       <c r="T3" s="6"/>
     </row>
     <row r="4" spans="1:20">
@@ -1562,10 +2150,10 @@
         <v>250000</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D4" s="5">
         <v>0.05</v>
@@ -1585,7 +2173,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>30</v>
@@ -1600,11 +2188,25 @@
       <c r="M4" s="5">
         <v>5200</v>
       </c>
+      <c r="N4">
+        <v>4673</v>
+      </c>
       <c r="O4">
         <f>8*(M4/A4)^2</f>
         <v>3.4611199999999998E-3</v>
       </c>
-      <c r="P4" s="4"/>
+      <c r="P4" s="9">
+        <f t="shared" si="1"/>
+        <v>2.795126912E-3</v>
+      </c>
+      <c r="Q4" s="10">
+        <f t="shared" si="2"/>
+        <v>-0.19242126479289937</v>
+      </c>
+      <c r="R4" s="8">
+        <f t="shared" si="3"/>
+        <v>3.7383999999999999</v>
+      </c>
       <c r="T4" s="6"/>
     </row>
     <row r="5" spans="1:20">
@@ -1612,10 +2214,10 @@
         <v>250000</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="D5" s="5">
         <v>3.3000000000000002E-2</v>
@@ -1635,7 +2237,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>30</v>
@@ -1650,11 +2252,25 @@
       <c r="M5" s="5">
         <v>5200</v>
       </c>
+      <c r="N5">
+        <v>5040</v>
+      </c>
       <c r="O5">
         <f>8*(M5/A5)^2</f>
         <v>3.4611199999999998E-3</v>
       </c>
-      <c r="P5" s="4"/>
+      <c r="P5" s="9">
+        <f t="shared" si="1"/>
+        <v>3.2514048000000001E-3</v>
+      </c>
+      <c r="Q5" s="10">
+        <f t="shared" si="2"/>
+        <v>-6.0591715976331277E-2</v>
+      </c>
+      <c r="R5" s="8">
+        <f t="shared" si="3"/>
+        <v>4.032</v>
+      </c>
       <c r="T5" s="6"/>
     </row>
     <row r="6" spans="1:20">
@@ -1677,13 +2293,13 @@
         <v>250000</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D7" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E7" s="5">
         <v>0.1</v>
@@ -1699,7 +2315,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>30</v>
@@ -1726,13 +2342,14 @@
         <v>250000</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D8" s="5">
-        <v>6.7000000000000004E-2</v>
+        <f>E8*2</f>
+        <v>0.13400000000000001</v>
       </c>
       <c r="E8" s="5">
         <v>6.7000000000000004E-2</v>
@@ -1749,7 +2366,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>30</v>
@@ -1775,13 +2392,14 @@
         <v>250000</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D9" s="5">
-        <v>0.05</v>
+        <f t="shared" ref="D9:D10" si="4">E9*2</f>
+        <v>0.1</v>
       </c>
       <c r="E9" s="5">
         <v>0.05</v>
@@ -1798,7 +2416,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>30</v>
@@ -1824,13 +2442,14 @@
         <v>250000</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D10" s="5">
-        <v>3.3000000000000002E-2</v>
+        <f t="shared" si="4"/>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="E10" s="5">
         <v>3.3000000000000002E-2</v>
@@ -1847,7 +2466,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>30</v>
@@ -1876,7 +2495,139 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797B825A-8F5D-4559-BC02-F7413FCCDF08}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="15.6328125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="17" max="17" width="15.453125" customWidth="1"/>
+    <col min="18" max="18" width="16.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="5">
+        <f>2857*2</f>
+        <v>5714</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="12">
+        <f>12.8*182/328</f>
+        <v>7.102439024390244</v>
+      </c>
+      <c r="E2" s="12">
+        <f>4.8*182/192</f>
+        <v>4.55</v>
+      </c>
+      <c r="F2">
+        <v>6.5</v>
+      </c>
+      <c r="G2">
+        <v>0.05</v>
+      </c>
+      <c r="H2" s="4">
+        <f>D2/E2</f>
+        <v>1.5609756097560976</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>182</v>
+      </c>
+      <c r="O2">
+        <f>8*(M2/A2)^2</f>
+        <v>8.1161915988694072E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9793D359-A47C-4A9C-AA50-6D07B64231AE}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1917,7 +2668,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94B158E-7148-4AB6-B7D0-A5EFE522960E}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -1952,7 +2703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B65B28-909F-4DCB-A7FC-99B4B3E29597}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1973,7 +2724,7 @@
     </row>
     <row r="2" spans="1:1" ht="58">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
delete a line, wall model and neumann bc with the same fixed wall stress produce exactly the same results in debug mode with the explicit schem
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDriveRM\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7420D354-1F9D-4DCC-B860-81105E0EDF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AE0B77-4806-480C-8F76-28BBA246DD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" activeTab="4" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="1310" yWindow="2650" windowWidth="19200" windowHeight="11170" activeTab="4" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="74">
   <si>
     <t>nompi</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>328×192×104</t>
+  </si>
+  <si>
+    <t>du/dz_dns</t>
   </si>
 </sst>
 </file>
@@ -327,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -353,6 +356,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760F17C5-A88B-45BD-B60F-0BA67AB143DF}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -958,7 +962,7 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1938,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42F51E-90FA-449F-904F-669D9897EDC7}">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1959,6 +1963,7 @@
     <col min="16" max="16" width="10.90625" customWidth="1"/>
     <col min="17" max="17" width="15.453125" customWidth="1"/>
     <col min="18" max="18" width="14.7265625" customWidth="1"/>
+    <col min="19" max="19" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -2016,6 +2021,9 @@
       <c r="R1" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="S1" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="5">
@@ -2078,6 +2086,10 @@
       <c r="R2" s="8">
         <f>100*2*N2/A2</f>
         <v>4.4695999999999998</v>
+      </c>
+      <c r="S2">
+        <f>A2/4*O2</f>
+        <v>216.32</v>
       </c>
       <c r="T2" s="6"/>
     </row>
@@ -2497,10 +2509,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797B825A-8F5D-4559-BC02-F7413FCCDF08}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2513,11 +2525,13 @@
     <col min="8" max="8" width="12.26953125" customWidth="1"/>
     <col min="9" max="9" width="13.6328125" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="10.90625" customWidth="1"/>
     <col min="17" max="17" width="15.453125" customWidth="1"/>
     <col min="18" max="18" width="16.08984375" customWidth="1"/>
+    <col min="19" max="19" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="5" t="s">
         <v>24</v>
       </c>
@@ -2572,8 +2586,11 @@
       <c r="R1" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="5">
         <f>2857*2</f>
         <v>5714</v>
@@ -2599,8 +2616,7 @@
         <v>0.05</v>
       </c>
       <c r="H2" s="4">
-        <f>D2/E2</f>
-        <v>1.5609756097560976</v>
+        <v>1.56</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>50</v>
@@ -2620,6 +2636,27 @@
       <c r="O2">
         <f>8*(M2/A2)^2</f>
         <v>8.1161915988694072E-3</v>
+      </c>
+      <c r="S2">
+        <f>2857*O2/2</f>
+        <v>11.593979698984949</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="5">
+        <f>2857*2</f>
+        <v>5714</v>
+      </c>
+      <c r="M3" s="13">
+        <v>180.601843765257</v>
+      </c>
+      <c r="O3">
+        <f>8*(M3/A3)^2</f>
+        <v>7.9919705400696046E-3</v>
+      </c>
+      <c r="S3">
+        <f>2857*O3/2</f>
+        <v>11.416529916489431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wall model accelerated, and robustness increased for two/six walls
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92622A8-BAB5-47B3-92AC-F11AF41A9B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663DBA1A-16CB-4849-B1B9-2AA5B7774062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="13070" windowHeight="15370" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="135">
   <si>
     <t>nompi</t>
   </si>
@@ -461,6 +461,15 @@
   </si>
   <si>
     <t>WM+SMAG+CS0.2</t>
+  </si>
+  <si>
+    <t>WM+SMAG+VISSIMPLE</t>
+  </si>
+  <si>
+    <t>WM+SMAG+CFL0.5</t>
+  </si>
+  <si>
+    <t>WM+SMAG+NODAMP</t>
   </si>
 </sst>
 </file>
@@ -531,7 +540,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -566,6 +575,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -883,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760F17C5-A88B-45BD-B60F-0BA67AB143DF}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1271,7 +1281,7 @@
       </c>
     </row>
     <row r="56" spans="2:2">
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="18" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1461,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797B825A-8F5D-4559-BC02-F7413FCCDF08}">
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2426,13 +2436,13 @@
         <v>11.416529916489431</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2446,7 +2456,7 @@
   <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3256,7 +3266,7 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3644,10 +3654,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42F51E-90FA-449F-904F-669D9897EDC7}">
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:T60"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5154,197 +5164,1035 @@
         <v>215.14822155687202</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
-      <c r="A43" s="5">
+    <row r="33" spans="1:20">
+      <c r="A33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="5">
         <v>250000</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="D33" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F33" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G33">
+        <f>F33</f>
+        <v>0.1</v>
+      </c>
+      <c r="H33" s="5">
+        <f>0.25*G33</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I33" s="5">
+        <v>1</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L33">
+        <v>0.1</v>
+      </c>
+      <c r="M33" s="8">
+        <f>L33/H33</f>
+        <v>4</v>
+      </c>
+      <c r="N33" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O33" s="17">
+        <v>4968.7044767222396</v>
+      </c>
+      <c r="P33">
+        <f>8*(N33/B33)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q33" s="9">
+        <f>8*(O33/B33)^2</f>
+        <v>3.1600670946559523E-3</v>
+      </c>
+      <c r="R33" s="10">
+        <f>(Q33-P33)/P33</f>
+        <v>-8.2008710149672329E-2</v>
+      </c>
+      <c r="S33" s="8">
+        <f>500*2*O33/B33</f>
+        <v>19.874817906888957</v>
+      </c>
+      <c r="T33" s="4">
+        <f>B33/4*P33</f>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="A34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F34" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G34">
+        <f>F34</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H34" s="5">
+        <f>0.25*G34</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I34" s="5">
+        <v>1</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34">
+        <v>0.1</v>
+      </c>
+      <c r="M34" s="8">
+        <f>L34/H34</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N34" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O34" s="17">
+        <v>5151.55007882885</v>
+      </c>
+      <c r="P34">
+        <f>8*(N34/B34)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q34" s="9">
+        <f>8*(O34/B34)^2</f>
+        <v>3.3969239314792362E-3</v>
+      </c>
+      <c r="R34" s="10">
+        <f t="shared" ref="R34:R36" si="20">(Q34-P34)/P34</f>
+        <v>-1.3202413753947324E-2</v>
+      </c>
+      <c r="S34" s="8">
+        <f t="shared" ref="S34:S36" si="21">500*2*O34/B34</f>
+        <v>20.606200315315398</v>
+      </c>
+      <c r="T34" s="4">
+        <f t="shared" ref="T34:T36" si="22">B34/4*P34</f>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20">
+      <c r="A35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G35">
+        <f>F35</f>
+        <v>0.05</v>
+      </c>
+      <c r="H35" s="5">
+        <f>0.25*G35</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I35" s="5">
+        <v>1</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L35">
+        <v>0.1</v>
+      </c>
+      <c r="M35" s="8">
+        <f>L35/H35</f>
+        <v>8</v>
+      </c>
+      <c r="N35" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O35" s="17">
+        <v>5154.6921491920903</v>
+      </c>
+      <c r="P35">
+        <f>8*(N35/B35)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q35" s="9">
+        <f t="shared" ref="Q35:Q36" si="23">8*(O35/B35)^2</f>
+        <v>3.4010689475766484E-3</v>
+      </c>
+      <c r="R35" s="10">
+        <f t="shared" si="20"/>
+        <v>-1.1998297334979957E-2</v>
+      </c>
+      <c r="S35" s="8">
+        <f t="shared" si="21"/>
+        <v>20.618768596768362</v>
+      </c>
+      <c r="T35" s="4">
+        <f t="shared" si="22"/>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20">
+      <c r="A36" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F36" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G36">
+        <f>F36</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H36" s="5">
+        <f>0.25*G36</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I36" s="5">
+        <v>1</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L36">
+        <v>0.1</v>
+      </c>
+      <c r="M36" s="8">
+        <f>L36/H36</f>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N36" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O36" s="17">
+        <v>5164.9259814324196</v>
+      </c>
+      <c r="P36">
+        <f>8*(N36/B36)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q36" s="9">
+        <f t="shared" si="23"/>
+        <v>3.4145869303904824E-3</v>
+      </c>
+      <c r="R36" s="10">
+        <f t="shared" si="20"/>
+        <v>-8.0713584100337785E-3</v>
+      </c>
+      <c r="S36" s="8">
+        <f t="shared" si="21"/>
+        <v>20.659703925729676</v>
+      </c>
+      <c r="T36" s="4">
+        <f t="shared" si="22"/>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20">
+      <c r="A39" t="s">
+        <v>133</v>
+      </c>
+      <c r="B39" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G39">
+        <f>F39</f>
+        <v>0.1</v>
+      </c>
+      <c r="H39" s="5">
+        <f>0.25*G39</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I39" s="5">
+        <v>1</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L39">
+        <v>0.1</v>
+      </c>
+      <c r="M39" s="8">
+        <f>L39/H39</f>
+        <v>4</v>
+      </c>
+      <c r="N39" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O39" s="17">
+        <v>4860.27441469514</v>
+      </c>
+      <c r="P39">
+        <f>8*(N39/B39)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q39" s="9">
+        <f>8*(O39/B39)^2</f>
+        <v>3.0236502254259432E-3</v>
+      </c>
+      <c r="R39" s="10">
+        <f>(Q39-P39)/P39</f>
+        <v>-0.12163745662583968</v>
+      </c>
+      <c r="S39" s="8">
+        <f>500*2*O39/B39</f>
+        <v>19.44109765878056</v>
+      </c>
+      <c r="T39" s="4">
+        <f>B39/4*P39</f>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20">
+      <c r="A40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F40" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G40">
+        <f>F40</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H40" s="5">
+        <f>0.25*G40</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I40" s="5">
+        <v>1</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L40">
+        <v>0.1</v>
+      </c>
+      <c r="M40" s="8">
+        <f>L40/H40</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N40" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O40" s="17">
+        <v>5115.32676697441</v>
+      </c>
+      <c r="P40">
+        <f>8*(N40/B40)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q40" s="9">
+        <f>8*(O40/B40)^2</f>
+        <v>3.3493206954143834E-3</v>
+      </c>
+      <c r="R40" s="10">
+        <f t="shared" ref="R40:R42" si="24">(Q40-P40)/P40</f>
+        <v>-2.7031030288743259E-2</v>
+      </c>
+      <c r="S40" s="8">
+        <f t="shared" ref="S40:S42" si="25">500*2*O40/B40</f>
+        <v>20.461307067897639</v>
+      </c>
+      <c r="T40" s="4">
+        <f t="shared" ref="T40:T42" si="26">B40/4*P40</f>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20">
+      <c r="A41" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G41">
+        <f>F41</f>
+        <v>0.05</v>
+      </c>
+      <c r="H41" s="5">
+        <f>0.25*G41</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I41" s="5">
+        <v>1</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L41">
+        <v>0.1</v>
+      </c>
+      <c r="M41" s="8">
+        <f>L41/H41</f>
+        <v>8</v>
+      </c>
+      <c r="N41" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O41" s="17">
+        <v>5125.0459836528198</v>
+      </c>
+      <c r="P41">
+        <f>8*(N41/B41)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q41" s="9">
+        <f t="shared" ref="Q41:Q42" si="27">8*(O41/B41)^2</f>
+        <v>3.3620603308231549E-3</v>
+      </c>
+      <c r="R41" s="10">
+        <f t="shared" si="24"/>
+        <v>-2.3330199264965799E-2</v>
+      </c>
+      <c r="S41" s="8">
+        <f t="shared" si="25"/>
+        <v>20.500183934611279</v>
+      </c>
+      <c r="T41" s="4">
+        <f t="shared" si="26"/>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20">
+      <c r="A42" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F42" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G42">
+        <f>F42</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H42" s="5">
+        <f>0.25*G42</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I42" s="5">
+        <v>1</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L42">
+        <v>0.1</v>
+      </c>
+      <c r="M42" s="8">
+        <f>L42/H42</f>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N42" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O42" s="17">
+        <v>5082.5638219350403</v>
+      </c>
+      <c r="P42">
+        <f>8*(N42/B42)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q42" s="9">
+        <f t="shared" si="27"/>
+        <v>3.3065542405174937E-3</v>
+      </c>
+      <c r="R42" s="10">
+        <f t="shared" si="24"/>
+        <v>-3.9454574446876389E-2</v>
+      </c>
+      <c r="S42" s="8">
+        <f t="shared" si="25"/>
+        <v>20.330255287740158</v>
+      </c>
+      <c r="T42" s="4">
+        <f t="shared" si="26"/>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20">
+      <c r="A45" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F45" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G45">
+        <f>F45</f>
+        <v>0.1</v>
+      </c>
+      <c r="H45" s="5">
+        <f>0.25*G45</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I45" s="5">
+        <v>1</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L45">
+        <v>0.1</v>
+      </c>
+      <c r="M45" s="8">
+        <f>L45/H45</f>
+        <v>4</v>
+      </c>
+      <c r="N45" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O45" s="17">
+        <v>4839.8902912821904</v>
+      </c>
+      <c r="P45">
+        <f>8*(N45/B45)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q45" s="9">
+        <f>8*(O45/B45)^2</f>
+        <v>2.9983408680508937E-3</v>
+      </c>
+      <c r="R45" s="10">
+        <f>(Q45-P45)/P45</f>
+        <v>-0.12898975925931722</v>
+      </c>
+      <c r="S45" s="8">
+        <f>500*2*O45/B45</f>
+        <v>19.35956116512876</v>
+      </c>
+      <c r="T45" s="4">
+        <f>B45/4*P45</f>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20">
+      <c r="A46" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F46" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G46">
+        <f>F46</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H46" s="5">
+        <f>0.25*G46</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I46" s="5">
+        <v>1</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L46">
+        <v>0.1</v>
+      </c>
+      <c r="M46" s="8">
+        <f>L46/H46</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N46" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O46" s="17">
+        <v>5098.0300379374303</v>
+      </c>
+      <c r="P46">
+        <f>8*(N46/B46)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q46" s="9">
+        <f>8*(O46/B46)^2</f>
+        <v>3.3267085142671764E-3</v>
+      </c>
+      <c r="R46" s="10">
+        <f t="shared" ref="R46:R48" si="28">(Q46-P46)/P46</f>
+        <v>-3.3599810227864714E-2</v>
+      </c>
+      <c r="S46" s="8">
+        <f t="shared" ref="S46:S48" si="29">500*2*O46/B46</f>
+        <v>20.392120151749722</v>
+      </c>
+      <c r="T46" s="4">
+        <f t="shared" ref="T46:T48" si="30">B46/4*P46</f>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20">
+      <c r="A47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F47" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G47">
+        <f>F47</f>
+        <v>0.05</v>
+      </c>
+      <c r="H47" s="5">
+        <f>0.25*G47</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I47" s="5">
+        <v>1</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L47">
+        <v>0.1</v>
+      </c>
+      <c r="M47" s="8">
+        <f>L47/H47</f>
+        <v>8</v>
+      </c>
+      <c r="N47" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O47" s="17">
+        <v>5115.2850269746104</v>
+      </c>
+      <c r="P47">
+        <f>8*(N47/B47)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q47" s="9">
+        <f t="shared" ref="Q47:Q48" si="31">8*(O47/B47)^2</f>
+        <v>3.3492660361204023E-3</v>
+      </c>
+      <c r="R47" s="10">
+        <f t="shared" si="28"/>
+        <v>-2.7046908671790545E-2</v>
+      </c>
+      <c r="S47" s="8">
+        <f t="shared" si="29"/>
+        <v>20.461140107898441</v>
+      </c>
+      <c r="T47" s="4">
+        <f t="shared" si="30"/>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20">
+      <c r="A48" t="s">
+        <v>134</v>
+      </c>
+      <c r="B48" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F48" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G48">
+        <f>F48</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H48" s="5">
+        <f>0.25*G48</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I48" s="5">
+        <v>1</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L48">
+        <v>0.1</v>
+      </c>
+      <c r="M48" s="8">
+        <f>L48/H48</f>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N48" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O48" s="17"/>
+      <c r="P48">
+        <f>8*(N48/B48)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q48" s="9">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="R48" s="10">
+        <f t="shared" si="28"/>
+        <v>-1</v>
+      </c>
+      <c r="S48" s="8">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="T48" s="4">
+        <f t="shared" si="30"/>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" s="5">
+        <v>250000</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D57" s="5">
         <v>0.2</v>
       </c>
-      <c r="E43" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F43">
-        <v>0.1</v>
-      </c>
-      <c r="G43" s="5">
-        <f>0.25*F43</f>
+      <c r="E57" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F57">
+        <v>0.1</v>
+      </c>
+      <c r="G57" s="5">
+        <f>0.25*F57</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H43" s="5">
+      <c r="H57" s="5">
         <v>2</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="I57" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J43" s="5" t="s">
+      <c r="J57" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K43">
-        <v>0.1</v>
-      </c>
-      <c r="L43" s="8">
-        <f>K43/G43</f>
+      <c r="K57">
+        <v>0.1</v>
+      </c>
+      <c r="L57" s="8">
+        <f>K57/G57</f>
         <v>4</v>
       </c>
-      <c r="M43" s="8">
+      <c r="M57" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O43">
-        <f>8*(M43/A43)^2</f>
+      <c r="O57">
+        <f>8*(M57/A57)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
-      <c r="A44" s="5">
+    <row r="58" spans="1:15">
+      <c r="A58" s="5">
         <v>250000</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B58" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C58" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D44" s="5">
-        <f>E44*2</f>
+      <c r="D58" s="5">
+        <f>E58*2</f>
         <v>0.13400000000000001</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E58" s="5">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="F44">
-        <f>E44</f>
+      <c r="F58">
+        <f>E58</f>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="G44" s="5">
-        <f>0.25*F44</f>
+      <c r="G58" s="5">
+        <f>0.25*F58</f>
         <v>1.6750000000000001E-2</v>
       </c>
-      <c r="H44" s="5">
+      <c r="H58" s="5">
         <v>2</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="I58" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J44" s="5" t="s">
+      <c r="J58" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K44">
-        <v>0.1</v>
-      </c>
-      <c r="L44" s="8">
-        <f>K44/G44</f>
+      <c r="K58">
+        <v>0.1</v>
+      </c>
+      <c r="L58" s="8">
+        <f>K58/G58</f>
         <v>5.9701492537313436</v>
       </c>
-      <c r="M44" s="8">
+      <c r="M58" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O44">
-        <f>8*(M44/A44)^2</f>
+      <c r="O58">
+        <f>8*(M58/A58)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
-      <c r="A45" s="5">
+    <row r="59" spans="1:15">
+      <c r="A59" s="5">
         <v>250000</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B59" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C59" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D45" s="5">
-        <f t="shared" ref="D45:D46" si="20">E45*2</f>
-        <v>0.1</v>
-      </c>
-      <c r="E45" s="5">
+      <c r="D59" s="5">
+        <f t="shared" ref="D59:D60" si="32">E59*2</f>
+        <v>0.1</v>
+      </c>
+      <c r="E59" s="5">
         <v>0.05</v>
       </c>
-      <c r="F45">
-        <f>E45</f>
+      <c r="F59">
+        <f>E59</f>
         <v>0.05</v>
       </c>
-      <c r="G45" s="5">
-        <f>0.25*F45</f>
+      <c r="G59" s="5">
+        <f>0.25*F59</f>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="H45" s="5">
+      <c r="H59" s="5">
         <v>2</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="I59" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J45" s="5" t="s">
+      <c r="J59" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K45">
-        <v>0.1</v>
-      </c>
-      <c r="L45" s="8">
-        <f>K45/G45</f>
+      <c r="K59">
+        <v>0.1</v>
+      </c>
+      <c r="L59" s="8">
+        <f>K59/G59</f>
         <v>8</v>
       </c>
-      <c r="M45" s="8">
+      <c r="M59" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O45">
-        <f>8*(M45/A45)^2</f>
+      <c r="O59">
+        <f>8*(M59/A59)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
-      <c r="A46" s="5">
+    <row r="60" spans="1:15">
+      <c r="A60" s="5">
         <v>250000</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B60" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D46" s="5">
-        <f t="shared" si="20"/>
+      <c r="D60" s="5">
+        <f t="shared" si="32"/>
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E60" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F46">
-        <f>E46</f>
+      <c r="F60">
+        <f>E60</f>
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="G46" s="5">
-        <f>0.25*F46</f>
+      <c r="G60" s="5">
+        <f>0.25*F60</f>
         <v>8.2500000000000004E-3</v>
       </c>
-      <c r="H46" s="5">
+      <c r="H60" s="5">
         <v>2</v>
       </c>
-      <c r="I46" s="5" t="s">
+      <c r="I60" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J46" s="5" t="s">
+      <c r="J60" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K46">
-        <v>0.1</v>
-      </c>
-      <c r="L46" s="8">
-        <f>K46/G46</f>
+      <c r="K60">
+        <v>0.1</v>
+      </c>
+      <c r="L60" s="8">
+        <f>K60/G60</f>
         <v>12.121212121212121</v>
       </c>
-      <c r="M46" s="8">
+      <c r="M60" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O46">
-        <f>8*(M46/A46)^2</f>
+      <c r="O60">
+        <f>8*(M60/A60)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
always update wall model
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663DBA1A-16CB-4849-B1B9-2AA5B7774062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AEF7B5-9AED-4C9C-8C08-F8BAEF7F3FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="143">
   <si>
     <t>nompi</t>
   </si>
@@ -470,6 +470,30 @@
   </si>
   <si>
     <t>WM+SMAG+NODAMP</t>
+  </si>
+  <si>
+    <t>WM+SMAG+LARGE</t>
+  </si>
+  <si>
+    <t>25.6×9.6×2.0</t>
+  </si>
+  <si>
+    <t>256×96×32</t>
+  </si>
+  <si>
+    <t>384×144×48</t>
+  </si>
+  <si>
+    <t>512×192×64</t>
+  </si>
+  <si>
+    <t>768×288×96</t>
+  </si>
+  <si>
+    <t>WM+SMAG+CFL0.25</t>
+  </si>
+  <si>
+    <t>WM+SMAG+ACC</t>
   </si>
 </sst>
 </file>
@@ -893,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760F17C5-A88B-45BD-B60F-0BA67AB143DF}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1471,978 +1495,1710 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797B825A-8F5D-4559-BC02-F7413FCCDF08}">
-  <dimension ref="A1:W39"/>
+  <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="15.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" customWidth="1"/>
-    <col min="7" max="7" width="11.90625" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" customWidth="1"/>
-    <col min="9" max="9" width="20.7265625" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
-    <col min="13" max="13" width="10.90625" customWidth="1"/>
-    <col min="17" max="17" width="14.08984375" customWidth="1"/>
-    <col min="18" max="18" width="16.08984375" customWidth="1"/>
-    <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="20" width="12.1796875" customWidth="1"/>
-    <col min="21" max="21" width="11.7265625" customWidth="1"/>
-    <col min="22" max="22" width="13" customWidth="1"/>
-    <col min="23" max="23" width="13.36328125" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="11.08984375" customWidth="1"/>
+    <col min="6" max="6" width="11.36328125" customWidth="1"/>
+    <col min="7" max="7" width="14.26953125" customWidth="1"/>
+    <col min="8" max="8" width="11.90625" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" customWidth="1"/>
+    <col min="10" max="10" width="20.7265625" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="14" max="14" width="10.90625" customWidth="1"/>
+    <col min="18" max="18" width="14.08984375" customWidth="1"/>
+    <col min="19" max="19" width="16.08984375" customWidth="1"/>
+    <col min="20" max="20" width="13" customWidth="1"/>
+    <col min="21" max="21" width="12.1796875" customWidth="1"/>
+    <col min="22" max="22" width="11.7265625" customWidth="1"/>
+    <col min="23" max="23" width="13" customWidth="1"/>
+    <col min="24" max="24" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:24">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
-      <c r="A2" s="5">
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="5">
         <v>5714</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="5">
-        <v>0.1</v>
-      </c>
       <c r="E2" s="5">
         <v>0.1</v>
       </c>
-      <c r="F2">
-        <f>E2</f>
-        <v>0.1</v>
-      </c>
-      <c r="G2" s="5">
-        <f>0.25*F2</f>
+      <c r="F2" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G2">
+        <f>F2</f>
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="5">
+        <f>0.25*G2</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H2" s="5">
+      <c r="I2" s="5">
         <v>1</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K2">
-        <v>0.1</v>
-      </c>
-      <c r="L2" s="8">
-        <f>K2/G2</f>
+      <c r="L2">
+        <v>0.1</v>
+      </c>
+      <c r="M2" s="8">
+        <f>L2/H2</f>
         <v>4</v>
       </c>
-      <c r="M2" s="13">
+      <c r="N2" s="13">
         <v>180.601843765257</v>
       </c>
-      <c r="N2" s="4">
+      <c r="O2" s="4">
         <v>179.99818440102101</v>
       </c>
-      <c r="O2">
-        <f>8*(M2/A2)^2</f>
+      <c r="P2">
+        <f>8*(N2/B2)^2</f>
         <v>7.9919705400696046E-3</v>
       </c>
-      <c r="P2" s="9">
-        <f>8*(N2/A2)^2</f>
+      <c r="Q2" s="9">
+        <f>8*(O2/B2)^2</f>
         <v>7.9386337085019347E-3</v>
       </c>
-      <c r="Q2" s="10">
-        <f>(P2-O2)/O2</f>
+      <c r="R2" s="10">
+        <f>(Q2-P2)/P2</f>
         <v>-6.6738023245022388E-3</v>
       </c>
-      <c r="R2" s="8">
-        <f>100*2*N2/A2</f>
+      <c r="S2" s="8">
+        <f>100*2*O2/B2</f>
         <v>6.3002514666090654</v>
       </c>
-      <c r="S2" s="4">
-        <f>A2/4*O2</f>
+      <c r="T2" s="4">
+        <f>B2/4*P2</f>
         <v>11.416529916489431</v>
-      </c>
-      <c r="T2" s="8">
-        <f>D2*M2</f>
-        <v>18.060184376525701</v>
       </c>
       <c r="U2" s="8">
         <f>E2*N2</f>
+        <v>18.060184376525701</v>
+      </c>
+      <c r="V2" s="8">
+        <f>F2*O2</f>
         <v>17.9998184401021</v>
       </c>
-      <c r="V2" s="8">
-        <f>F2*M2</f>
+      <c r="W2" s="8">
+        <f>G2*N2</f>
         <v>18.060184376525701</v>
       </c>
-      <c r="W2" s="4">
-        <f>G2*M2</f>
+      <c r="X2" s="4">
+        <f>H2*N2</f>
         <v>4.5150460941314252</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
-      <c r="A3" s="5">
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="5">
         <v>5714</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="D3" s="5">
-        <v>6.7000000000000004E-2</v>
       </c>
       <c r="E3" s="5">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="F3">
-        <f>E3</f>
+      <c r="F3" s="5">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="G3" s="5">
-        <f>0.25*F3</f>
+      <c r="G3">
+        <f>F3</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H3" s="5">
+        <f>0.25*G3</f>
         <v>1.6750000000000001E-2</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="5">
         <v>1</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K3">
-        <v>0.1</v>
-      </c>
-      <c r="L3" s="8">
-        <f t="shared" ref="L3:L5" si="0">K3/G3</f>
+      <c r="L3">
+        <v>0.1</v>
+      </c>
+      <c r="M3" s="8">
+        <f t="shared" ref="M3:M5" si="0">L3/H3</f>
         <v>5.9701492537313436</v>
       </c>
-      <c r="M3" s="13">
+      <c r="N3" s="13">
         <v>180.601843765257</v>
       </c>
-      <c r="N3" s="4">
+      <c r="O3" s="4">
         <v>182.74010750150001</v>
       </c>
-      <c r="O3">
-        <f>8*(M3/A3)^2</f>
+      <c r="P3">
+        <f>8*(N3/B3)^2</f>
         <v>7.9919705400696046E-3</v>
       </c>
-      <c r="P3" s="9">
-        <f t="shared" ref="P3:P6" si="1">8*(N3/A3)^2</f>
+      <c r="Q3" s="9">
+        <f t="shared" ref="Q3:Q6" si="1">8*(O3/B3)^2</f>
         <v>8.1823352010309113E-3</v>
       </c>
-      <c r="Q3" s="10">
-        <f t="shared" ref="Q3:Q6" si="2">(P3-O3)/O3</f>
+      <c r="R3" s="10">
+        <f t="shared" ref="R3:R6" si="2">(Q3-P3)/P3</f>
         <v>2.3819489825052425E-2</v>
       </c>
-      <c r="R3" s="8">
-        <f t="shared" ref="R3:R6" si="3">100*2*N3/A3</f>
+      <c r="S3" s="8">
+        <f t="shared" ref="S3:S6" si="3">100*2*O3/B3</f>
         <v>6.396223573731187</v>
       </c>
-      <c r="S3" s="4">
-        <f t="shared" ref="S3:S6" si="4">A3/4*O3</f>
+      <c r="T3" s="4">
+        <f t="shared" ref="T3:T6" si="4">B3/4*P3</f>
         <v>11.416529916489431</v>
       </c>
-      <c r="T3" s="8">
-        <f t="shared" ref="T3:T6" si="5">D3*M3</f>
+      <c r="U3" s="8">
+        <f t="shared" ref="U3:U6" si="5">E3*N3</f>
         <v>12.10032353227222</v>
       </c>
-      <c r="U3" s="8">
-        <f t="shared" ref="U3:U6" si="6">E3*N3</f>
+      <c r="V3" s="8">
+        <f t="shared" ref="V3:V6" si="6">F3*O3</f>
         <v>12.243587202600501</v>
       </c>
-      <c r="V3" s="8">
-        <f t="shared" ref="V3:V6" si="7">F3*M3</f>
+      <c r="W3" s="8">
+        <f t="shared" ref="W3:W6" si="7">G3*N3</f>
         <v>12.10032353227222</v>
       </c>
-      <c r="W3" s="4">
-        <f t="shared" ref="W3:W6" si="8">G3*M3</f>
+      <c r="X3" s="4">
+        <f t="shared" ref="X3:X6" si="8">H3*N3</f>
         <v>3.0250808830680551</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
-      <c r="A4" s="5">
+    <row r="4" spans="1:24">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="5">
         <v>5714</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.05</v>
       </c>
       <c r="E4" s="5">
         <v>0.05</v>
       </c>
-      <c r="F4">
-        <f>E4</f>
+      <c r="F4" s="5">
         <v>0.05</v>
       </c>
-      <c r="G4" s="5">
-        <f>0.25*F4</f>
+      <c r="G4">
+        <f>F4</f>
+        <v>0.05</v>
+      </c>
+      <c r="H4" s="5">
+        <f>0.25*G4</f>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <v>1</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K4">
-        <v>0.1</v>
-      </c>
-      <c r="L4" s="8">
+      <c r="L4">
+        <v>0.1</v>
+      </c>
+      <c r="M4" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M4" s="13">
+      <c r="N4" s="13">
         <v>180.601843765257</v>
       </c>
-      <c r="N4" s="4">
+      <c r="O4" s="4">
         <v>183.383339658707</v>
       </c>
-      <c r="O4">
-        <f>8*(M4/A4)^2</f>
+      <c r="P4">
+        <f>8*(N4/B4)^2</f>
         <v>7.9919705400696046E-3</v>
       </c>
-      <c r="P4" s="9">
+      <c r="Q4" s="9">
         <f t="shared" si="1"/>
         <v>8.2400390530784837E-3</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="R4" s="10">
         <f t="shared" si="2"/>
         <v>3.1039718147749643E-2</v>
       </c>
-      <c r="R4" s="8">
+      <c r="S4" s="8">
         <f t="shared" si="3"/>
         <v>6.4187378249459925</v>
       </c>
-      <c r="S4" s="4">
+      <c r="T4" s="4">
         <f t="shared" si="4"/>
         <v>11.416529916489431</v>
       </c>
-      <c r="T4" s="8">
+      <c r="U4" s="8">
         <f t="shared" si="5"/>
         <v>9.0300921882628504</v>
       </c>
-      <c r="U4" s="8">
+      <c r="V4" s="8">
         <f t="shared" si="6"/>
         <v>9.1691669829353497</v>
       </c>
-      <c r="V4" s="8">
+      <c r="W4" s="8">
         <f t="shared" si="7"/>
         <v>9.0300921882628504</v>
       </c>
-      <c r="W4" s="4">
+      <c r="X4" s="4">
         <f t="shared" si="8"/>
         <v>2.2575230470657126</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
-      <c r="A5" s="5">
+    <row r="5" spans="1:24">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="5">
         <v>5714</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="D5" s="5">
-        <v>3.3000000000000002E-2</v>
       </c>
       <c r="E5" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F5">
-        <f>E5</f>
+      <c r="F5" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="G5" s="5">
-        <f>0.25*F5</f>
+      <c r="G5">
+        <f>F5</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H5" s="5">
+        <f>0.25*G5</f>
         <v>8.2500000000000004E-3</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <v>1</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K5">
-        <v>0.1</v>
-      </c>
-      <c r="L5" s="8">
+      <c r="L5">
+        <v>0.1</v>
+      </c>
+      <c r="M5" s="8">
         <f t="shared" si="0"/>
         <v>12.121212121212121</v>
       </c>
-      <c r="M5" s="13">
+      <c r="N5" s="13">
         <v>180.601843765257</v>
       </c>
-      <c r="N5" s="4">
+      <c r="O5" s="4">
         <v>183.668368577509</v>
       </c>
-      <c r="O5">
-        <f>8*(M5/A5)^2</f>
+      <c r="P5">
+        <f>8*(N5/B5)^2</f>
         <v>7.9919705400696046E-3</v>
       </c>
-      <c r="P5" s="9">
+      <c r="Q5" s="9">
         <f t="shared" si="1"/>
         <v>8.2656736025973811E-3</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="R5" s="10">
         <f t="shared" si="2"/>
         <v>3.4247256187382384E-2</v>
       </c>
-      <c r="R5" s="8">
+      <c r="S5" s="8">
         <f t="shared" si="3"/>
         <v>6.4287143359296115</v>
       </c>
-      <c r="S5" s="4">
+      <c r="T5" s="4">
         <f t="shared" si="4"/>
         <v>11.416529916489431</v>
       </c>
-      <c r="T5" s="8">
+      <c r="U5" s="8">
         <f t="shared" si="5"/>
         <v>5.9598608442534813</v>
       </c>
-      <c r="U5" s="8">
+      <c r="V5" s="8">
         <f t="shared" si="6"/>
         <v>6.0610561630577973</v>
       </c>
-      <c r="V5" s="8">
+      <c r="W5" s="8">
         <f t="shared" si="7"/>
         <v>5.9598608442534813</v>
       </c>
-      <c r="W5" s="4">
+      <c r="X5" s="4">
         <f t="shared" si="8"/>
         <v>1.4899652110633703</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
-      <c r="A6" s="5">
+    <row r="6" spans="1:24">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="5">
         <v>5714</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f>18.84/384</f>
         <v>4.9062500000000002E-2</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <f>6.28/256</f>
         <v>2.4531250000000001E-2</v>
       </c>
-      <c r="F6" s="14">
+      <c r="G6" s="14">
         <v>2.2990199999999999E-2</v>
       </c>
-      <c r="G6" s="14">
+      <c r="H6" s="14">
         <v>1.5090470000000001E-4</v>
       </c>
-      <c r="H6" s="5">
-        <f>D6/E6</f>
+      <c r="I6" s="5">
+        <f>E6/F6</f>
         <v>2</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K6">
-        <v>0.1</v>
-      </c>
-      <c r="L6" s="8">
-        <f>K6/G6</f>
+      <c r="L6">
+        <v>0.1</v>
+      </c>
+      <c r="M6" s="8">
+        <f>L6/H6</f>
         <v>662.66988370806212</v>
       </c>
-      <c r="M6" s="13">
+      <c r="N6" s="13">
         <v>180.601843765257</v>
       </c>
-      <c r="N6" s="4">
+      <c r="O6" s="4">
         <v>183.51840919111899</v>
       </c>
-      <c r="O6">
-        <f>8*(M6/A6)^2</f>
+      <c r="P6">
+        <f>8*(N6/B6)^2</f>
         <v>7.9919705400696046E-3</v>
       </c>
-      <c r="P6" s="9">
+      <c r="Q6" s="9">
         <f t="shared" si="1"/>
         <v>8.2521817929983986E-3</v>
       </c>
-      <c r="Q6" s="10">
+      <c r="R6" s="10">
         <f t="shared" si="2"/>
         <v>3.2559085600248942E-2</v>
       </c>
-      <c r="R6" s="8">
+      <c r="S6" s="8">
         <f t="shared" si="3"/>
         <v>6.4234654949639127</v>
       </c>
-      <c r="S6" s="4">
+      <c r="T6" s="4">
         <f t="shared" si="4"/>
         <v>11.416529916489431</v>
       </c>
-      <c r="T6" s="8">
+      <c r="U6" s="8">
         <f t="shared" si="5"/>
         <v>8.8607779597329213</v>
       </c>
-      <c r="U6" s="8">
+      <c r="V6" s="8">
         <f t="shared" si="6"/>
         <v>4.501935975469638</v>
       </c>
-      <c r="V6" s="8">
+      <c r="W6" s="8">
         <f t="shared" si="7"/>
         <v>4.1520725085320116</v>
       </c>
-      <c r="W6" s="4">
+      <c r="X6" s="4">
         <f t="shared" si="8"/>
         <v>2.7253667052842979E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
-      <c r="A12" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23">
-      <c r="A13" s="5">
+    <row r="9" spans="1:24">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="5">
         <v>5714</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F13">
-        <f>E13</f>
-        <v>0.1</v>
-      </c>
-      <c r="G13" s="5">
-        <f>0.25*F13</f>
+      <c r="E9" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G9">
+        <f>F9</f>
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="5">
+        <f>0.25*G9</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I9" s="5">
         <v>1</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13" s="8">
-        <v>0</v>
-      </c>
-      <c r="M13" s="13">
+      <c r="L9">
+        <v>0.1</v>
+      </c>
+      <c r="M9" s="8">
+        <f>L9/H9</f>
+        <v>4</v>
+      </c>
+      <c r="N9" s="13">
         <v>180.601843765257</v>
       </c>
-      <c r="N13" s="4">
-        <v>181.51132402826201</v>
-      </c>
-      <c r="O13">
-        <f>8*(M13/A13)^2</f>
+      <c r="O9" s="4">
+        <v>178.80960212652499</v>
+      </c>
+      <c r="P9">
+        <f>8*(N9/B9)^2</f>
         <v>7.9919705400696046E-3</v>
       </c>
-      <c r="P13" s="9">
-        <f>8*(N13/A13)^2</f>
-        <v>8.0726656302520777E-3</v>
-      </c>
-      <c r="Q13" s="10">
-        <f>(P13-O13)/O13</f>
-        <v>1.0097020475474653E-2</v>
-      </c>
-      <c r="R13" s="8">
-        <f>100*2*N13/A13</f>
-        <v>6.3532140016892553</v>
-      </c>
-      <c r="S13" s="4">
-        <f>A13/4*O13</f>
+      <c r="Q9" s="9">
+        <f>8*(O9/B9)^2</f>
+        <v>7.8341374782607952E-3</v>
+      </c>
+      <c r="R9" s="10">
+        <f>(Q9-P9)/P9</f>
+        <v>-1.9748954405859807E-2</v>
+      </c>
+      <c r="S9" s="8">
+        <f>100*2*O9/B9</f>
+        <v>6.2586490068787182</v>
+      </c>
+      <c r="T9" s="4">
+        <f>B9/4*P9</f>
         <v>11.416529916489431</v>
       </c>
-      <c r="T13" s="8">
-        <f>D13*M13</f>
+      <c r="U9" s="8">
+        <f>E9*N9</f>
         <v>18.060184376525701</v>
       </c>
-      <c r="U13" s="8">
-        <f>E13*N13</f>
-        <v>18.151132402826203</v>
-      </c>
-      <c r="V13" s="8">
-        <f>F13*M13</f>
+      <c r="V9" s="8">
+        <f>F9*N9</f>
         <v>18.060184376525701</v>
       </c>
-      <c r="W13" s="8">
-        <f>G13*M13</f>
+      <c r="W9" s="8">
+        <f>G9*N9</f>
+        <v>18.060184376525701</v>
+      </c>
+      <c r="X9" s="4">
+        <f>H9*N9</f>
         <v>4.5150460941314252</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
-      <c r="A14" s="5">
+    <row r="10" spans="1:24">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="5">
         <v>5714</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="5">
+      <c r="E10" s="5">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="E14" s="5">
+      <c r="F10" s="5">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="F14">
-        <f>E14</f>
+      <c r="G10">
+        <f>F10</f>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="G14" s="5">
-        <f>0.25*F14</f>
+      <c r="H10" s="5">
+        <f>0.25*G10</f>
         <v>1.6750000000000001E-2</v>
       </c>
-      <c r="H14" s="5">
+      <c r="I10" s="5">
         <v>1</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14" s="8">
-        <v>0</v>
-      </c>
-      <c r="M14" s="13">
+      <c r="L10">
+        <v>0.1</v>
+      </c>
+      <c r="M10" s="8">
+        <f t="shared" ref="M10:M12" si="9">L10/H10</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N10" s="13">
         <v>180.601843765257</v>
       </c>
-      <c r="N14" s="4">
-        <v>182.633280201991</v>
-      </c>
-      <c r="O14">
-        <f>8*(M14/A14)^2</f>
+      <c r="O10" s="4">
+        <v>181.94836980537099</v>
+      </c>
+      <c r="P10">
+        <f>8*(N10/B10)^2</f>
         <v>7.9919705400696046E-3</v>
       </c>
-      <c r="P14" s="9">
-        <f t="shared" ref="P14:P16" si="9">8*(N14/A14)^2</f>
-        <v>8.1727714408602013E-3</v>
-      </c>
-      <c r="Q14" s="10">
-        <f t="shared" ref="Q14:Q16" si="10">(P14-O14)/O14</f>
-        <v>2.2622818725883596E-2</v>
-      </c>
-      <c r="R14" s="8">
-        <f t="shared" ref="R14:R16" si="11">100*2*N14/A14</f>
-        <v>6.3924844312912494</v>
-      </c>
-      <c r="S14" s="4">
-        <f t="shared" ref="S14:S16" si="12">A14/4*O14</f>
+      <c r="Q10" s="9">
+        <f t="shared" ref="Q10:Q12" si="10">8*(O10/B10)^2</f>
+        <v>8.1115874107959614E-3</v>
+      </c>
+      <c r="R10" s="10">
+        <f t="shared" ref="R10:R12" si="11">(Q10-P10)/P10</f>
+        <v>1.4967131088212824E-2</v>
+      </c>
+      <c r="S10" s="8">
+        <f t="shared" ref="S10:S12" si="12">100*2*O10/B10</f>
+        <v>6.3685113687564225</v>
+      </c>
+      <c r="T10" s="4">
+        <f t="shared" ref="T10:T12" si="13">B10/4*P10</f>
         <v>11.416529916489431</v>
       </c>
-      <c r="T14" s="8">
-        <f t="shared" ref="T14:T16" si="13">D14*M14</f>
+      <c r="U10" s="8">
+        <f t="shared" ref="U10:U12" si="14">E10*N10</f>
         <v>12.10032353227222</v>
       </c>
-      <c r="U14" s="8">
-        <f t="shared" ref="U14:U16" si="14">E14*N14</f>
-        <v>12.236429773533398</v>
-      </c>
-      <c r="V14" s="8">
-        <f t="shared" ref="V14:V16" si="15">F14*M14</f>
+      <c r="V10" s="8">
+        <f>F10*N10</f>
         <v>12.10032353227222</v>
       </c>
-      <c r="W14" s="8">
-        <f t="shared" ref="W14:W16" si="16">G14*M14</f>
+      <c r="W10" s="8">
+        <f t="shared" ref="W10:W12" si="15">G10*N10</f>
+        <v>12.10032353227222</v>
+      </c>
+      <c r="X10" s="4">
+        <f t="shared" ref="X10:X12" si="16">H10*N10</f>
         <v>3.0250808830680551</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
-      <c r="A15" s="5">
+    <row r="11" spans="1:24">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="5">
         <v>5714</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="5">
+      <c r="E11" s="5">
         <v>0.05</v>
       </c>
-      <c r="E15" s="5">
+      <c r="F11" s="5">
         <v>0.05</v>
       </c>
-      <c r="F15">
-        <f>E15</f>
+      <c r="G11">
+        <f>F11</f>
         <v>0.05</v>
       </c>
-      <c r="G15" s="5">
-        <f>0.25*F15</f>
+      <c r="H11" s="5">
+        <f>0.25*G11</f>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="H15" s="5">
+      <c r="I11" s="5">
         <v>1</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15" s="8">
-        <v>0</v>
-      </c>
-      <c r="M15" s="13">
+      <c r="L11">
+        <v>0.1</v>
+      </c>
+      <c r="M11" s="8">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="N11" s="13">
         <v>180.601843765257</v>
       </c>
-      <c r="N15" s="4">
-        <v>181.289661622458</v>
-      </c>
-      <c r="O15">
-        <f>8*(M15/A15)^2</f>
+      <c r="O11" s="4">
+        <v>183.24478220022101</v>
+      </c>
+      <c r="P11">
+        <f>8*(N11/B11)^2</f>
         <v>7.9919705400696046E-3</v>
       </c>
-      <c r="P15" s="9">
-        <f t="shared" si="9"/>
-        <v>8.0529609217001707E-3</v>
-      </c>
-      <c r="Q15" s="10">
+      <c r="Q11" s="9">
         <f t="shared" si="10"/>
-        <v>7.6314572638595908E-3</v>
-      </c>
-      <c r="R15" s="8">
+        <v>8.2275920385184477E-3</v>
+      </c>
+      <c r="R11" s="10">
         <f t="shared" si="11"/>
-        <v>6.3454554295575081</v>
-      </c>
-      <c r="S15" s="4">
+        <v>2.9482278152490656E-2</v>
+      </c>
+      <c r="S11" s="8">
         <f t="shared" si="12"/>
+        <v>6.4138880714113062</v>
+      </c>
+      <c r="T11" s="4">
+        <f t="shared" si="13"/>
         <v>11.416529916489431</v>
       </c>
-      <c r="T15" s="8">
-        <f t="shared" si="13"/>
+      <c r="U11" s="8">
+        <f t="shared" si="14"/>
         <v>9.0300921882628504</v>
       </c>
-      <c r="U15" s="8">
-        <f t="shared" si="14"/>
-        <v>9.0644830811228996</v>
-      </c>
-      <c r="V15" s="8">
+      <c r="V11" s="8">
+        <f>F11*N11</f>
+        <v>9.0300921882628504</v>
+      </c>
+      <c r="W11" s="8">
         <f t="shared" si="15"/>
         <v>9.0300921882628504</v>
       </c>
-      <c r="W15" s="8">
+      <c r="X11" s="4">
         <f t="shared" si="16"/>
         <v>2.2575230470657126</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
-      <c r="A16" s="5">
+    <row r="12" spans="1:24">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="5">
         <v>5714</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="5">
+      <c r="E12" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="E16" s="5">
+      <c r="F12" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F16">
-        <f>E16</f>
+      <c r="G12">
+        <f>F12</f>
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="G16" s="5">
-        <f>0.25*F16</f>
+      <c r="H12" s="5">
+        <f>0.25*G12</f>
         <v>8.2500000000000004E-3</v>
       </c>
-      <c r="H16" s="5">
+      <c r="I12" s="5">
         <v>1</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16" s="8">
-        <v>0</v>
-      </c>
-      <c r="M16" s="13">
+      <c r="L12">
+        <v>0.1</v>
+      </c>
+      <c r="M12" s="8">
+        <f t="shared" si="9"/>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N12" s="13">
         <v>180.601843765257</v>
       </c>
-      <c r="N16" s="4">
-        <v>180.70061309741001</v>
-      </c>
-      <c r="O16">
-        <f>8*(M16/A16)^2</f>
+      <c r="O12" s="4">
+        <v>184.211294112139</v>
+      </c>
+      <c r="P12">
+        <f>8*(N12/B12)^2</f>
         <v>7.9919705400696046E-3</v>
       </c>
-      <c r="P16" s="9">
-        <f t="shared" si="9"/>
-        <v>8.0007143870129832E-3</v>
-      </c>
-      <c r="Q16" s="10">
+      <c r="Q12" s="9">
         <f t="shared" si="10"/>
-        <v>1.0940789758344649E-3</v>
-      </c>
-      <c r="R16" s="8">
+        <v>8.3146126557039363E-3</v>
+      </c>
+      <c r="R12" s="10">
         <f t="shared" si="11"/>
-        <v>6.3248377002943652</v>
-      </c>
-      <c r="S16" s="4">
+        <v>4.0370783903255193E-2</v>
+      </c>
+      <c r="S12" s="8">
         <f t="shared" si="12"/>
+        <v>6.4477176798088554</v>
+      </c>
+      <c r="T12" s="4">
+        <f t="shared" si="13"/>
         <v>11.416529916489431</v>
       </c>
-      <c r="T16" s="8">
-        <f t="shared" si="13"/>
+      <c r="U12" s="8">
+        <f t="shared" si="14"/>
         <v>5.9598608442534813</v>
       </c>
-      <c r="U16" s="8">
-        <f t="shared" si="14"/>
-        <v>5.9631202322145311</v>
-      </c>
-      <c r="V16" s="8">
+      <c r="V12" s="8">
+        <f>F12*N12</f>
+        <v>5.9598608442534813</v>
+      </c>
+      <c r="W12" s="8">
         <f t="shared" si="15"/>
         <v>5.9598608442534813</v>
       </c>
-      <c r="W16" s="8">
+      <c r="X12" s="4">
         <f t="shared" si="16"/>
         <v>1.4899652110633703</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
-      <c r="A25" s="5" t="s">
+    <row r="15" spans="1:24">
+      <c r="A15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="5">
+        <v>5714</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G15">
+        <f>F15</f>
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="5">
+        <f>0.25*G15</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15">
+        <v>0.1</v>
+      </c>
+      <c r="M15" s="8">
+        <f>L15/H15</f>
+        <v>4</v>
+      </c>
+      <c r="N15" s="13">
+        <v>180.601843765257</v>
+      </c>
+      <c r="O15" s="4">
+        <v>179.05626668398401</v>
+      </c>
+      <c r="P15">
+        <f>8*(N15/B15)^2</f>
+        <v>7.9919705400696046E-3</v>
+      </c>
+      <c r="Q15" s="9">
+        <f>8*(O15/B15)^2</f>
+        <v>7.8557664835164076E-3</v>
+      </c>
+      <c r="R15" s="10">
+        <f>(Q15-P15)/P15</f>
+        <v>-1.7042612440862526E-2</v>
+      </c>
+      <c r="S15" s="8">
+        <f>100*2*O15/B15</f>
+        <v>6.2672826980743439</v>
+      </c>
+      <c r="T15" s="4">
+        <f>B15/4*P15</f>
+        <v>11.416529916489431</v>
+      </c>
+      <c r="U15" s="8">
+        <f>E15*N15</f>
+        <v>18.060184376525701</v>
+      </c>
+      <c r="V15" s="8">
+        <f>F15*N15</f>
+        <v>18.060184376525701</v>
+      </c>
+      <c r="W15" s="8">
+        <f>G15*N15</f>
+        <v>18.060184376525701</v>
+      </c>
+      <c r="X15" s="4">
+        <f>H15*N15</f>
+        <v>4.5150460941314252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="A16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="5">
+        <v>5714</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F16" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G16">
+        <f>F16</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H16" s="5">
+        <f>0.25*G16</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I16" s="5">
+        <v>1</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16">
+        <v>0.1</v>
+      </c>
+      <c r="M16" s="8">
+        <f t="shared" ref="M16:M18" si="17">L16/H16</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N16" s="13">
+        <v>180.601843765257</v>
+      </c>
+      <c r="O16" s="4">
+        <v>182.10670162320901</v>
+      </c>
+      <c r="P16">
+        <f>8*(N16/B16)^2</f>
+        <v>7.9919705400696046E-3</v>
+      </c>
+      <c r="Q16" s="9">
+        <f t="shared" ref="Q16:Q18" si="18">8*(O16/B16)^2</f>
+        <v>8.1257109909255113E-3</v>
+      </c>
+      <c r="R16" s="10">
+        <f t="shared" ref="R16:R18" si="19">(Q16-P16)/P16</f>
+        <v>1.6734352333428633E-2</v>
+      </c>
+      <c r="S16" s="8">
+        <f t="shared" ref="S16:S18" si="20">100*2*O16/B16</f>
+        <v>6.3740532594752892</v>
+      </c>
+      <c r="T16" s="4">
+        <f t="shared" ref="T16:T18" si="21">B16/4*P16</f>
+        <v>11.416529916489431</v>
+      </c>
+      <c r="U16" s="8">
+        <f t="shared" ref="U16:U18" si="22">E16*N16</f>
+        <v>12.10032353227222</v>
+      </c>
+      <c r="V16" s="8">
+        <f>F16*N16</f>
+        <v>12.10032353227222</v>
+      </c>
+      <c r="W16" s="8">
+        <f t="shared" ref="W16:W18" si="23">G16*N16</f>
+        <v>12.10032353227222</v>
+      </c>
+      <c r="X16" s="4">
+        <f t="shared" ref="X16:X18" si="24">H16*N16</f>
+        <v>3.0250808830680551</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" s="5">
+        <v>5714</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G17">
+        <f>F17</f>
+        <v>0.05</v>
+      </c>
+      <c r="H17" s="5">
+        <f>0.25*G17</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I17" s="5">
+        <v>1</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17">
+        <v>0.1</v>
+      </c>
+      <c r="M17" s="8">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="N17" s="13">
+        <v>180.601843765257</v>
+      </c>
+      <c r="O17" s="4">
+        <v>183.13948018760399</v>
+      </c>
+      <c r="P17">
+        <f>8*(N17/B17)^2</f>
+        <v>7.9919705400696046E-3</v>
+      </c>
+      <c r="Q17" s="9">
+        <f t="shared" si="18"/>
+        <v>8.2181387481589877E-3</v>
+      </c>
+      <c r="R17" s="10">
+        <f t="shared" si="19"/>
+        <v>2.8299429653229589E-2</v>
+      </c>
+      <c r="S17" s="8">
+        <f t="shared" si="20"/>
+        <v>6.4102023166819739</v>
+      </c>
+      <c r="T17" s="4">
+        <f t="shared" si="21"/>
+        <v>11.416529916489431</v>
+      </c>
+      <c r="U17" s="8">
+        <f t="shared" si="22"/>
+        <v>9.0300921882628504</v>
+      </c>
+      <c r="V17" s="8">
+        <f>F17*N17</f>
+        <v>9.0300921882628504</v>
+      </c>
+      <c r="W17" s="8">
+        <f t="shared" si="23"/>
+        <v>9.0300921882628504</v>
+      </c>
+      <c r="X17" s="4">
+        <f t="shared" si="24"/>
+        <v>2.2575230470657126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="5">
+        <v>5714</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F18" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G18">
+        <f>F18</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H18" s="5">
+        <f>0.25*G18</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I18" s="5">
+        <v>1</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18">
+        <v>0.1</v>
+      </c>
+      <c r="M18" s="8">
+        <f t="shared" si="17"/>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N18" s="13">
+        <v>180.601843765257</v>
+      </c>
+      <c r="O18" s="4">
+        <v>183.956931737708</v>
+      </c>
+      <c r="P18">
+        <f>8*(N18/B18)^2</f>
+        <v>7.9919705400696046E-3</v>
+      </c>
+      <c r="Q18" s="9">
+        <f t="shared" si="18"/>
+        <v>8.291666565843599E-3</v>
+      </c>
+      <c r="R18" s="10">
+        <f t="shared" si="19"/>
+        <v>3.7499640954805652E-2</v>
+      </c>
+      <c r="S18" s="8">
+        <f t="shared" si="20"/>
+        <v>6.4388145515473578</v>
+      </c>
+      <c r="T18" s="4">
+        <f t="shared" si="21"/>
+        <v>11.416529916489431</v>
+      </c>
+      <c r="U18" s="8">
+        <f t="shared" si="22"/>
+        <v>5.9598608442534813</v>
+      </c>
+      <c r="V18" s="8">
+        <f>F18*N18</f>
+        <v>5.9598608442534813</v>
+      </c>
+      <c r="W18" s="8">
+        <f t="shared" si="23"/>
+        <v>5.9598608442534813</v>
+      </c>
+      <c r="X18" s="4">
+        <f t="shared" si="24"/>
+        <v>1.4899652110633703</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="V19" s="8"/>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+    </row>
+    <row r="27" spans="1:24">
+      <c r="B27" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24">
+      <c r="B28" s="5">
+        <v>5714</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G28">
+        <f>F28</f>
+        <v>0.1</v>
+      </c>
+      <c r="H28" s="5">
+        <f>0.25*G28</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I28" s="5">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28" s="8">
+        <v>0</v>
+      </c>
+      <c r="N28" s="13">
+        <v>180.601843765257</v>
+      </c>
+      <c r="O28" s="4">
+        <v>181.51132402826201</v>
+      </c>
+      <c r="P28">
+        <f>8*(N28/B28)^2</f>
+        <v>7.9919705400696046E-3</v>
+      </c>
+      <c r="Q28" s="9">
+        <f>8*(O28/B28)^2</f>
+        <v>8.0726656302520777E-3</v>
+      </c>
+      <c r="R28" s="10">
+        <f>(Q28-P28)/P28</f>
+        <v>1.0097020475474653E-2</v>
+      </c>
+      <c r="S28" s="8">
+        <f>100*2*O28/B28</f>
+        <v>6.3532140016892553</v>
+      </c>
+      <c r="T28" s="4">
+        <f>B28/4*P28</f>
+        <v>11.416529916489431</v>
+      </c>
+      <c r="U28" s="8">
+        <f>E28*N28</f>
+        <v>18.060184376525701</v>
+      </c>
+      <c r="V28" s="8">
+        <f>F28*N28</f>
+        <v>18.060184376525701</v>
+      </c>
+      <c r="W28" s="8">
+        <f>G28*N28</f>
+        <v>18.060184376525701</v>
+      </c>
+      <c r="X28" s="8">
+        <f>H28*N28</f>
+        <v>4.5150460941314252</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
+      <c r="B29" s="5">
+        <v>5714</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F29" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G29">
+        <f>F29</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H29" s="5">
+        <f>0.25*G29</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I29" s="5">
+        <v>1</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29" s="8">
+        <v>0</v>
+      </c>
+      <c r="N29" s="13">
+        <v>180.601843765257</v>
+      </c>
+      <c r="O29" s="4">
+        <v>182.633280201991</v>
+      </c>
+      <c r="P29">
+        <f>8*(N29/B29)^2</f>
+        <v>7.9919705400696046E-3</v>
+      </c>
+      <c r="Q29" s="9">
+        <f t="shared" ref="Q29:Q31" si="25">8*(O29/B29)^2</f>
+        <v>8.1727714408602013E-3</v>
+      </c>
+      <c r="R29" s="10">
+        <f t="shared" ref="R29:R31" si="26">(Q29-P29)/P29</f>
+        <v>2.2622818725883596E-2</v>
+      </c>
+      <c r="S29" s="8">
+        <f t="shared" ref="S29:S31" si="27">100*2*O29/B29</f>
+        <v>6.3924844312912494</v>
+      </c>
+      <c r="T29" s="4">
+        <f t="shared" ref="T29:T31" si="28">B29/4*P29</f>
+        <v>11.416529916489431</v>
+      </c>
+      <c r="U29" s="8">
+        <f t="shared" ref="U29:U31" si="29">E29*N29</f>
+        <v>12.10032353227222</v>
+      </c>
+      <c r="V29" s="8">
+        <f>F29*N29</f>
+        <v>12.10032353227222</v>
+      </c>
+      <c r="W29" s="8">
+        <f t="shared" ref="W29:W31" si="30">G29*N29</f>
+        <v>12.10032353227222</v>
+      </c>
+      <c r="X29" s="8">
+        <f t="shared" ref="X29:X31" si="31">H29*N29</f>
+        <v>3.0250808830680551</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
+      <c r="B30" s="5">
+        <v>5714</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G30">
+        <f>F30</f>
+        <v>0.05</v>
+      </c>
+      <c r="H30" s="5">
+        <f>0.25*G30</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I30" s="5">
+        <v>1</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30" s="8">
+        <v>0</v>
+      </c>
+      <c r="N30" s="13">
+        <v>180.601843765257</v>
+      </c>
+      <c r="O30" s="4">
+        <v>181.289661622458</v>
+      </c>
+      <c r="P30">
+        <f>8*(N30/B30)^2</f>
+        <v>7.9919705400696046E-3</v>
+      </c>
+      <c r="Q30" s="9">
+        <f t="shared" si="25"/>
+        <v>8.0529609217001707E-3</v>
+      </c>
+      <c r="R30" s="10">
+        <f t="shared" si="26"/>
+        <v>7.6314572638595908E-3</v>
+      </c>
+      <c r="S30" s="8">
+        <f t="shared" si="27"/>
+        <v>6.3454554295575081</v>
+      </c>
+      <c r="T30" s="4">
+        <f t="shared" si="28"/>
+        <v>11.416529916489431</v>
+      </c>
+      <c r="U30" s="8">
+        <f t="shared" si="29"/>
+        <v>9.0300921882628504</v>
+      </c>
+      <c r="V30" s="8">
+        <f>F30*N30</f>
+        <v>9.0300921882628504</v>
+      </c>
+      <c r="W30" s="8">
+        <f t="shared" si="30"/>
+        <v>9.0300921882628504</v>
+      </c>
+      <c r="X30" s="8">
+        <f t="shared" si="31"/>
+        <v>2.2575230470657126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
+      <c r="B31" s="5">
+        <v>5714</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F31" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G31">
+        <f>F31</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H31" s="5">
+        <f>0.25*G31</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I31" s="5">
+        <v>1</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31" s="8">
+        <v>0</v>
+      </c>
+      <c r="N31" s="13">
+        <v>180.601843765257</v>
+      </c>
+      <c r="O31" s="4">
+        <v>180.70061309741001</v>
+      </c>
+      <c r="P31">
+        <f>8*(N31/B31)^2</f>
+        <v>7.9919705400696046E-3</v>
+      </c>
+      <c r="Q31" s="9">
+        <f t="shared" si="25"/>
+        <v>8.0007143870129832E-3</v>
+      </c>
+      <c r="R31" s="10">
+        <f t="shared" si="26"/>
+        <v>1.0940789758344649E-3</v>
+      </c>
+      <c r="S31" s="8">
+        <f t="shared" si="27"/>
+        <v>6.3248377002943652</v>
+      </c>
+      <c r="T31" s="4">
+        <f t="shared" si="28"/>
+        <v>11.416529916489431</v>
+      </c>
+      <c r="U31" s="8">
+        <f t="shared" si="29"/>
+        <v>5.9598608442534813</v>
+      </c>
+      <c r="V31" s="8">
+        <f>F31*N31</f>
+        <v>5.9598608442534813</v>
+      </c>
+      <c r="W31" s="8">
+        <f t="shared" si="30"/>
+        <v>5.9598608442534813</v>
+      </c>
+      <c r="X31" s="8">
+        <f t="shared" si="31"/>
+        <v>1.4899652110633703</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24">
+      <c r="B32" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
-      <c r="A26" s="5" t="s">
+    <row r="33" spans="2:20">
+      <c r="B33" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I33" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="J33" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="K33" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L33" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="M33" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="M26" s="5" t="s">
+      <c r="N33" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="O33" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O26" s="5" t="s">
+      <c r="P33" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="P26" s="5" t="s">
+      <c r="Q33" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q26" s="5" t="s">
+      <c r="R33" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R26" s="5" t="s">
+      <c r="S33" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="S26" s="5" t="s">
+      <c r="T33" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
-      <c r="A27" s="5">
+    <row r="34" spans="2:20">
+      <c r="B34" s="5">
         <v>5714</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D27" s="8">
-        <f>18.84*M27/384</f>
+      <c r="E34" s="8">
+        <f>18.84*N34/384</f>
         <v>8.8607779597329213</v>
       </c>
-      <c r="E27" s="8">
-        <f>6.28*M27/256</f>
+      <c r="F34" s="8">
+        <f>6.28*N34/256</f>
         <v>4.4303889798664606</v>
       </c>
-      <c r="F27" s="8">
-        <f>0.0229902*M27</f>
+      <c r="G34" s="8">
+        <f>0.0229902*N34</f>
         <v>4.1520725085320116</v>
       </c>
-      <c r="G27" s="4">
-        <f>0.0001509047*M27</f>
+      <c r="H34" s="4">
+        <f>0.0001509047*N34</f>
         <v>2.7253667052842979E-2</v>
       </c>
-      <c r="H27" s="4">
-        <f>D27/E27</f>
+      <c r="I34" s="4">
+        <f>E34/F34</f>
         <v>2</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="J34" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="K34" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K27">
+      <c r="L34">
         <v>0</v>
       </c>
-      <c r="L27">
+      <c r="M34">
         <v>0</v>
       </c>
-      <c r="M27" s="4">
+      <c r="N34" s="4">
         <v>180.601843765257</v>
       </c>
-      <c r="O27">
-        <f>8*(M27/A27)^2</f>
+      <c r="P34">
+        <f>8*(N34/B34)^2</f>
         <v>7.9919705400696046E-3</v>
       </c>
-      <c r="S27" s="4">
-        <f>2857*O27/2</f>
+      <c r="T34" s="4">
+        <f>2857*P34/2</f>
         <v>11.416529916489431</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
+    <row r="45" spans="2:20">
+      <c r="B45" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
+    <row r="46" spans="2:20">
+      <c r="B46" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3654,10 +4410,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42F51E-90FA-449F-904F-669D9897EDC7}">
-  <dimension ref="A1:T60"/>
+  <dimension ref="A1:T84"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5726,7 +6482,7 @@
     </row>
     <row r="45" spans="1:20">
       <c r="A45" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B45" s="5">
         <v>250000</v>
@@ -5771,7 +6527,7 @@
         <v>5185.8969999999999</v>
       </c>
       <c r="O45" s="17">
-        <v>4839.8902912821904</v>
+        <v>4861.1847284975702</v>
       </c>
       <c r="P45">
         <f>8*(N45/B45)^2</f>
@@ -5779,15 +6535,15 @@
       </c>
       <c r="Q45" s="9">
         <f>8*(O45/B45)^2</f>
-        <v>2.9983408680508937E-3</v>
+        <v>3.0247829714659838E-3</v>
       </c>
       <c r="R45" s="10">
         <f>(Q45-P45)/P45</f>
-        <v>-0.12898975925931722</v>
+        <v>-0.12130839684096101</v>
       </c>
       <c r="S45" s="8">
         <f>500*2*O45/B45</f>
-        <v>19.35956116512876</v>
+        <v>19.444738913990282</v>
       </c>
       <c r="T45" s="4">
         <f>B45/4*P45</f>
@@ -5796,7 +6552,7 @@
     </row>
     <row r="46" spans="1:20">
       <c r="A46" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B46" s="5">
         <v>250000</v>
@@ -5841,7 +6597,7 @@
         <v>5185.8969999999999</v>
       </c>
       <c r="O46" s="17">
-        <v>5098.0300379374303</v>
+        <v>5114.3460867537297</v>
       </c>
       <c r="P46">
         <f>8*(N46/B46)^2</f>
@@ -5849,15 +6605,15 @@
       </c>
       <c r="Q46" s="9">
         <f>8*(O46/B46)^2</f>
-        <v>3.3267085142671764E-3</v>
+        <v>3.3480365945719281E-3</v>
       </c>
       <c r="R46" s="10">
         <f t="shared" ref="R46:R48" si="28">(Q46-P46)/P46</f>
-        <v>-3.3599810227864714E-2</v>
+        <v>-2.7404058250920682E-2</v>
       </c>
       <c r="S46" s="8">
         <f t="shared" ref="S46:S48" si="29">500*2*O46/B46</f>
-        <v>20.392120151749722</v>
+        <v>20.457384347014919</v>
       </c>
       <c r="T46" s="4">
         <f t="shared" ref="T46:T48" si="30">B46/4*P46</f>
@@ -5866,7 +6622,7 @@
     </row>
     <row r="47" spans="1:20">
       <c r="A47" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B47" s="5">
         <v>250000</v>
@@ -5911,7 +6667,7 @@
         <v>5185.8969999999999</v>
       </c>
       <c r="O47" s="17">
-        <v>5115.2850269746104</v>
+        <v>5128.4397753326903</v>
       </c>
       <c r="P47">
         <f>8*(N47/B47)^2</f>
@@ -5919,15 +6675,15 @@
       </c>
       <c r="Q47" s="9">
         <f t="shared" ref="Q47:Q48" si="31">8*(O47/B47)^2</f>
-        <v>3.3492660361204023E-3</v>
+        <v>3.3665144997394457E-3</v>
       </c>
       <c r="R47" s="10">
         <f t="shared" si="28"/>
-        <v>-2.7046908671790545E-2</v>
+        <v>-2.2036274754441386E-2</v>
       </c>
       <c r="S47" s="8">
         <f t="shared" si="29"/>
-        <v>20.461140107898441</v>
+        <v>20.513759101330759</v>
       </c>
       <c r="T47" s="4">
         <f t="shared" si="30"/>
@@ -5936,7 +6692,7 @@
     </row>
     <row r="48" spans="1:20">
       <c r="A48" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B48" s="5">
         <v>250000</v>
@@ -5980,219 +6736,1061 @@
       <c r="N48" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O48" s="17"/>
+      <c r="O48" s="17">
+        <v>5071.0831041415604</v>
+      </c>
       <c r="P48">
         <f>8*(N48/B48)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
       <c r="Q48" s="9">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>3.2916331326860804E-3</v>
       </c>
       <c r="R48" s="10">
         <f t="shared" si="28"/>
-        <v>-1</v>
+        <v>-4.3789117547976646E-2</v>
       </c>
       <c r="S48" s="8">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>20.28433241656624</v>
       </c>
       <c r="T48" s="4">
         <f t="shared" si="30"/>
         <v>215.14822155687202</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
-      <c r="A57" s="5">
+    <row r="51" spans="1:20">
+      <c r="A51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" s="5">
         <v>250000</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="C51" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="D51" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E51" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F51" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G51">
+        <f>F51</f>
+        <v>0.1</v>
+      </c>
+      <c r="H51" s="5">
+        <f>0.25*G51</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I51" s="5">
+        <v>1</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L51">
+        <v>0.1</v>
+      </c>
+      <c r="M51" s="8">
+        <f>L51/H51</f>
+        <v>4</v>
+      </c>
+      <c r="N51" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O51" s="17">
+        <v>4839.8902912821904</v>
+      </c>
+      <c r="P51">
+        <f>8*(N51/B51)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q51" s="9">
+        <f>8*(O51/B51)^2</f>
+        <v>2.9983408680508937E-3</v>
+      </c>
+      <c r="R51" s="10">
+        <f>(Q51-P51)/P51</f>
+        <v>-0.12898975925931722</v>
+      </c>
+      <c r="S51" s="8">
+        <f>500*2*O51/B51</f>
+        <v>19.35956116512876</v>
+      </c>
+      <c r="T51" s="4">
+        <f>B51/4*P51</f>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20">
+      <c r="A52" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E52" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F52" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G52">
+        <f>F52</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H52" s="5">
+        <f>0.25*G52</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I52" s="5">
+        <v>1</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L52">
+        <v>0.1</v>
+      </c>
+      <c r="M52" s="8">
+        <f>L52/H52</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N52" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O52" s="17">
+        <v>5098.0300379374303</v>
+      </c>
+      <c r="P52">
+        <f>8*(N52/B52)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q52" s="9">
+        <f>8*(O52/B52)^2</f>
+        <v>3.3267085142671764E-3</v>
+      </c>
+      <c r="R52" s="10">
+        <f t="shared" ref="R52:R54" si="32">(Q52-P52)/P52</f>
+        <v>-3.3599810227864714E-2</v>
+      </c>
+      <c r="S52" s="8">
+        <f t="shared" ref="S52:S54" si="33">500*2*O52/B52</f>
+        <v>20.392120151749722</v>
+      </c>
+      <c r="T52" s="4">
+        <f t="shared" ref="T52:T54" si="34">B52/4*P52</f>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20">
+      <c r="A53" t="s">
+        <v>134</v>
+      </c>
+      <c r="B53" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F53" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G53">
+        <f>F53</f>
+        <v>0.05</v>
+      </c>
+      <c r="H53" s="5">
+        <f>0.25*G53</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I53" s="5">
+        <v>1</v>
+      </c>
+      <c r="J53" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L53">
+        <v>0.1</v>
+      </c>
+      <c r="M53" s="8">
+        <f>L53/H53</f>
+        <v>8</v>
+      </c>
+      <c r="N53" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O53" s="17">
+        <v>5115.2850269746104</v>
+      </c>
+      <c r="P53">
+        <f>8*(N53/B53)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q53" s="9">
+        <f t="shared" ref="Q53:Q54" si="35">8*(O53/B53)^2</f>
+        <v>3.3492660361204023E-3</v>
+      </c>
+      <c r="R53" s="10">
+        <f t="shared" si="32"/>
+        <v>-2.7046908671790545E-2</v>
+      </c>
+      <c r="S53" s="8">
+        <f t="shared" si="33"/>
+        <v>20.461140107898441</v>
+      </c>
+      <c r="T53" s="4">
+        <f t="shared" si="34"/>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20">
+      <c r="A54" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F54" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G54">
+        <f>F54</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H54" s="5">
+        <f>0.25*G54</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I54" s="5">
+        <v>1</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L54">
+        <v>0.1</v>
+      </c>
+      <c r="M54" s="8">
+        <f>L54/H54</f>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N54" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O54" s="17">
+        <v>5085.5458759715702</v>
+      </c>
+      <c r="P54">
+        <f>8*(N54/B54)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q54" s="9">
+        <f t="shared" si="35"/>
+        <v>3.3104354376462647E-3</v>
+      </c>
+      <c r="R54" s="10">
+        <f t="shared" si="32"/>
+        <v>-3.8327096753624487E-2</v>
+      </c>
+      <c r="S54" s="8">
+        <f t="shared" si="33"/>
+        <v>20.342183503886282</v>
+      </c>
+      <c r="T54" s="4">
+        <f t="shared" si="34"/>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20">
+      <c r="A57" t="s">
+        <v>135</v>
+      </c>
+      <c r="B57" s="5">
+        <v>250000</v>
+      </c>
       <c r="C57" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D57" s="5">
-        <v>0.2</v>
+        <v>136</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="E57" s="5">
         <v>0.1</v>
       </c>
-      <c r="F57">
-        <v>0.1</v>
-      </c>
-      <c r="G57" s="5">
-        <f>0.25*F57</f>
+      <c r="F57" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G57">
+        <f>F57</f>
+        <v>0.1</v>
+      </c>
+      <c r="H57" s="5">
+        <f>0.25*G57</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H57" s="5">
-        <v>2</v>
-      </c>
-      <c r="I57" s="5" t="s">
+      <c r="I57" s="5">
+        <v>1</v>
+      </c>
+      <c r="J57" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J57" s="5" t="s">
+      <c r="K57" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K57">
-        <v>0.1</v>
-      </c>
-      <c r="L57" s="8">
-        <f>K57/G57</f>
+      <c r="L57">
+        <v>0.1</v>
+      </c>
+      <c r="M57" s="8">
+        <f>L57/H57</f>
         <v>4</v>
       </c>
-      <c r="M57" s="8">
+      <c r="N57" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O57">
-        <f>8*(M57/A57)^2</f>
+      <c r="O57" s="17">
+        <v>4865.4971166567602</v>
+      </c>
+      <c r="P57">
+        <f>8*(N57/B57)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
-    </row>
-    <row r="58" spans="1:15">
-      <c r="A58" s="5">
+      <c r="Q57" s="9">
+        <f>8*(O57/B57)^2</f>
+        <v>3.030151960600992E-3</v>
+      </c>
+      <c r="R57" s="10">
+        <f>(Q57-P57)/P57</f>
+        <v>-0.11974871943108145</v>
+      </c>
+      <c r="S57" s="8">
+        <f>500*2*O57/B57</f>
+        <v>19.461988466627044</v>
+      </c>
+      <c r="T57" s="4">
+        <f>B57/4*P57</f>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20">
+      <c r="A58" t="s">
+        <v>135</v>
+      </c>
+      <c r="B58" s="5">
         <v>250000</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C58" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D58" s="5">
-        <f>E58*2</f>
-        <v>0.13400000000000001</v>
+        <v>136</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="E58" s="5">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="F58">
-        <f>E58</f>
+      <c r="F58" s="5">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="G58" s="5">
-        <f>0.25*F58</f>
+      <c r="G58">
+        <f>F58</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H58" s="5">
+        <f>0.25*G58</f>
         <v>1.6750000000000001E-2</v>
       </c>
-      <c r="H58" s="5">
-        <v>2</v>
-      </c>
-      <c r="I58" s="5" t="s">
+      <c r="I58" s="5">
+        <v>1</v>
+      </c>
+      <c r="J58" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J58" s="5" t="s">
+      <c r="K58" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K58">
-        <v>0.1</v>
-      </c>
-      <c r="L58" s="8">
-        <f>K58/G58</f>
+      <c r="L58">
+        <v>0.1</v>
+      </c>
+      <c r="M58" s="8">
+        <f>L58/H58</f>
         <v>5.9701492537313436</v>
       </c>
-      <c r="M58" s="8">
+      <c r="N58" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O58">
-        <f>8*(M58/A58)^2</f>
+      <c r="O58" s="17">
+        <v>5122.4277977756801</v>
+      </c>
+      <c r="P58">
+        <f>8*(N58/B58)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
-    </row>
-    <row r="59" spans="1:15">
-      <c r="A59" s="5">
+      <c r="Q58" s="9">
+        <f>8*(O58/B58)^2</f>
+        <v>3.3586261175584009E-3</v>
+      </c>
+      <c r="R58" s="10">
+        <f t="shared" ref="R58:R60" si="36">(Q58-P58)/P58</f>
+        <v>-2.4327829305753234E-2</v>
+      </c>
+      <c r="S58" s="8">
+        <f t="shared" ref="S58:S60" si="37">500*2*O58/B58</f>
+        <v>20.489711191102721</v>
+      </c>
+      <c r="T58" s="4">
+        <f t="shared" ref="T58:T60" si="38">B58/4*P58</f>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20">
+      <c r="A59" t="s">
+        <v>135</v>
+      </c>
+      <c r="B59" s="5">
         <v>250000</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C59" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D59" s="5">
-        <f t="shared" ref="D59:D60" si="32">E59*2</f>
-        <v>0.1</v>
+        <v>136</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="E59" s="5">
         <v>0.05</v>
       </c>
-      <c r="F59">
-        <f>E59</f>
+      <c r="F59" s="5">
         <v>0.05</v>
       </c>
-      <c r="G59" s="5">
-        <f>0.25*F59</f>
+      <c r="G59">
+        <f>F59</f>
+        <v>0.05</v>
+      </c>
+      <c r="H59" s="5">
+        <f>0.25*G59</f>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="H59" s="5">
-        <v>2</v>
-      </c>
-      <c r="I59" s="5" t="s">
+      <c r="I59" s="5">
+        <v>1</v>
+      </c>
+      <c r="J59" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J59" s="5" t="s">
+      <c r="K59" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K59">
-        <v>0.1</v>
-      </c>
-      <c r="L59" s="8">
-        <f>K59/G59</f>
+      <c r="L59">
+        <v>0.1</v>
+      </c>
+      <c r="M59" s="8">
+        <f>L59/H59</f>
         <v>8</v>
       </c>
-      <c r="M59" s="8">
+      <c r="N59" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O59">
-        <f>8*(M59/A59)^2</f>
+      <c r="O59" s="17">
+        <v>5140.7578715457903</v>
+      </c>
+      <c r="P59">
+        <f>8*(N59/B59)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
-    </row>
-    <row r="60" spans="1:15">
-      <c r="A60" s="5">
+      <c r="Q59" s="9">
+        <f t="shared" ref="Q59:Q60" si="39">8*(O59/B59)^2</f>
+        <v>3.382706111214081E-3</v>
+      </c>
+      <c r="R59" s="10">
+        <f t="shared" si="36"/>
+        <v>-1.7332653642252921E-2</v>
+      </c>
+      <c r="S59" s="8">
+        <f t="shared" si="37"/>
+        <v>20.563031486183164</v>
+      </c>
+      <c r="T59" s="4">
+        <f t="shared" si="38"/>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20">
+      <c r="A60" t="s">
+        <v>135</v>
+      </c>
+      <c r="B60" s="5">
         <v>250000</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C60" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D60" s="5">
-        <f t="shared" si="32"/>
-        <v>6.6000000000000003E-2</v>
+        <v>136</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="E60" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F60">
-        <f>E60</f>
+      <c r="F60" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="G60" s="5">
-        <f>0.25*F60</f>
+      <c r="G60">
+        <f>F60</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H60" s="5">
+        <f>0.25*G60</f>
         <v>8.2500000000000004E-3</v>
       </c>
-      <c r="H60" s="5">
+      <c r="I60" s="5">
+        <v>1</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K60" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L60">
+        <v>0.1</v>
+      </c>
+      <c r="M60" s="8">
+        <f>L60/H60</f>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N60" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O60" s="17">
+        <v>5161.2717558357099</v>
+      </c>
+      <c r="P60">
+        <f>8*(N60/B60)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q60" s="9">
+        <f t="shared" si="39"/>
+        <v>3.4097569456111917E-3</v>
+      </c>
+      <c r="R60" s="10">
+        <f t="shared" si="36"/>
+        <v>-9.4744564534255601E-3</v>
+      </c>
+      <c r="S60" s="8">
+        <f t="shared" si="37"/>
+        <v>20.645087023342839</v>
+      </c>
+      <c r="T60" s="4">
+        <f t="shared" si="38"/>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20">
+      <c r="A63" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E63" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F63" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G63">
+        <f>F63</f>
+        <v>0.1</v>
+      </c>
+      <c r="H63" s="5">
+        <f>0.25*G63</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I63" s="5">
+        <v>1</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L63">
+        <v>0.1</v>
+      </c>
+      <c r="M63" s="8">
+        <f>L63/H63</f>
+        <v>4</v>
+      </c>
+      <c r="N63" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O63" s="17">
+        <v>4863.0764273383802</v>
+      </c>
+      <c r="P63">
+        <f>8*(N63/B63)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q63" s="9">
+        <f>8*(O63/B63)^2</f>
+        <v>3.0271375792811804E-3</v>
+      </c>
+      <c r="R63" s="10">
+        <f>(Q63-P63)/P63</f>
+        <v>-0.12062438938142973</v>
+      </c>
+      <c r="S63" s="8">
+        <f>500*2*O63/B63</f>
+        <v>19.452305709353521</v>
+      </c>
+      <c r="T63" s="4">
+        <f>B63/4*P63</f>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20">
+      <c r="A64" t="s">
+        <v>142</v>
+      </c>
+      <c r="B64" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E64" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F64" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G64">
+        <f>F64</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H64" s="5">
+        <f>0.25*G64</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I64" s="5">
+        <v>1</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L64">
+        <v>0.1</v>
+      </c>
+      <c r="M64" s="8">
+        <f>L64/H64</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N64" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O64" s="17">
+        <v>5118.5994558266202</v>
+      </c>
+      <c r="P64">
+        <f>8*(N64/B64)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q64" s="9">
+        <f>8*(O64/B64)^2</f>
+        <v>3.353607729816137E-3</v>
+      </c>
+      <c r="R64" s="10">
+        <f t="shared" ref="R64:R66" si="40">(Q64-P64)/P64</f>
+        <v>-2.5785657920936959E-2</v>
+      </c>
+      <c r="S64" s="8">
+        <f t="shared" ref="S64:S66" si="41">500*2*O64/B64</f>
+        <v>20.474397823306482</v>
+      </c>
+      <c r="T64" s="4">
+        <f t="shared" ref="T64:T66" si="42">B64/4*P64</f>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20">
+      <c r="A65" t="s">
+        <v>142</v>
+      </c>
+      <c r="B65" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E65" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F65" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G65">
+        <f>F65</f>
+        <v>0.05</v>
+      </c>
+      <c r="H65" s="5">
+        <f>0.25*G65</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I65" s="5">
+        <v>1</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L65">
+        <v>0.1</v>
+      </c>
+      <c r="M65" s="8">
+        <f>L65/H65</f>
+        <v>8</v>
+      </c>
+      <c r="N65" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O65" s="17">
+        <v>5140.2711235485604</v>
+      </c>
+      <c r="P65">
+        <f>8*(N65/B65)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q65" s="9">
+        <f t="shared" ref="Q65:Q66" si="43">8*(O65/B65)^2</f>
+        <v>3.3820655646191588E-3</v>
+      </c>
+      <c r="R65" s="10">
+        <f t="shared" si="40"/>
+        <v>-1.7518730765702695E-2</v>
+      </c>
+      <c r="S65" s="8">
+        <f t="shared" si="41"/>
+        <v>20.561084494194244</v>
+      </c>
+      <c r="T65" s="4">
+        <f t="shared" si="42"/>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20">
+      <c r="A66" t="s">
+        <v>142</v>
+      </c>
+      <c r="B66" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E66" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F66" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G66">
+        <f>F66</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H66" s="5">
+        <f>0.25*G66</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I66" s="5">
+        <v>1</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L66">
+        <v>0.1</v>
+      </c>
+      <c r="M66" s="8">
+        <f>L66/H66</f>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N66" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O66" s="17">
+        <v>5164.2975147391799</v>
+      </c>
+      <c r="P66">
+        <f>8*(N66/B66)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q66" s="9">
+        <f t="shared" si="43"/>
+        <v>3.4137560090548827E-3</v>
+      </c>
+      <c r="R66" s="10">
+        <f t="shared" si="40"/>
+        <v>-8.3127389015813305E-3</v>
+      </c>
+      <c r="S66" s="8">
+        <f t="shared" si="41"/>
+        <v>20.657190058956719</v>
+      </c>
+      <c r="T66" s="4">
+        <f t="shared" si="42"/>
+        <v>215.14822155687202</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
+      <c r="A81" s="5">
+        <v>250000</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D81" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E81" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F81">
+        <v>0.1</v>
+      </c>
+      <c r="G81" s="5">
+        <f>0.25*F81</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H81" s="5">
         <v>2</v>
       </c>
-      <c r="I60" s="5" t="s">
+      <c r="I81" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J60" s="5" t="s">
+      <c r="J81" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K60">
-        <v>0.1</v>
-      </c>
-      <c r="L60" s="8">
-        <f>K60/G60</f>
+      <c r="K81">
+        <v>0.1</v>
+      </c>
+      <c r="L81" s="8">
+        <f>K81/G81</f>
+        <v>4</v>
+      </c>
+      <c r="M81" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O81">
+        <f>8*(M81/A81)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
+      <c r="A82" s="5">
+        <v>250000</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D82" s="5">
+        <f>E82*2</f>
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="E82" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F82">
+        <f>E82</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G82" s="5">
+        <f>0.25*F82</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="H82" s="5">
+        <v>2</v>
+      </c>
+      <c r="I82" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K82">
+        <v>0.1</v>
+      </c>
+      <c r="L82" s="8">
+        <f>K82/G82</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="M82" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O82">
+        <f>8*(M82/A82)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
+      <c r="A83" s="5">
+        <v>250000</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D83" s="5">
+        <f t="shared" ref="D83:D84" si="44">E83*2</f>
+        <v>0.1</v>
+      </c>
+      <c r="E83" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F83">
+        <f>E83</f>
+        <v>0.05</v>
+      </c>
+      <c r="G83" s="5">
+        <f>0.25*F83</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="H83" s="5">
+        <v>2</v>
+      </c>
+      <c r="I83" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K83">
+        <v>0.1</v>
+      </c>
+      <c r="L83" s="8">
+        <f>K83/G83</f>
+        <v>8</v>
+      </c>
+      <c r="M83" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O83">
+        <f>8*(M83/A83)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
+      <c r="A84" s="5">
+        <v>250000</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D84" s="5">
+        <f t="shared" si="44"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="E84" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F84">
+        <f>E84</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G84" s="5">
+        <f>0.25*F84</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="H84" s="5">
+        <v>2</v>
+      </c>
+      <c r="I84" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J84" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K84">
+        <v>0.1</v>
+      </c>
+      <c r="L84" s="8">
+        <f>K84/G84</f>
         <v>12.121212121212121</v>
       </c>
-      <c r="M60" s="8">
+      <c r="M84" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O60">
-        <f>8*(M60/A60)^2</f>
+      <c r="O84">
+        <f>8*(M84/A84)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
temporary damping of Moin, Kim 1982
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7595DB3F-A977-4B2D-8034-EA81125513FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDD73BE-779A-4D69-A6D7-1CA01A1ABF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="debug" sheetId="1" r:id="rId1"/>
     <sheet name="CHA_RETAU180" sheetId="9" r:id="rId2"/>
     <sheet name="CHA_RETAU550" sheetId="7" r:id="rId3"/>
-    <sheet name="CHA_RETAU1000" sheetId="4" r:id="rId4"/>
-    <sheet name="CHA_RETAU5200" sheetId="6" r:id="rId5"/>
-    <sheet name="main" sheetId="2" r:id="rId6"/>
-    <sheet name="initsolver" sheetId="3" r:id="rId7"/>
-    <sheet name="notes" sheetId="5" r:id="rId8"/>
+    <sheet name="CHA_RETAU395" sheetId="10" r:id="rId4"/>
+    <sheet name="CHA_RETAU1000" sheetId="4" r:id="rId5"/>
+    <sheet name="CHA_RETAU5200" sheetId="6" r:id="rId6"/>
+    <sheet name="main" sheetId="2" r:id="rId7"/>
+    <sheet name="initsolver" sheetId="3" r:id="rId8"/>
+    <sheet name="notes" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="175">
   <si>
     <t>nompi</t>
   </si>
@@ -531,14 +532,76 @@
   <si>
     <t>dz</t>
   </si>
+  <si>
+    <t>328×256×196</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>(gtype,gr)=(1,5)</t>
+  </si>
+  <si>
+    <t>6.4×2.4×2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 192×128×128</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 96×64×128</t>
+  </si>
+  <si>
+    <t>NOSLIP+SMAG+SMALL</t>
+  </si>
+  <si>
+    <t>NOSLIP+SMAG+SMALL+EXP</t>
+  </si>
+  <si>
+    <t>NOSLIP+SMAG+SMALL+CS0.2</t>
+  </si>
+  <si>
+    <t>NOSLIP+SMAG+SMALL+CS0</t>
+  </si>
+  <si>
+    <t>NOSLIP+SMAG+SMALL+CS0.16</t>
+  </si>
+  <si>
+    <t>NOSLIP+SMAG+SMALL+CS0.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 192×128×192</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 96×64×64</t>
+  </si>
+  <si>
+    <t>(gtype,gr)=(1,4)</t>
+  </si>
+  <si>
+    <t>NOSLIP+SMAG+SMALL+CS0.1</t>
+  </si>
+  <si>
+    <t>6.28×2.355×2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 48×48×64</t>
+  </si>
+  <si>
+    <t>(gtype,gr)=(1,4.3)</t>
+  </si>
+  <si>
+    <t>NOSLIP+SMAG+SMALL+CS0.18</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -600,7 +663,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -632,16 +695,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760F17C5-A88B-45BD-B60F-0BA67AB143DF}">
   <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView topLeftCell="A62" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1406,185 +1472,150 @@
         <v>99</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
         <v>151</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B80" t="s">
         <v>144</v>
-      </c>
-      <c r="C75" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="B76" t="s">
-        <v>145</v>
-      </c>
-      <c r="C76" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="B77" t="s">
-        <v>146</v>
-      </c>
-      <c r="C77" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>153</v>
-      </c>
-      <c r="B79" t="s">
-        <v>144</v>
-      </c>
-      <c r="C79" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="B80" t="s">
-        <v>145</v>
       </c>
       <c r="C80" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:3">
       <c r="B81" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C81" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
-      <c r="A85" t="s">
+    <row r="82" spans="1:3">
+      <c r="B82" t="s">
+        <v>146</v>
+      </c>
+      <c r="C82" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>153</v>
+      </c>
+      <c r="B84" t="s">
+        <v>144</v>
+      </c>
+      <c r="C84" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="B85" t="s">
+        <v>145</v>
+      </c>
+      <c r="C85" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="B86" t="s">
+        <v>146</v>
+      </c>
+      <c r="C86" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
         <v>150</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B90" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
-      <c r="B86" t="s">
+    <row r="91" spans="1:3">
+      <c r="B91" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="B87" t="s">
+    <row r="92" spans="1:3">
+      <c r="B92" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
-      <c r="A93" t="s">
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
         <v>90</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B98" t="s">
         <v>88</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C98" t="s">
         <v>87</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D98" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
-      <c r="A94" t="s">
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
         <v>91</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B99" t="s">
         <v>95</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C99" t="s">
         <v>95</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D99" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="15" t="s">
+    <row r="100" spans="1:4">
+      <c r="A100" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B100" t="s">
         <v>95</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C100" t="s">
         <v>95</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D100" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="15" t="s">
+    <row r="101" spans="1:4">
+      <c r="A101" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B101" t="s">
         <v>95</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C101" t="s">
         <v>95</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D101" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
-      <c r="A97" t="s">
+    <row r="102" spans="1:4">
+      <c r="A102" t="s">
         <v>94</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B102" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
-      <c r="C100" t="s">
+    <row r="105" spans="1:4">
+      <c r="C105" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
-      <c r="A101" t="s">
+    <row r="106" spans="1:4">
+      <c r="A106" t="s">
         <v>114</v>
-      </c>
-      <c r="B101" t="s">
-        <v>110</v>
-      </c>
-      <c r="C101" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="B102" t="s">
-        <v>108</v>
-      </c>
-      <c r="C102" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="B103" t="s">
-        <v>109</v>
-      </c>
-      <c r="C103" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="B104" t="s">
-        <v>111</v>
-      </c>
-      <c r="C104" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" t="s">
-        <v>112</v>
       </c>
       <c r="B106" t="s">
         <v>110</v>
@@ -1593,11 +1624,46 @@
         <v>117</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="s">
+    <row r="107" spans="1:4">
+      <c r="B107" t="s">
+        <v>108</v>
+      </c>
+      <c r="C107" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="B108" t="s">
+        <v>109</v>
+      </c>
+      <c r="C108" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="B109" t="s">
+        <v>111</v>
+      </c>
+      <c r="C109" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>112</v>
+      </c>
+      <c r="B111" t="s">
+        <v>110</v>
+      </c>
+      <c r="C111" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
         <v>113</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B113" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1654,7 +1720,7 @@
   <dimension ref="A1:X46"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:X24"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2009,59 +2075,59 @@
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="17" t="s">
+      <c r="A5" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="5">
         <v>5714</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5">
         <f>F5</f>
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="5">
         <f>0.25*G5</f>
         <v>8.2500000000000004E-3</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="5">
         <v>1</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="M5" s="19">
+      <c r="L5">
+        <v>0.1</v>
+      </c>
+      <c r="M5" s="8">
         <f t="shared" si="0"/>
         <v>12.121212121212121</v>
       </c>
-      <c r="N5" s="20">
+      <c r="N5" s="12">
         <v>180.601843765257</v>
       </c>
-      <c r="O5" s="21">
+      <c r="O5" s="4">
         <v>183.668368577509</v>
       </c>
-      <c r="P5" s="17">
+      <c r="P5">
         <f>8*(N5/B5)^2</f>
         <v>7.9919705400696046E-3</v>
       </c>
-      <c r="Q5" s="22">
+      <c r="Q5" s="9">
         <f t="shared" si="1"/>
         <v>8.2656736025973811E-3</v>
       </c>
@@ -2069,27 +2135,27 @@
         <f t="shared" si="2"/>
         <v>3.4247256187382384E-2</v>
       </c>
-      <c r="S5" s="19">
+      <c r="S5" s="8">
         <f t="shared" si="3"/>
         <v>6.4287143359296115</v>
       </c>
-      <c r="T5" s="21">
+      <c r="T5" s="4">
         <f t="shared" si="4"/>
         <v>11.416529916489431</v>
       </c>
-      <c r="U5" s="19">
+      <c r="U5" s="8">
         <f t="shared" si="5"/>
         <v>5.9598608442534813</v>
       </c>
-      <c r="V5" s="19">
+      <c r="V5" s="8">
         <f t="shared" si="6"/>
         <v>6.0610561630577973</v>
       </c>
-      <c r="W5" s="19">
+      <c r="W5" s="8">
         <f t="shared" si="7"/>
         <v>5.9598608442534813</v>
       </c>
-      <c r="X5" s="21">
+      <c r="X5" s="4">
         <f t="shared" si="8"/>
         <v>1.4899652110633703</v>
       </c>
@@ -3467,15 +3533,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3643DFC1-43AF-4E64-819A-C97D29654F85}">
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection sqref="A1:X29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="1" max="1" width="29.81640625" customWidth="1"/>
     <col min="3" max="3" width="16.81640625" customWidth="1"/>
     <col min="4" max="4" width="14.7265625" customWidth="1"/>
     <col min="7" max="7" width="12.26953125" customWidth="1"/>
@@ -4481,11 +4547,11 @@
         <v>36.96725</v>
       </c>
       <c r="W15" s="8">
-        <f t="shared" ref="W15:W17" si="25">G15*N15</f>
+        <f t="shared" ref="W15:W20" si="25">G15*N15</f>
         <v>36.96725</v>
       </c>
       <c r="X15" s="8">
-        <f t="shared" ref="X15:X17" si="26">H15*N15</f>
+        <f t="shared" ref="X15:X20" si="26">H15*N15</f>
         <v>9.2418125</v>
       </c>
     </row>
@@ -4661,26 +4727,851 @@
         <v>4.5519375000000002</v>
       </c>
     </row>
+    <row r="18" spans="1:24">
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="A20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E20" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F20" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G20" s="18">
+        <v>3.9572349999999999E-2</v>
+      </c>
+      <c r="H20" s="13">
+        <v>1.094476E-3</v>
+      </c>
+      <c r="I20" s="19">
+        <f>E20/F20</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M20" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N20" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O20" s="4">
+        <v>578.06178766221899</v>
+      </c>
+      <c r="P20" s="9">
+        <f>8*(N20/B20)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q20" s="9">
+        <f>8*(O20/B20)^2</f>
+        <v>6.3363277269372579E-3</v>
+      </c>
+      <c r="R20" s="10">
+        <f>(Q20-P20)/P20</f>
+        <v>9.7649893413621749E-2</v>
+      </c>
+      <c r="S20" s="8">
+        <f>200*2*O20/B20</f>
+        <v>11.257288951552463</v>
+      </c>
+      <c r="T20" s="4">
+        <f>B20/4*P20</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U20" s="8">
+        <f>E20*N20</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V20" s="8">
+        <f>F20*N20</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W20" s="8">
+        <f t="shared" si="25"/>
+        <v>21.834044112499999</v>
+      </c>
+      <c r="X20" s="8">
+        <f t="shared" si="26"/>
+        <v>0.60387713300000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
+      <c r="A21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E21" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F21" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G21" s="18">
+        <v>3.9572349999999999E-2</v>
+      </c>
+      <c r="H21" s="13">
+        <v>1.094476E-3</v>
+      </c>
+      <c r="I21" s="19">
+        <f>E21/F21</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M21" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N21" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O21" s="4">
+        <v>578.37192198948799</v>
+      </c>
+      <c r="P21" s="9">
+        <f>8*(N21/B21)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q21" s="9">
+        <f>8*(O21/B21)^2</f>
+        <v>6.3431285220338944E-3</v>
+      </c>
+      <c r="R21" s="10">
+        <f>(Q21-P21)/P21</f>
+        <v>9.8828003564271918E-2</v>
+      </c>
+      <c r="S21" s="8">
+        <f>200*2*O21/B21</f>
+        <v>11.26332856844183</v>
+      </c>
+      <c r="T21" s="4">
+        <f>B21/4*P21</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U21" s="8">
+        <f>E21*N21</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V21" s="8">
+        <f>F21*N21</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W21" s="8">
+        <f t="shared" ref="W21" si="27">G21*N21</f>
+        <v>21.834044112499999</v>
+      </c>
+      <c r="X21" s="8">
+        <f t="shared" ref="X21" si="28">H21*N21</f>
+        <v>0.60387713300000001</v>
+      </c>
+    </row>
     <row r="22" spans="1:24">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
+      <c r="A22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F22" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G22" s="18">
+        <v>3.9572349999999999E-2</v>
+      </c>
+      <c r="H22" s="13">
+        <v>1.094476E-3</v>
+      </c>
+      <c r="I22" s="19">
+        <f>E22/F22</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M22" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N22" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O22" s="4">
+        <v>579.86554202636</v>
+      </c>
+      <c r="P22" s="9">
+        <f>8*(N22/B22)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q22" s="9">
+        <f>8*(O22/B22)^2</f>
+        <v>6.3759325254074605E-3</v>
+      </c>
+      <c r="R22" s="10">
+        <f>(Q22-P22)/P22</f>
+        <v>0.10451068166399509</v>
+      </c>
+      <c r="S22" s="8">
+        <f>200*2*O22/B22</f>
+        <v>11.292415618819085</v>
+      </c>
+      <c r="T22" s="4">
+        <f>B22/4*P22</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U22" s="8">
+        <f>E22*N22</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V22" s="8">
+        <f>F22*N22</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W22" s="8">
+        <f t="shared" ref="W22:W25" si="29">G22*N22</f>
+        <v>21.834044112499999</v>
+      </c>
+      <c r="X22" s="8">
+        <f t="shared" ref="X22:X25" si="30">H22*N22</f>
+        <v>0.60387713300000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
+      <c r="A23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E23" s="18">
+        <v>3.3333333333333298E-2</v>
+      </c>
+      <c r="F23" s="5">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="G23" s="18">
+        <v>2.6389220000000001E-2</v>
+      </c>
+      <c r="H23" s="13">
+        <v>7.2024380000000002E-4</v>
+      </c>
+      <c r="I23" s="19">
+        <f>E23/F23</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M23" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N23" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O23" s="4">
+        <v>565.82317299089596</v>
+      </c>
+      <c r="P23" s="9">
+        <f>8*(N23/B23)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q23" s="9">
+        <f>8*(O23/B23)^2</f>
+        <v>6.0708648969258526E-3</v>
+      </c>
+      <c r="R23" s="10">
+        <f>(Q23-P23)/P23</f>
+        <v>5.1663438857531101E-2</v>
+      </c>
+      <c r="S23" s="8">
+        <v>11</v>
+      </c>
+      <c r="T23" s="4">
+        <f>B23/4*P23</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U23" s="8">
+        <f>E23*N23</f>
+        <v>18.391666666666648</v>
+      </c>
+      <c r="V23" s="8">
+        <f>F23*N23</f>
+        <v>10.3453125</v>
+      </c>
+      <c r="W23" s="8">
+        <f t="shared" si="29"/>
+        <v>14.560252135000001</v>
+      </c>
+      <c r="X23" s="8">
+        <f t="shared" si="30"/>
+        <v>0.39739451665000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
+      <c r="A24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E24" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F24" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G24" s="18">
+        <v>3.9572349999999999E-2</v>
+      </c>
+      <c r="H24" s="13">
+        <v>1.094476E-3</v>
+      </c>
+      <c r="I24" s="19">
+        <f>E24/F24</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M24" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N24" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O24" s="4">
+        <v>596.476571008257</v>
+      </c>
+      <c r="P24" s="9">
+        <f>8*(N24/B24)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q24" s="9">
+        <f>8*(O24/B24)^2</f>
+        <v>6.7464590385163999E-3</v>
+      </c>
+      <c r="R24" s="10">
+        <f>(Q24-P24)/P24</f>
+        <v>0.16869744806055201</v>
+      </c>
+      <c r="S24" s="8">
+        <f>200*2*O24/B24</f>
+        <v>11.615902064425647</v>
+      </c>
+      <c r="T24" s="4">
+        <f>B24/4*P24</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U24" s="8">
+        <f>E24*N24</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V24" s="8">
+        <f>F24*N24</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W24" s="8">
+        <f t="shared" si="29"/>
+        <v>21.834044112499999</v>
+      </c>
+      <c r="X24" s="8">
+        <f t="shared" si="30"/>
+        <v>0.60387713300000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24">
+      <c r="A25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B25" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E25" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F25" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G25" s="18">
+        <v>3.9572349999999999E-2</v>
+      </c>
+      <c r="H25" s="13">
+        <v>1.094476E-3</v>
+      </c>
+      <c r="I25" s="19">
+        <f>E25/F25</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M25" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N25" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O25" s="4">
+        <v>534.15584016732998</v>
+      </c>
+      <c r="P25" s="9">
+        <f>8*(N25/B25)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q25" s="9">
+        <f>8*(O25/B25)^2</f>
+        <v>5.4103463844241738E-3</v>
+      </c>
+      <c r="R25" s="10">
+        <f>(Q25-P25)/P25</f>
+        <v>-6.2759000462165856E-2</v>
+      </c>
+      <c r="S25" s="8">
+        <f>200*2*O25/B25</f>
+        <v>10.402255894203115</v>
+      </c>
+      <c r="T25" s="4">
+        <f>B25/4*P25</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U25" s="8">
+        <f>E25*N25</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V25" s="8">
+        <f>F25*N25</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W25" s="8">
+        <f t="shared" si="29"/>
+        <v>21.834044112499999</v>
+      </c>
+      <c r="X25" s="8">
+        <f t="shared" si="30"/>
+        <v>0.60387713300000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24">
+      <c r="A26" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E26" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F26" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G26" s="18">
+        <v>3.9572349999999999E-2</v>
+      </c>
+      <c r="H26" s="13">
+        <v>1.094476E-3</v>
+      </c>
+      <c r="I26" s="19">
+        <f>E26/F26</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M26" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N26" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O26" s="4">
+        <v>554.62637104913404</v>
+      </c>
+      <c r="P26" s="9">
+        <f>8*(N26/B26)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q26" s="9">
+        <f>8*(O26/B26)^2</f>
+        <v>5.832975322820017E-3</v>
+      </c>
+      <c r="R26" s="10">
+        <f>(Q26-P26)/P26</f>
+        <v>1.0453533544174207E-2</v>
+      </c>
+      <c r="S26" s="8">
+        <f>200*2*O26/B26</f>
+        <v>10.80090303893153</v>
+      </c>
+      <c r="T26" s="4">
+        <f>B26/4*P26</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U26" s="8">
+        <f>E26*N26</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V26" s="8">
+        <f>F26*N26</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W26" s="8">
+        <f t="shared" ref="W26" si="31">G26*N26</f>
+        <v>21.834044112499999</v>
+      </c>
+      <c r="X26" s="8">
+        <f t="shared" ref="X26" si="32">H26*N26</f>
+        <v>0.60387713300000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24">
+      <c r="A27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B27" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F27" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G27" s="18">
+        <v>3.9572349999999999E-2</v>
+      </c>
+      <c r="H27" s="13">
+        <v>1.094476E-3</v>
+      </c>
+      <c r="I27" s="19">
+        <f>E27/F27</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M27" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N27" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O27" s="4">
+        <v>559.636338939957</v>
+      </c>
+      <c r="P27" s="9">
+        <f>8*(N27/B27)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q27" s="9">
+        <f>8*(O27/B27)^2</f>
+        <v>5.9388303888888699E-3</v>
+      </c>
+      <c r="R27" s="10">
+        <f>(Q27-P27)/P27</f>
+        <v>2.879093763610727E-2</v>
+      </c>
+      <c r="S27" s="8">
+        <f>200*2*O27/B27</f>
+        <v>10.898468139044926</v>
+      </c>
+      <c r="T27" s="4">
+        <f>B27/4*P27</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U27" s="8">
+        <f>E27*N27</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V27" s="8">
+        <f>F27*N27</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W27" s="8">
+        <f t="shared" ref="W27:W29" si="33">G27*N27</f>
+        <v>21.834044112499999</v>
+      </c>
+      <c r="X27" s="8">
+        <f t="shared" ref="X27:X29" si="34">H27*N27</f>
+        <v>0.60387713300000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24">
+      <c r="A28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E28" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F28" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G28" s="18">
+        <v>7.9024239999999996E-2</v>
+      </c>
+      <c r="H28" s="13">
+        <v>2.2765490000000001E-3</v>
+      </c>
+      <c r="I28" s="19">
+        <f>E28/F28</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M28" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N28" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O28" s="4">
+        <v>552.56079223245501</v>
+      </c>
+      <c r="P28" s="9">
+        <f>8*(N28/B28)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q28" s="9">
+        <f>8*(O28/B28)^2</f>
+        <v>5.7896090675909791E-3</v>
+      </c>
+      <c r="R28" s="10">
+        <f>(Q28-P28)/P28</f>
+        <v>2.9411434846231123E-3</v>
+      </c>
+      <c r="S28" s="8">
+        <v>11</v>
+      </c>
+      <c r="T28" s="4">
+        <f>B28/4*P28</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U28" s="8">
+        <f>E28*N28</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V28" s="8">
+        <f>F28*N28</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W28" s="8">
+        <f t="shared" si="33"/>
+        <v>43.60162442</v>
+      </c>
+      <c r="X28" s="8">
+        <f t="shared" si="34"/>
+        <v>1.25608591075</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
+      <c r="A29" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E29" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F29" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G29" s="18">
+        <v>3.2405539999999997E-2</v>
+      </c>
+      <c r="H29" s="13">
+        <v>2.3605689999999999E-3</v>
+      </c>
+      <c r="I29" s="19">
+        <f>E29/F29</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M29" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N29" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O29" s="4">
+        <v>579.946521286814</v>
+      </c>
+      <c r="P29" s="9">
+        <f>8*(N29/B29)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q29" s="9">
+        <f>8*(O29/B29)^2</f>
+        <v>6.3777134705251676E-3</v>
+      </c>
+      <c r="R29" s="10">
+        <f>(Q29-P29)/P29</f>
+        <v>0.10481919699067493</v>
+      </c>
+      <c r="S29" s="8">
+        <f>200*2*O29/B29</f>
+        <v>11.293992624864927</v>
+      </c>
+      <c r="T29" s="4">
+        <f>B29/4*P29</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U29" s="8">
+        <f>E29*N29</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V29" s="8">
+        <f>F29*N29</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W29" s="8">
+        <f t="shared" si="33"/>
+        <v>17.879756694999998</v>
+      </c>
+      <c r="X29" s="8">
+        <f t="shared" si="34"/>
+        <v>1.3024439457499999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4688,11 +5579,857 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B745900-CF34-4783-B8B3-D2DA1ADCC55F}">
+  <dimension ref="A1:X29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y11" sqref="Y11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26953125" customWidth="1"/>
+    <col min="16" max="17" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.08984375" customWidth="1"/>
+    <col min="19" max="19" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="5">
+        <v>13750</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="18">
+        <v>0.130833333333333</v>
+      </c>
+      <c r="F2" s="21">
+        <v>4.8645833333333298E-2</v>
+      </c>
+      <c r="G2" s="18">
+        <v>6.8932160000000006E-2</v>
+      </c>
+      <c r="H2" s="13">
+        <v>3.896123E-3</v>
+      </c>
+      <c r="I2" s="19">
+        <f>E2/F2</f>
+        <v>2.6895074946466759</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N2" s="12">
+        <v>392.24</v>
+      </c>
+      <c r="O2" s="12">
+        <v>419.189718479828</v>
+      </c>
+      <c r="P2" s="9">
+        <f>8*(N2/B2)^2</f>
+        <v>6.5101103645619834E-3</v>
+      </c>
+      <c r="Q2" s="9">
+        <f>8*(O2/B2)^2</f>
+        <v>7.4354256430205863E-3</v>
+      </c>
+      <c r="R2" s="10">
+        <f>(Q2-P2)/P2</f>
+        <v>0.14213511394454836</v>
+      </c>
+      <c r="S2" s="8">
+        <f>200*2*O2/B2</f>
+        <v>12.194609992140451</v>
+      </c>
+      <c r="T2" s="4">
+        <f>B2/4*P2</f>
+        <v>22.37850437818182</v>
+      </c>
+      <c r="U2" s="8">
+        <f>E2*N2</f>
+        <v>51.318066666666539</v>
+      </c>
+      <c r="V2" s="8">
+        <f>F2*N2</f>
+        <v>19.080841666666654</v>
+      </c>
+      <c r="W2" s="8">
+        <f>G2*N2</f>
+        <v>27.037950438400003</v>
+      </c>
+      <c r="X2" s="8">
+        <f>H2*N2</f>
+        <v>1.52821528552</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="5">
+        <v>13750</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="18">
+        <v>0.130833333333333</v>
+      </c>
+      <c r="F3" s="21">
+        <v>4.8645833333333298E-2</v>
+      </c>
+      <c r="G3" s="18">
+        <v>6.8932160000000006E-2</v>
+      </c>
+      <c r="H3" s="13">
+        <v>3.896123E-3</v>
+      </c>
+      <c r="I3" s="19">
+        <f>E3/F3</f>
+        <v>2.6895074946466759</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N3" s="12">
+        <v>392.24</v>
+      </c>
+      <c r="O3" s="12">
+        <v>400.57025121806299</v>
+      </c>
+      <c r="P3" s="9">
+        <f>8*(N3/B3)^2</f>
+        <v>6.5101103645619834E-3</v>
+      </c>
+      <c r="Q3" s="9">
+        <f>8*(O3/B3)^2</f>
+        <v>6.7895654044943703E-3</v>
+      </c>
+      <c r="R3" s="10">
+        <f>(Q3-P3)/P3</f>
+        <v>4.2926313730963811E-2</v>
+      </c>
+      <c r="S3" s="8">
+        <f>200*2*O3/B3</f>
+        <v>11.652952762707287</v>
+      </c>
+      <c r="T3" s="4">
+        <f>B3/4*P3</f>
+        <v>22.37850437818182</v>
+      </c>
+      <c r="U3" s="8">
+        <f>E3*N3</f>
+        <v>51.318066666666539</v>
+      </c>
+      <c r="V3" s="8">
+        <f>F3*N3</f>
+        <v>19.080841666666654</v>
+      </c>
+      <c r="W3" s="8">
+        <f>G3*N3</f>
+        <v>27.037950438400003</v>
+      </c>
+      <c r="X3" s="8">
+        <f>H3*N3</f>
+        <v>1.52821528552</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" s="5">
+        <v>13750</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.130833333333333</v>
+      </c>
+      <c r="F4" s="21">
+        <v>4.8645833333333298E-2</v>
+      </c>
+      <c r="G4" s="18">
+        <v>6.8932160000000006E-2</v>
+      </c>
+      <c r="H4" s="13">
+        <v>3.896123E-3</v>
+      </c>
+      <c r="I4" s="19">
+        <f>E4/F4</f>
+        <v>2.6895074946466759</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N4" s="12">
+        <v>392.24</v>
+      </c>
+      <c r="O4" s="12">
+        <v>352.74297174230901</v>
+      </c>
+      <c r="P4" s="9">
+        <f>8*(N4/B4)^2</f>
+        <v>6.5101103645619834E-3</v>
+      </c>
+      <c r="Q4" s="9">
+        <f>8*(O4/B4)^2</f>
+        <v>5.2650358104265162E-3</v>
+      </c>
+      <c r="R4" s="10">
+        <f>(Q4-P4)/P4</f>
+        <v>-0.19125244956108189</v>
+      </c>
+      <c r="S4" s="8">
+        <f>200*2*O4/B4</f>
+        <v>10.261613723412626</v>
+      </c>
+      <c r="T4" s="4">
+        <f>B4/4*P4</f>
+        <v>22.37850437818182</v>
+      </c>
+      <c r="U4" s="8">
+        <f>E4*N4</f>
+        <v>51.318066666666539</v>
+      </c>
+      <c r="V4" s="8">
+        <f>F4*N4</f>
+        <v>19.080841666666654</v>
+      </c>
+      <c r="W4" s="8">
+        <f>G4*N4</f>
+        <v>27.037950438400003</v>
+      </c>
+      <c r="X4" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="12"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="4"/>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="12"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="4"/>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="4"/>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="4"/>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+    </row>
+    <row r="18" spans="2:24">
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+    </row>
+    <row r="19" spans="2:24">
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+    </row>
+    <row r="20" spans="2:24">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+    </row>
+    <row r="21" spans="2:24">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+    </row>
+    <row r="22" spans="2:24">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+    </row>
+    <row r="23" spans="2:24">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="4"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+    </row>
+    <row r="24" spans="2:24">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+    </row>
+    <row r="26" spans="2:24">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+    </row>
+    <row r="27" spans="2:24">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="8"/>
+    </row>
+    <row r="28" spans="2:24">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="8"/>
+      <c r="X28" s="8"/>
+    </row>
+    <row r="29" spans="2:24">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BFF680-E330-4D55-9962-B9A4D02270CE}">
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4703,10 +6440,10 @@
     <col min="4" max="4" width="13.36328125" customWidth="1"/>
     <col min="5" max="5" width="13.7265625" customWidth="1"/>
     <col min="6" max="6" width="12.08984375" customWidth="1"/>
-    <col min="7" max="7" width="11.08984375" customWidth="1"/>
-    <col min="8" max="8" width="9.26953125" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" customWidth="1"/>
     <col min="9" max="9" width="10.81640625" customWidth="1"/>
-    <col min="10" max="10" width="13.90625" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" customWidth="1"/>
     <col min="11" max="11" width="12.36328125" customWidth="1"/>
     <col min="12" max="12" width="14.1796875" customWidth="1"/>
     <col min="13" max="13" width="12.453125" customWidth="1"/>
@@ -5118,19 +6855,19 @@
         <f t="shared" si="5"/>
         <v>49.490138977871972</v>
       </c>
-      <c r="U5" s="19">
+      <c r="U5" s="8">
         <f t="shared" si="6"/>
         <v>33.069300000000005</v>
       </c>
-      <c r="V5" s="19">
+      <c r="V5" s="8">
         <f t="shared" si="6"/>
         <v>32.650016026515495</v>
       </c>
-      <c r="W5" s="19">
+      <c r="W5" s="8">
         <f t="shared" si="7"/>
         <v>33.069300000000005</v>
       </c>
-      <c r="X5" s="21">
+      <c r="X5" s="4">
         <f t="shared" si="8"/>
         <v>8.2673250000000014</v>
       </c>
@@ -5145,10 +6882,10 @@
       <c r="H6" s="5"/>
       <c r="L6" s="7"/>
       <c r="M6" s="4"/>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
-      <c r="W6" s="19"/>
-      <c r="X6" s="21"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="4"/>
     </row>
     <row r="7" spans="1:24">
       <c r="B7" s="5"/>
@@ -5160,10 +6897,10 @@
       <c r="H7" s="5"/>
       <c r="L7" s="7"/>
       <c r="M7" s="4"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19"/>
-      <c r="W7" s="19"/>
-      <c r="X7" s="21"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="4"/>
     </row>
     <row r="8" spans="1:24">
       <c r="A8" t="s">
@@ -5234,19 +6971,19 @@
         <f>B8/4*P8</f>
         <v>49.490138977871972</v>
       </c>
-      <c r="U8" s="19">
+      <c r="U8" s="8">
         <f t="shared" si="6"/>
         <v>100.21000000000001</v>
       </c>
-      <c r="V8" s="19">
+      <c r="V8" s="8">
         <f t="shared" si="6"/>
         <v>100.41610701336801</v>
       </c>
-      <c r="W8" s="19">
+      <c r="W8" s="8">
         <f t="shared" si="7"/>
         <v>100.21000000000001</v>
       </c>
-      <c r="X8" s="21">
+      <c r="X8" s="4">
         <f t="shared" si="8"/>
         <v>25.052500000000002</v>
       </c>
@@ -5320,19 +7057,19 @@
         <f t="shared" ref="T9:T11" si="14">B9/4*P9</f>
         <v>49.490138977871972</v>
       </c>
-      <c r="U9" s="19">
+      <c r="U9" s="8">
         <f t="shared" si="6"/>
         <v>67.14070000000001</v>
       </c>
-      <c r="V9" s="19">
+      <c r="V9" s="8">
         <f t="shared" si="6"/>
         <v>68.494842662602153</v>
       </c>
-      <c r="W9" s="19">
+      <c r="W9" s="8">
         <f t="shared" si="7"/>
         <v>67.14070000000001</v>
       </c>
-      <c r="X9" s="21">
+      <c r="X9" s="4">
         <f t="shared" si="8"/>
         <v>16.785175000000002</v>
       </c>
@@ -5414,11 +7151,11 @@
         <f>F10*N10</f>
         <v>50.105000000000004</v>
       </c>
-      <c r="W10" s="19">
+      <c r="W10" s="8">
         <f t="shared" si="7"/>
         <v>50.105000000000004</v>
       </c>
-      <c r="X10" s="21">
+      <c r="X10" s="4">
         <f t="shared" si="8"/>
         <v>12.526250000000001</v>
       </c>
@@ -5501,10 +7238,10 @@
         <v>33.069300000000005</v>
       </c>
       <c r="W11" s="8">
-        <f t="shared" ref="W10:W15" si="16">G11*N11</f>
+        <f t="shared" ref="W11:W15" si="16">G11*N11</f>
         <v>33.069300000000005</v>
       </c>
-      <c r="X11" s="21">
+      <c r="X11" s="4">
         <f t="shared" si="8"/>
         <v>8.2673250000000014</v>
       </c>
@@ -5513,13 +7250,13 @@
       <c r="U12" s="8"/>
       <c r="V12" s="8"/>
       <c r="W12" s="8"/>
-      <c r="X12" s="21"/>
+      <c r="X12" s="4"/>
     </row>
     <row r="13" spans="1:24">
       <c r="U13" s="8"/>
       <c r="V13" s="8"/>
       <c r="W13" s="8"/>
-      <c r="X13" s="21"/>
+      <c r="X13" s="4"/>
     </row>
     <row r="14" spans="1:24">
       <c r="A14" t="s">
@@ -5595,14 +7332,14 @@
         <v>100.21000000000001</v>
       </c>
       <c r="V14" s="8">
-        <f t="shared" ref="V12:V14" si="17">F14*N14</f>
+        <f t="shared" ref="V14" si="17">F14*N14</f>
         <v>100.21000000000001</v>
       </c>
       <c r="W14" s="8">
         <f t="shared" si="16"/>
         <v>100.21000000000001</v>
       </c>
-      <c r="X14" s="21">
+      <c r="X14" s="4">
         <f t="shared" si="8"/>
         <v>25.052500000000002</v>
       </c>
@@ -5688,7 +7425,7 @@
         <f t="shared" si="16"/>
         <v>67.14070000000001</v>
       </c>
-      <c r="X15" s="21">
+      <c r="X15" s="4">
         <f t="shared" si="8"/>
         <v>16.785175000000002</v>
       </c>
@@ -5763,7 +7500,7 @@
         <v>49.490138977871972</v>
       </c>
       <c r="U16" s="8">
-        <f t="shared" ref="U16:U18" si="24">E16*N16</f>
+        <f t="shared" ref="U16:U17" si="24">E16*N16</f>
         <v>50.105000000000004</v>
       </c>
       <c r="V16" s="8">
@@ -5771,10 +7508,10 @@
         <v>50.105000000000004</v>
       </c>
       <c r="W16" s="8">
-        <f t="shared" ref="W16:W18" si="25">G16*N16</f>
+        <f t="shared" ref="W16:W17" si="25">G16*N16</f>
         <v>50.105000000000004</v>
       </c>
-      <c r="X16" s="21">
+      <c r="X16" s="4">
         <f t="shared" si="8"/>
         <v>12.526250000000001</v>
       </c>
@@ -5860,7 +7597,7 @@
         <f t="shared" si="25"/>
         <v>33.069300000000005</v>
       </c>
-      <c r="X17" s="21">
+      <c r="X17" s="4">
         <f t="shared" si="8"/>
         <v>8.2673250000000014</v>
       </c>
@@ -5875,10 +7612,90 @@
       <c r="V19" s="8"/>
     </row>
     <row r="20" spans="1:24">
-      <c r="U20" s="5"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="5"/>
-      <c r="X20" s="5"/>
+      <c r="A20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="5">
+        <v>40582</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20" s="18">
+        <f>12.8/328</f>
+        <v>3.9024390243902439E-2</v>
+      </c>
+      <c r="F20" s="21">
+        <f>4.8/256</f>
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="G20" s="20">
+        <v>2.5850689999999999E-2</v>
+      </c>
+      <c r="H20" s="17">
+        <v>7.0517210000000004E-4</v>
+      </c>
+      <c r="I20" s="19">
+        <f>E20/F20</f>
+        <v>2.0813008130081303</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M20" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N20" s="12">
+        <v>1002.1</v>
+      </c>
+      <c r="O20" s="8">
+        <v>1060.5001774294601</v>
+      </c>
+      <c r="P20" s="9">
+        <f>8*(N20/B20)^2</f>
+        <v>4.8780384385069212E-3</v>
+      </c>
+      <c r="Q20" s="9">
+        <f>8*(O20/B20)^2</f>
+        <v>5.4631683657940158E-3</v>
+      </c>
+      <c r="R20" s="10">
+        <f>(Q20-P20)/P20</f>
+        <v>0.11995188940458455</v>
+      </c>
+      <c r="S20" s="8">
+        <f>200*O20/B20</f>
+        <v>5.2264559530307038</v>
+      </c>
+      <c r="T20" s="4">
+        <f>B20/4*P20</f>
+        <v>49.490138977871972</v>
+      </c>
+      <c r="U20" s="8">
+        <f t="shared" ref="U20" si="26">E20*N20</f>
+        <v>39.106341463414637</v>
+      </c>
+      <c r="V20" s="8">
+        <f t="shared" ref="V20" si="27">F20*N20</f>
+        <v>18.789375</v>
+      </c>
+      <c r="W20" s="8">
+        <f t="shared" ref="W20" si="28">G20*N20</f>
+        <v>25.904976448999999</v>
+      </c>
+      <c r="X20" s="4">
+        <f t="shared" ref="X20" si="29">H20*N20</f>
+        <v>0.70665296141</v>
+      </c>
     </row>
     <row r="21" spans="1:24">
       <c r="U21" s="8"/>
@@ -5910,12 +7727,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42F51E-90FA-449F-904F-669D9897EDC7}">
   <dimension ref="A1:X87"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="W78" sqref="W78"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6172,19 +7989,19 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U3" s="8">
-        <f t="shared" ref="U3:U32" si="4">E3*N3</f>
+        <f t="shared" ref="U3:U30" si="4">E3*N3</f>
         <v>347.45509900000002</v>
       </c>
       <c r="V3" s="8">
-        <f t="shared" ref="V3:V32" si="5">F3*O3</f>
+        <f t="shared" ref="V3:V30" si="5">F3*O3</f>
         <v>334.86600000000004</v>
       </c>
       <c r="W3" s="8">
-        <f t="shared" ref="W3:W32" si="6">G3*N3</f>
+        <f t="shared" ref="W3:W30" si="6">G3*N3</f>
         <v>347.45509900000002</v>
       </c>
       <c r="X3" s="4">
-        <f t="shared" ref="X3:X32" si="7">H3*N3</f>
+        <f t="shared" ref="X3:X30" si="7">H3*N3</f>
         <v>86.863774750000005</v>
       </c>
     </row>
@@ -9668,19 +11485,19 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U63" s="8">
-        <f t="shared" ref="U61:U78" si="48">E63*N63</f>
+        <f t="shared" ref="U63:U78" si="48">E63*N63</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V63" s="8">
-        <f t="shared" ref="V61:V78" si="49">F63*O63</f>
+        <f t="shared" ref="V63:V78" si="49">F63*O63</f>
         <v>486.30764273383807</v>
       </c>
       <c r="W63" s="8">
-        <f t="shared" ref="W61:W78" si="50">G63*N63</f>
+        <f t="shared" ref="W63:W78" si="50">G63*N63</f>
         <v>518.58969999999999</v>
       </c>
       <c r="X63" s="4">
-        <f t="shared" ref="X61:X78" si="51">H63*N63</f>
+        <f t="shared" ref="X63:X78" si="51">H63*N63</f>
         <v>129.647425</v>
       </c>
     </row>
@@ -10853,7 +12670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9793D359-A47C-4A9C-AA50-6D07B64231AE}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -10894,7 +12711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94B158E-7148-4AB6-B7D0-A5EFE522960E}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -10929,7 +12746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B65B28-909F-4DCB-A7FC-99B4B3E29597}">
   <dimension ref="A1:A3"/>
   <sheetViews>

</xml_diff>

<commit_message>
damping function, Orlandi's toolkit
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDD73BE-779A-4D69-A6D7-1CA01A1ABF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8D56E8-5959-4493-83E0-C234737B59CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="176">
   <si>
     <t>nompi</t>
   </si>
@@ -591,6 +591,9 @@
   </si>
   <si>
     <t>NOSLIP+SMAG+SMALL+CS0.18</t>
+  </si>
+  <si>
+    <t>NOSLIP+SMAG+SMALL+CS0.18+NEWDAMP</t>
   </si>
 </sst>
 </file>
@@ -5583,12 +5586,12 @@
   <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.90625" customWidth="1"/>
     <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
@@ -5935,27 +5938,87 @@
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
+      <c r="A5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="5">
+        <v>13750</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.130833333333333</v>
+      </c>
+      <c r="F5" s="21">
+        <v>4.8645833333333298E-2</v>
+      </c>
+      <c r="G5" s="18">
+        <v>6.8932160000000006E-2</v>
+      </c>
+      <c r="H5" s="13">
+        <v>3.896123E-3</v>
+      </c>
+      <c r="I5" s="19">
+        <f>E5/F5</f>
+        <v>2.6895074946466759</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N5" s="12">
+        <v>392.24</v>
+      </c>
+      <c r="O5" s="12">
+        <v>352.74297174230901</v>
+      </c>
+      <c r="P5" s="9">
+        <f>8*(N5/B5)^2</f>
+        <v>6.5101103645619834E-3</v>
+      </c>
+      <c r="Q5" s="9">
+        <f>8*(O5/B5)^2</f>
+        <v>5.2650358104265162E-3</v>
+      </c>
+      <c r="R5" s="10">
+        <f>(Q5-P5)/P5</f>
+        <v>-0.19125244956108189</v>
+      </c>
+      <c r="S5" s="8">
+        <f>200*2*O5/B5</f>
+        <v>10.261613723412626</v>
+      </c>
+      <c r="T5" s="4">
+        <f>B5/4*P5</f>
+        <v>22.37850437818182</v>
+      </c>
+      <c r="U5" s="8">
+        <f>E5*N5</f>
+        <v>51.318066666666539</v>
+      </c>
+      <c r="V5" s="8">
+        <f>F5*N5</f>
+        <v>19.080841666666654</v>
+      </c>
+      <c r="W5" s="8">
+        <f>G5*N5</f>
+        <v>27.037950438400003</v>
+      </c>
+      <c r="X5" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="6" spans="1:24">
       <c r="B6" s="5"/>

</xml_diff>

<commit_message>
compute sgs once a physical time step
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B6895B-1AE2-4E9F-8DB3-C21C08214AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448B0750-D09E-4F53-8FC9-6A175C7FC1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="194">
   <si>
     <t>nompi</t>
   </si>
@@ -645,6 +645,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 384×256×512</t>
+  </si>
+  <si>
+    <t>NOSLIP+DSMAG+SMALL</t>
   </si>
 </sst>
 </file>
@@ -4570,10 +4573,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3643DFC1-43AF-4E64-819A-C97D29654F85}">
-  <dimension ref="A1:X33"/>
+  <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="V32" sqref="V32"/>
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6810,7 +6813,7 @@
         <v>2.6576520000000001E-4</v>
       </c>
       <c r="I32" s="19">
-        <f t="shared" ref="I32:I33" si="44">E32/F32</f>
+        <f t="shared" ref="I32:I34" si="44">E32/F32</f>
         <v>1.7777777777777779</v>
       </c>
       <c r="J32" s="5" t="s">
@@ -6832,15 +6835,15 @@
         <v>550.14047743079595</v>
       </c>
       <c r="P32" s="9">
-        <f t="shared" ref="P32:P33" si="45">8*(N32/B32)^2</f>
+        <f t="shared" ref="P32:P34" si="45">8*(N32/B32)^2</f>
         <v>5.772630931736967E-3</v>
       </c>
       <c r="Q32" s="9">
-        <f t="shared" ref="Q32:Q33" si="46">8*(O32/B32)^2</f>
+        <f t="shared" ref="Q32:Q34" si="46">8*(O32/B32)^2</f>
         <v>5.7390011065929555E-3</v>
       </c>
       <c r="R32" s="10">
-        <f t="shared" ref="R32:R33" si="47">(Q32-P32)/P32</f>
+        <f t="shared" ref="R32:R34" si="47">(Q32-P32)/P32</f>
         <v>-5.8257362269810769E-3</v>
       </c>
       <c r="S32" s="8">
@@ -6848,15 +6851,15 @@
         <v>10.71354386428035</v>
       </c>
       <c r="T32" s="4">
-        <f t="shared" ref="T32:T33" si="48">B32/4*P32</f>
+        <f t="shared" ref="T32:T34" si="48">B32/4*P32</f>
         <v>29.642459834469324</v>
       </c>
       <c r="U32" s="8">
-        <f t="shared" ref="U32:U33" si="49">E32*N32</f>
+        <f t="shared" ref="U32:U34" si="49">E32*N32</f>
         <v>9.1958333333333329</v>
       </c>
       <c r="V32" s="8">
-        <f t="shared" ref="V32:V33" si="50">F32*N32</f>
+        <f t="shared" ref="V32:V34" si="50">F32*N32</f>
         <v>5.1726562500000002</v>
       </c>
       <c r="W32" s="8">
@@ -6946,12 +6949,95 @@
         <v>10.3453125</v>
       </c>
       <c r="W33" s="8">
-        <f t="shared" ref="W33" si="51">G33*N33</f>
+        <f t="shared" ref="W33:W34" si="51">G33*N33</f>
         <v>10.92118501</v>
       </c>
       <c r="X33" s="8">
-        <f t="shared" ref="X33" si="52">H33*N33</f>
+        <f t="shared" ref="X33:X34" si="52">H33*N33</f>
         <v>0.29612416982499995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24">
+      <c r="A34" t="s">
+        <v>193</v>
+      </c>
+      <c r="B34" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E34" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F34" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G34" s="18">
+        <v>7.9024239999999996E-2</v>
+      </c>
+      <c r="H34" s="13">
+        <v>2.2765490000000001E-3</v>
+      </c>
+      <c r="I34" s="19">
+        <f t="shared" si="44"/>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M34" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N34" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O34" s="4">
+        <v>530.15400812668804</v>
+      </c>
+      <c r="P34" s="9">
+        <f t="shared" si="45"/>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q34" s="9">
+        <f t="shared" si="46"/>
+        <v>5.3295827142857055E-3</v>
+      </c>
+      <c r="R34" s="10">
+        <f t="shared" si="47"/>
+        <v>-7.6749790986195915E-2</v>
+      </c>
+      <c r="S34" s="8">
+        <v>11</v>
+      </c>
+      <c r="T34" s="4">
+        <f t="shared" si="48"/>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U34" s="8">
+        <f t="shared" si="49"/>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V34" s="8">
+        <f t="shared" si="50"/>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W34" s="8">
+        <f t="shared" si="51"/>
+        <v>43.60162442</v>
+      </c>
+      <c r="X34" s="8">
+        <f t="shared" si="52"/>
+        <v>1.25608591075</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alpha depends on 2d/3d filter
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448B0750-D09E-4F53-8FC9-6A175C7FC1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD04D5D5-2E5F-47B1-AD1D-A1F46E0CF417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="195">
   <si>
     <t>nompi</t>
   </si>
@@ -648,6 +648,9 @@
   </si>
   <si>
     <t>NOSLIP+DSMAG+SMALL</t>
+  </si>
+  <si>
+    <t>NOSLIP+DSMAG+SMALL+UPDATE1</t>
   </si>
 </sst>
 </file>
@@ -4573,10 +4576,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3643DFC1-43AF-4E64-819A-C97D29654F85}">
-  <dimension ref="A1:X34"/>
+  <dimension ref="A1:X37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+      <selection activeCell="T42" sqref="T42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6813,7 +6816,7 @@
         <v>2.6576520000000001E-4</v>
       </c>
       <c r="I32" s="19">
-        <f t="shared" ref="I32:I34" si="44">E32/F32</f>
+        <f t="shared" ref="I32:I35" si="44">E32/F32</f>
         <v>1.7777777777777779</v>
       </c>
       <c r="J32" s="5" t="s">
@@ -6835,15 +6838,15 @@
         <v>550.14047743079595</v>
       </c>
       <c r="P32" s="9">
-        <f t="shared" ref="P32:P34" si="45">8*(N32/B32)^2</f>
+        <f t="shared" ref="P32:P35" si="45">8*(N32/B32)^2</f>
         <v>5.772630931736967E-3</v>
       </c>
       <c r="Q32" s="9">
-        <f t="shared" ref="Q32:Q34" si="46">8*(O32/B32)^2</f>
+        <f t="shared" ref="Q32:Q35" si="46">8*(O32/B32)^2</f>
         <v>5.7390011065929555E-3</v>
       </c>
       <c r="R32" s="10">
-        <f t="shared" ref="R32:R34" si="47">(Q32-P32)/P32</f>
+        <f t="shared" ref="R32:R35" si="47">(Q32-P32)/P32</f>
         <v>-5.8257362269810769E-3</v>
       </c>
       <c r="S32" s="8">
@@ -6851,15 +6854,15 @@
         <v>10.71354386428035</v>
       </c>
       <c r="T32" s="4">
-        <f t="shared" ref="T32:T34" si="48">B32/4*P32</f>
+        <f t="shared" ref="T32:T35" si="48">B32/4*P32</f>
         <v>29.642459834469324</v>
       </c>
       <c r="U32" s="8">
-        <f t="shared" ref="U32:U34" si="49">E32*N32</f>
+        <f t="shared" ref="U32:U35" si="49">E32*N32</f>
         <v>9.1958333333333329</v>
       </c>
       <c r="V32" s="8">
-        <f t="shared" ref="V32:V34" si="50">F32*N32</f>
+        <f t="shared" ref="V32:V35" si="50">F32*N32</f>
         <v>5.1726562500000002</v>
       </c>
       <c r="W32" s="8">
@@ -6949,94 +6952,261 @@
         <v>10.3453125</v>
       </c>
       <c r="W33" s="8">
-        <f t="shared" ref="W33:W34" si="51">G33*N33</f>
+        <f t="shared" ref="W33:W35" si="51">G33*N33</f>
         <v>10.92118501</v>
       </c>
       <c r="X33" s="8">
-        <f t="shared" ref="X33:X34" si="52">H33*N33</f>
+        <f t="shared" ref="X33:X35" si="52">H33*N33</f>
         <v>0.29612416982499995</v>
       </c>
     </row>
-    <row r="34" spans="1:24">
-      <c r="A34" t="s">
+    <row r="35" spans="1:24">
+      <c r="A35" t="s">
         <v>193</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B35" s="5">
         <v>20540</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E34" s="18">
+      <c r="D35" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E35" s="18">
         <v>6.6666666666666596E-2</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F35" s="5">
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="G34" s="18">
-        <v>7.9024239999999996E-2</v>
-      </c>
-      <c r="H34" s="13">
-        <v>2.2765490000000001E-3</v>
-      </c>
-      <c r="I34" s="19">
+      <c r="G35" s="18">
+        <v>3.9572349999999999E-2</v>
+      </c>
+      <c r="H35" s="13">
+        <v>1.094476E-3</v>
+      </c>
+      <c r="I35" s="19">
         <f t="shared" si="44"/>
         <v>1.7777777777777759</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="J35" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="K35" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="L35" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="M34" s="19" t="s">
+      <c r="M35" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="N34" s="12">
+      <c r="N35" s="12">
         <v>551.75</v>
       </c>
-      <c r="O34" s="4">
-        <v>530.15400812668804</v>
-      </c>
-      <c r="P34" s="9">
+      <c r="O35" s="4">
+        <v>546.75185455158396</v>
+      </c>
+      <c r="P35" s="9">
         <f t="shared" si="45"/>
         <v>5.772630931736967E-3</v>
       </c>
-      <c r="Q34" s="9">
+      <c r="Q35" s="9">
         <f t="shared" si="46"/>
-        <v>5.3295827142857055E-3</v>
-      </c>
-      <c r="R34" s="10">
+        <v>5.6685194103053282E-3</v>
+      </c>
+      <c r="R35" s="10">
         <f t="shared" si="47"/>
-        <v>-7.6749790986195915E-2</v>
-      </c>
-      <c r="S34" s="8">
-        <v>11</v>
-      </c>
-      <c r="T34" s="4">
+        <v>-1.8035367696772529E-2</v>
+      </c>
+      <c r="S35" s="8">
+        <f>200*2*O35/B35</f>
+        <v>10.64755315582442</v>
+      </c>
+      <c r="T35" s="4">
         <f t="shared" si="48"/>
         <v>29.642459834469324</v>
       </c>
-      <c r="U34" s="8">
+      <c r="U35" s="8">
         <f t="shared" si="49"/>
         <v>36.783333333333296</v>
       </c>
-      <c r="V34" s="8">
+      <c r="V35" s="8">
         <f t="shared" si="50"/>
         <v>20.690625000000001</v>
       </c>
-      <c r="W34" s="8">
+      <c r="W35" s="8">
         <f t="shared" si="51"/>
+        <v>21.834044112499999</v>
+      </c>
+      <c r="X35" s="8">
+        <f t="shared" si="52"/>
+        <v>0.60387713300000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24">
+      <c r="A36" t="s">
+        <v>193</v>
+      </c>
+      <c r="B36" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E36" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F36" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G36" s="18">
+        <v>7.9024239999999996E-2</v>
+      </c>
+      <c r="H36" s="13">
+        <v>2.2765490000000001E-3</v>
+      </c>
+      <c r="I36" s="19">
+        <f>E36/F36</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L36" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M36" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N36" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O36" s="4">
+        <v>530.15400812668804</v>
+      </c>
+      <c r="P36" s="9">
+        <f>8*(N36/B36)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q36" s="9">
+        <f>8*(O36/B36)^2</f>
+        <v>5.3295827142857055E-3</v>
+      </c>
+      <c r="R36" s="10">
+        <f>(Q36-P36)/P36</f>
+        <v>-7.6749790986195915E-2</v>
+      </c>
+      <c r="S36" s="8">
+        <v>11</v>
+      </c>
+      <c r="T36" s="4">
+        <f>B36/4*P36</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U36" s="8">
+        <f>E36*N36</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V36" s="8">
+        <f>F36*N36</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W36" s="8">
+        <f>G36*N36</f>
         <v>43.60162442</v>
       </c>
-      <c r="X34" s="8">
-        <f t="shared" si="52"/>
+      <c r="X36" s="8">
+        <f>H36*N36</f>
+        <v>1.25608591075</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24">
+      <c r="A37" t="s">
+        <v>194</v>
+      </c>
+      <c r="B37" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E37" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F37" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G37" s="18">
+        <v>7.9024239999999996E-2</v>
+      </c>
+      <c r="H37" s="13">
+        <v>2.2765490000000001E-3</v>
+      </c>
+      <c r="I37" s="19">
+        <f>E37/F37</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M37" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N37" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O37" s="4">
+        <v>530.10940935888505</v>
+      </c>
+      <c r="P37" s="9">
+        <f>8*(N37/B37)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q37" s="9">
+        <f>8*(O37/B37)^2</f>
+        <v>5.3286860585197897E-3</v>
+      </c>
+      <c r="R37" s="10">
+        <f>(Q37-P37)/P37</f>
+        <v>-7.6905119774147018E-2</v>
+      </c>
+      <c r="S37" s="8">
+        <v>11</v>
+      </c>
+      <c r="T37" s="4">
+        <f>B37/4*P37</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U37" s="8">
+        <f>E37*N37</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V37" s="8">
+        <f>F37*N37</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W37" s="8">
+        <f>G37*N37</f>
+        <v>43.60162442</v>
+      </c>
+      <c r="X37" s="8">
+        <f>H37*N37</f>
         <v>1.25608591075</v>
       </c>
     </row>

</xml_diff>

<commit_message>
strain rate computation modified
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FF3898-6870-4234-8925-5CDDA300E0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5C71CD-B9BC-4376-8D37-79FA3664B837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="200">
   <si>
     <t>nompi</t>
   </si>
@@ -663,6 +663,9 @@
   </si>
   <si>
     <t>NOSLIP+DSMAG+SMALL+FILTER2D</t>
+  </si>
+  <si>
+    <t>NOSLIP+SMAG+SMALL+TEST</t>
   </si>
 </sst>
 </file>
@@ -4588,10 +4591,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3643DFC1-43AF-4E64-819A-C97D29654F85}">
-  <dimension ref="A1:X40"/>
+  <dimension ref="A1:X43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6972,259 +6975,92 @@
         <v>0.29612416982499995</v>
       </c>
     </row>
-    <row r="35" spans="1:24">
-      <c r="A35" t="s">
-        <v>193</v>
-      </c>
-      <c r="B35" s="5">
+    <row r="34" spans="1:24">
+      <c r="A34" t="s">
+        <v>199</v>
+      </c>
+      <c r="B34" s="5">
         <v>20540</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="E35" s="18">
+      <c r="D34" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E34" s="18">
         <v>6.6666666666666596E-2</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F34" s="5">
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="G35" s="18">
-        <v>3.9572349999999999E-2</v>
-      </c>
-      <c r="H35" s="13">
-        <v>1.094476E-3</v>
-      </c>
-      <c r="I35" s="19">
+      <c r="G34" s="18">
+        <v>7.9024239999999996E-2</v>
+      </c>
+      <c r="H34" s="13">
+        <v>2.2765490000000001E-3</v>
+      </c>
+      <c r="I34" s="19">
         <f t="shared" si="44"/>
         <v>1.7777777777777759</v>
       </c>
-      <c r="J35" s="5" t="s">
+      <c r="J34" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L35" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="M35" s="19" t="s">
+      <c r="M34" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="N35" s="12">
+      <c r="N34" s="12">
         <v>551.75</v>
       </c>
-      <c r="O35" s="4">
-        <v>549.52612835823697</v>
-      </c>
-      <c r="P35" s="9">
+      <c r="O34" s="4">
+        <v>559.65770138097696</v>
+      </c>
+      <c r="P34" s="9">
         <f t="shared" si="45"/>
         <v>5.772630931736967E-3</v>
       </c>
-      <c r="Q35" s="9">
+      <c r="Q34" s="9">
         <f t="shared" si="46"/>
-        <v>5.7261906280834897E-3</v>
-      </c>
-      <c r="R35" s="10">
+        <v>5.9392837916666516E-3</v>
+      </c>
+      <c r="R34" s="10">
         <f t="shared" si="47"/>
-        <v>-8.0449112722859699E-3</v>
-      </c>
-      <c r="S35" s="8">
-        <f>200*2*O35/B35</f>
-        <v>10.701579909605394</v>
-      </c>
-      <c r="T35" s="4">
+        <v>2.8869481160393392E-2</v>
+      </c>
+      <c r="S34" s="8">
+        <v>11</v>
+      </c>
+      <c r="T34" s="4">
         <f t="shared" si="48"/>
         <v>29.642459834469324</v>
       </c>
-      <c r="U35" s="8">
+      <c r="U34" s="8">
         <f t="shared" si="49"/>
         <v>36.783333333333296</v>
       </c>
-      <c r="V35" s="8">
+      <c r="V34" s="8">
         <f t="shared" si="50"/>
         <v>20.690625000000001</v>
       </c>
-      <c r="W35" s="8">
+      <c r="W34" s="8">
         <f t="shared" si="51"/>
-        <v>21.834044112499999</v>
-      </c>
-      <c r="X35" s="8">
+        <v>43.60162442</v>
+      </c>
+      <c r="X34" s="8">
         <f t="shared" si="52"/>
-        <v>0.60387713300000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24">
-      <c r="A36" t="s">
-        <v>193</v>
-      </c>
-      <c r="B36" s="5">
-        <v>20540</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E36" s="18">
-        <v>6.6666666666666596E-2</v>
-      </c>
-      <c r="F36" s="5">
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="G36" s="18">
-        <v>7.9024239999999996E-2</v>
-      </c>
-      <c r="H36" s="13">
-        <v>2.2765490000000001E-3</v>
-      </c>
-      <c r="I36" s="19">
-        <f>E36/F36</f>
-        <v>1.7777777777777759</v>
-      </c>
-      <c r="J36" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="M36" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="N36" s="12">
-        <v>551.75</v>
-      </c>
-      <c r="O36" s="4">
-        <v>529.85379316914896</v>
-      </c>
-      <c r="P36" s="9">
-        <f>8*(N36/B36)^2</f>
-        <v>5.772630931736967E-3</v>
-      </c>
-      <c r="Q36" s="9">
-        <f>8*(O36/B36)^2</f>
-        <v>5.3235483642857136E-3</v>
-      </c>
-      <c r="R36" s="10">
-        <f>(Q36-P36)/P36</f>
-        <v>-7.7795128904269983E-2</v>
-      </c>
-      <c r="S36" s="8">
-        <v>11</v>
-      </c>
-      <c r="T36" s="4">
-        <f>B36/4*P36</f>
-        <v>29.642459834469324</v>
-      </c>
-      <c r="U36" s="8">
-        <f>E36*N36</f>
-        <v>36.783333333333296</v>
-      </c>
-      <c r="V36" s="8">
-        <f>F36*N36</f>
-        <v>20.690625000000001</v>
-      </c>
-      <c r="W36" s="8">
-        <f>G36*N36</f>
-        <v>43.60162442</v>
-      </c>
-      <c r="X36" s="8">
-        <f>H36*N36</f>
-        <v>1.25608591075</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24">
-      <c r="A37" t="s">
-        <v>196</v>
-      </c>
-      <c r="B37" s="5">
-        <v>20540</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E37" s="18">
-        <v>6.6666666666666596E-2</v>
-      </c>
-      <c r="F37" s="5">
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="G37" s="18">
-        <v>7.9024239999999996E-2</v>
-      </c>
-      <c r="H37" s="13">
-        <v>2.2765490000000001E-3</v>
-      </c>
-      <c r="I37" s="19">
-        <f>E37/F37</f>
-        <v>1.7777777777777759</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="M37" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="N37" s="12">
-        <v>551.75</v>
-      </c>
-      <c r="O37" s="4">
-        <v>500.92975237128002</v>
-      </c>
-      <c r="P37" s="9">
-        <f>8*(N37/B37)^2</f>
-        <v>5.772630931736967E-3</v>
-      </c>
-      <c r="Q37" s="9">
-        <f>8*(O37/B37)^2</f>
-        <v>4.7582007664670623E-3</v>
-      </c>
-      <c r="R37" s="10">
-        <f>(Q37-P37)/P37</f>
-        <v>-0.17573099289835697</v>
-      </c>
-      <c r="S37" s="8">
-        <v>11</v>
-      </c>
-      <c r="T37" s="4">
-        <f>B37/4*P37</f>
-        <v>29.642459834469324</v>
-      </c>
-      <c r="U37" s="8">
-        <f>E37*N37</f>
-        <v>36.783333333333296</v>
-      </c>
-      <c r="V37" s="8">
-        <f>F37*N37</f>
-        <v>20.690625000000001</v>
-      </c>
-      <c r="W37" s="8">
-        <f>G37*N37</f>
-        <v>43.60162442</v>
-      </c>
-      <c r="X37" s="8">
-        <f>H37*N37</f>
         <v>1.25608591075</v>
       </c>
     </row>
     <row r="38" spans="1:24">
       <c r="A38" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B38" s="5">
         <v>20540</v>
@@ -7233,7 +7069,7 @@
         <v>158</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E38" s="18">
         <v>6.6666666666666596E-2</v>
@@ -7242,10 +7078,10 @@
         <v>3.7499999999999999E-2</v>
       </c>
       <c r="G38" s="18">
-        <v>7.9024239999999996E-2</v>
+        <v>3.9572349999999999E-2</v>
       </c>
       <c r="H38" s="13">
-        <v>2.2765490000000001E-3</v>
+        <v>1.094476E-3</v>
       </c>
       <c r="I38" s="19">
         <f>E38/F38</f>
@@ -7267,7 +7103,7 @@
         <v>551.75</v>
       </c>
       <c r="O38" s="4">
-        <v>530.15400812668804</v>
+        <v>549.52612835823697</v>
       </c>
       <c r="P38" s="9">
         <f>8*(N38/B38)^2</f>
@@ -7275,14 +7111,15 @@
       </c>
       <c r="Q38" s="9">
         <f>8*(O38/B38)^2</f>
-        <v>5.3295827142857055E-3</v>
+        <v>5.7261906280834897E-3</v>
       </c>
       <c r="R38" s="10">
         <f>(Q38-P38)/P38</f>
-        <v>-7.6749790986195915E-2</v>
+        <v>-8.0449112722859699E-3</v>
       </c>
       <c r="S38" s="8">
-        <v>11</v>
+        <f>200*2*O38/B38</f>
+        <v>10.701579909605394</v>
       </c>
       <c r="T38" s="4">
         <f>B38/4*P38</f>
@@ -7298,16 +7135,16 @@
       </c>
       <c r="W38" s="8">
         <f>G38*N38</f>
-        <v>43.60162442</v>
+        <v>21.834044112499999</v>
       </c>
       <c r="X38" s="8">
         <f>H38*N38</f>
-        <v>1.25608591075</v>
+        <v>0.60387713300000001</v>
       </c>
     </row>
     <row r="39" spans="1:24">
       <c r="A39" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B39" s="5">
         <v>20540</v>
@@ -7350,7 +7187,7 @@
         <v>551.75</v>
       </c>
       <c r="O39" s="4">
-        <v>513.70343622884798</v>
+        <v>529.92020309073598</v>
       </c>
       <c r="P39" s="9">
         <f>8*(N39/B39)^2</f>
@@ -7358,11 +7195,11 @@
       </c>
       <c r="Q39" s="9">
         <f>8*(O39/B39)^2</f>
-        <v>5.0039625419103125E-3</v>
+        <v>5.3248829157769781E-3</v>
       </c>
       <c r="R39" s="10">
         <f>(Q39-P39)/P39</f>
-        <v>-0.13315737640538275</v>
+        <v>-7.7563942897915863E-2</v>
       </c>
       <c r="S39" s="8">
         <v>11</v>
@@ -7390,7 +7227,7 @@
     </row>
     <row r="40" spans="1:24">
       <c r="A40" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B40" s="5">
         <v>20540</v>
@@ -7433,7 +7270,7 @@
         <v>551.75</v>
       </c>
       <c r="O40" s="4">
-        <v>532.50976369392004</v>
+        <v>500.92975237128002</v>
       </c>
       <c r="P40" s="9">
         <f>8*(N40/B40)^2</f>
@@ -7441,11 +7278,11 @@
       </c>
       <c r="Q40" s="9">
         <f>8*(O40/B40)^2</f>
-        <v>5.3770522746478871E-3</v>
+        <v>4.7582007664670623E-3</v>
       </c>
       <c r="R40" s="10">
         <f>(Q40-P40)/P40</f>
-        <v>-6.852658030054444E-2</v>
+        <v>-0.17573099289835697</v>
       </c>
       <c r="S40" s="8">
         <v>11</v>
@@ -7468,6 +7305,255 @@
       </c>
       <c r="X40" s="8">
         <f>H40*N40</f>
+        <v>1.25608591075</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24">
+      <c r="A41" t="s">
+        <v>197</v>
+      </c>
+      <c r="B41" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E41" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F41" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G41" s="18">
+        <v>7.9024239999999996E-2</v>
+      </c>
+      <c r="H41" s="13">
+        <v>2.2765490000000001E-3</v>
+      </c>
+      <c r="I41" s="19">
+        <f>E41/F41</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M41" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N41" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O41" s="4">
+        <v>528.25196296092702</v>
+      </c>
+      <c r="P41" s="9">
+        <f>8*(N41/B41)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q41" s="9">
+        <f>8*(O41/B41)^2</f>
+        <v>5.2914091936805113E-3</v>
+      </c>
+      <c r="R41" s="10">
+        <f>(Q41-P41)/P41</f>
+        <v>-8.3362637200791498E-2</v>
+      </c>
+      <c r="S41" s="8">
+        <v>11</v>
+      </c>
+      <c r="T41" s="4">
+        <f>B41/4*P41</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U41" s="8">
+        <f>E41*N41</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V41" s="8">
+        <f>F41*N41</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W41" s="8">
+        <f>G41*N41</f>
+        <v>43.60162442</v>
+      </c>
+      <c r="X41" s="8">
+        <f>H41*N41</f>
+        <v>1.25608591075</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24">
+      <c r="A42" t="s">
+        <v>198</v>
+      </c>
+      <c r="B42" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E42" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F42" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G42" s="18">
+        <v>7.9024239999999996E-2</v>
+      </c>
+      <c r="H42" s="13">
+        <v>2.2765490000000001E-3</v>
+      </c>
+      <c r="I42" s="19">
+        <f>E42/F42</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M42" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N42" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O42" s="4">
+        <v>513.70343622884798</v>
+      </c>
+      <c r="P42" s="9">
+        <f>8*(N42/B42)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q42" s="9">
+        <f>8*(O42/B42)^2</f>
+        <v>5.0039625419103125E-3</v>
+      </c>
+      <c r="R42" s="10">
+        <f>(Q42-P42)/P42</f>
+        <v>-0.13315737640538275</v>
+      </c>
+      <c r="S42" s="8">
+        <v>11</v>
+      </c>
+      <c r="T42" s="4">
+        <f>B42/4*P42</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U42" s="8">
+        <f>E42*N42</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V42" s="8">
+        <f>F42*N42</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W42" s="8">
+        <f>G42*N42</f>
+        <v>43.60162442</v>
+      </c>
+      <c r="X42" s="8">
+        <f>H42*N42</f>
+        <v>1.25608591075</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24">
+      <c r="A43" t="s">
+        <v>195</v>
+      </c>
+      <c r="B43" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F43" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G43" s="18">
+        <v>7.9024239999999996E-2</v>
+      </c>
+      <c r="H43" s="13">
+        <v>2.2765490000000001E-3</v>
+      </c>
+      <c r="I43" s="19">
+        <f>E43/F43</f>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L43" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M43" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N43" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O43" s="4">
+        <v>530.67093902860302</v>
+      </c>
+      <c r="P43" s="9">
+        <f>8*(N43/B43)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q43" s="9">
+        <f>8*(O43/B43)^2</f>
+        <v>5.3399810857480785E-3</v>
+      </c>
+      <c r="R43" s="10">
+        <f>(Q43-P43)/P43</f>
+        <v>-7.4948468229668289E-2</v>
+      </c>
+      <c r="S43" s="8">
+        <v>11</v>
+      </c>
+      <c r="T43" s="4">
+        <f>B43/4*P43</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U43" s="8">
+        <f>E43*N43</f>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V43" s="8">
+        <f>F43*N43</f>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W43" s="8">
+        <f>G43*N43</f>
+        <v>43.60162442</v>
+      </c>
+      <c r="X43" s="8">
+        <f>H43*N43</f>
         <v>1.25608591075</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bug fixed. filter and strain_rate optimized
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5C71CD-B9BC-4376-8D37-79FA3664B837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4DFD1D-3FD6-4A33-A1A1-6072DD6B6BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="14120" windowHeight="15370" activeTab="3" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="200">
   <si>
     <t>nompi</t>
   </si>
@@ -665,7 +665,7 @@
     <t>NOSLIP+DSMAG+SMALL+FILTER2D</t>
   </si>
   <si>
-    <t>NOSLIP+SMAG+SMALL+TEST</t>
+    <t>NOSLIP+SMAG+SMALL+NEWS</t>
   </si>
 </sst>
 </file>
@@ -4593,13 +4593,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3643DFC1-43AF-4E64-819A-C97D29654F85}">
   <dimension ref="A1:X43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="29.81640625" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" customWidth="1"/>
     <col min="3" max="3" width="16.81640625" customWidth="1"/>
     <col min="4" max="4" width="14.7265625" customWidth="1"/>
     <col min="7" max="7" width="12.26953125" customWidth="1"/>
@@ -7001,7 +7001,7 @@
         <v>2.2765490000000001E-3</v>
       </c>
       <c r="I34" s="19">
-        <f t="shared" si="44"/>
+        <f t="shared" ref="I34:I35" si="53">E34/F34</f>
         <v>1.7777777777777759</v>
       </c>
       <c r="J34" s="5" t="s">
@@ -7023,39 +7023,123 @@
         <v>559.65770138097696</v>
       </c>
       <c r="P34" s="9">
-        <f t="shared" si="45"/>
+        <f t="shared" ref="P34:P35" si="54">8*(N34/B34)^2</f>
         <v>5.772630931736967E-3</v>
       </c>
       <c r="Q34" s="9">
-        <f t="shared" si="46"/>
+        <f t="shared" ref="Q34:Q35" si="55">8*(O34/B34)^2</f>
         <v>5.9392837916666516E-3</v>
       </c>
       <c r="R34" s="10">
-        <f t="shared" si="47"/>
+        <f t="shared" ref="R34:R35" si="56">(Q34-P34)/P34</f>
         <v>2.8869481160393392E-2</v>
       </c>
       <c r="S34" s="8">
         <v>11</v>
       </c>
       <c r="T34" s="4">
-        <f t="shared" si="48"/>
+        <f t="shared" ref="T34:T35" si="57">B34/4*P34</f>
         <v>29.642459834469324</v>
       </c>
       <c r="U34" s="8">
-        <f t="shared" si="49"/>
+        <f t="shared" ref="U34:U35" si="58">E34*N34</f>
         <v>36.783333333333296</v>
       </c>
       <c r="V34" s="8">
-        <f t="shared" si="50"/>
+        <f t="shared" ref="V34:V35" si="59">F34*N34</f>
         <v>20.690625000000001</v>
       </c>
       <c r="W34" s="8">
-        <f t="shared" si="51"/>
+        <f t="shared" ref="W34:W35" si="60">G34*N34</f>
         <v>43.60162442</v>
       </c>
       <c r="X34" s="8">
-        <f t="shared" si="52"/>
+        <f t="shared" ref="X34:X35" si="61">H34*N34</f>
         <v>1.25608591075</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24">
+      <c r="A35" t="s">
+        <v>199</v>
+      </c>
+      <c r="B35" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E35" s="18">
+        <v>6.6666666666666596E-2</v>
+      </c>
+      <c r="F35" s="5">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="G35" s="18">
+        <v>3.9572349999999999E-2</v>
+      </c>
+      <c r="H35" s="13">
+        <v>1.094476E-3</v>
+      </c>
+      <c r="I35" s="19">
+        <f t="shared" si="53"/>
+        <v>1.7777777777777759</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M35" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N35" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O35" s="4">
+        <v>581.40691547732297</v>
+      </c>
+      <c r="P35" s="9">
+        <f t="shared" si="54"/>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q35" s="9">
+        <f t="shared" si="55"/>
+        <v>6.4098740314309163E-3</v>
+      </c>
+      <c r="R35" s="10">
+        <f t="shared" si="56"/>
+        <v>0.11039041075543085</v>
+      </c>
+      <c r="S35" s="8">
+        <f>200*2*O35/B35</f>
+        <v>11.322432628574937</v>
+      </c>
+      <c r="T35" s="4">
+        <f t="shared" si="57"/>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U35" s="8">
+        <f t="shared" si="58"/>
+        <v>36.783333333333296</v>
+      </c>
+      <c r="V35" s="8">
+        <f t="shared" si="59"/>
+        <v>20.690625000000001</v>
+      </c>
+      <c r="W35" s="8">
+        <f t="shared" si="60"/>
+        <v>21.834044112499999</v>
+      </c>
+      <c r="X35" s="8">
+        <f t="shared" si="61"/>
+        <v>0.60387713300000001</v>
       </c>
     </row>
     <row r="38" spans="1:24">

</xml_diff>

<commit_message>
restore the bug temporarily for test purpose
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4DFD1D-3FD6-4A33-A1A1-6072DD6B6BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DCE508-C6E7-47DB-AED1-1A015F0A0D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="14120" windowHeight="15370" activeTab="3" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="notes" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="198">
   <si>
     <t>nompi</t>
   </si>
@@ -653,19 +654,13 @@
     <t xml:space="preserve"> 384×256×256</t>
   </si>
   <si>
-    <t>NOSLIP+DSMAG+SMALL+UPDT1</t>
-  </si>
-  <si>
-    <t>NOSLIP+DSMAG+SMALL+ALPH2.52</t>
-  </si>
-  <si>
-    <t>NOSLIP+DSMAG+SMALL+ALPH4.00</t>
-  </si>
-  <si>
     <t>NOSLIP+DSMAG+SMALL+FILTER2D</t>
   </si>
   <si>
     <t>NOSLIP+SMAG+SMALL+NEWS</t>
+  </si>
+  <si>
+    <t>NOSLIP+DSMAG+SMALL+ALPH4</t>
   </si>
 </sst>
 </file>
@@ -4591,10 +4586,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3643DFC1-43AF-4E64-819A-C97D29654F85}">
-  <dimension ref="A1:X43"/>
+  <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6831,7 +6826,7 @@
         <v>2.6576520000000001E-4</v>
       </c>
       <c r="I32" s="19">
-        <f t="shared" ref="I32:I35" si="44">E32/F32</f>
+        <f t="shared" ref="I32:I33" si="44">E32/F32</f>
         <v>1.7777777777777779</v>
       </c>
       <c r="J32" s="5" t="s">
@@ -6853,15 +6848,15 @@
         <v>550.14047743079595</v>
       </c>
       <c r="P32" s="9">
-        <f t="shared" ref="P32:P35" si="45">8*(N32/B32)^2</f>
+        <f t="shared" ref="P32:P33" si="45">8*(N32/B32)^2</f>
         <v>5.772630931736967E-3</v>
       </c>
       <c r="Q32" s="9">
-        <f t="shared" ref="Q32:Q35" si="46">8*(O32/B32)^2</f>
+        <f t="shared" ref="Q32:Q33" si="46">8*(O32/B32)^2</f>
         <v>5.7390011065929555E-3</v>
       </c>
       <c r="R32" s="10">
-        <f t="shared" ref="R32:R35" si="47">(Q32-P32)/P32</f>
+        <f t="shared" ref="R32:R33" si="47">(Q32-P32)/P32</f>
         <v>-5.8257362269810769E-3</v>
       </c>
       <c r="S32" s="8">
@@ -6869,15 +6864,15 @@
         <v>10.71354386428035</v>
       </c>
       <c r="T32" s="4">
-        <f t="shared" ref="T32:T35" si="48">B32/4*P32</f>
+        <f t="shared" ref="T32:T33" si="48">B32/4*P32</f>
         <v>29.642459834469324</v>
       </c>
       <c r="U32" s="8">
-        <f t="shared" ref="U32:U35" si="49">E32*N32</f>
+        <f t="shared" ref="U32:U33" si="49">E32*N32</f>
         <v>9.1958333333333329</v>
       </c>
       <c r="V32" s="8">
-        <f t="shared" ref="V32:V35" si="50">F32*N32</f>
+        <f t="shared" ref="V32:V33" si="50">F32*N32</f>
         <v>5.1726562500000002</v>
       </c>
       <c r="W32" s="8">
@@ -6967,17 +6962,17 @@
         <v>5.1726562500000002</v>
       </c>
       <c r="W33" s="8">
-        <f t="shared" ref="W33:W35" si="51">G33*N33</f>
+        <f t="shared" ref="W33" si="51">G33*N33</f>
         <v>10.92118501</v>
       </c>
       <c r="X33" s="8">
-        <f t="shared" ref="X33:X35" si="52">H33*N33</f>
+        <f t="shared" ref="X33" si="52">H33*N33</f>
         <v>0.29612416982499995</v>
       </c>
     </row>
     <row r="34" spans="1:24">
       <c r="A34" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B34" s="5">
         <v>20540</v>
@@ -7060,7 +7055,7 @@
     </row>
     <row r="35" spans="1:24">
       <c r="A35" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B35" s="5">
         <v>20540</v>
@@ -7311,7 +7306,7 @@
     </row>
     <row r="40" spans="1:24">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B40" s="5">
         <v>20540</v>
@@ -7354,7 +7349,7 @@
         <v>551.75</v>
       </c>
       <c r="O40" s="4">
-        <v>500.92975237128002</v>
+        <v>528.25196296092702</v>
       </c>
       <c r="P40" s="9">
         <f>8*(N40/B40)^2</f>
@@ -7362,11 +7357,11 @@
       </c>
       <c r="Q40" s="9">
         <f>8*(O40/B40)^2</f>
-        <v>4.7582007664670623E-3</v>
+        <v>5.2914091936805113E-3</v>
       </c>
       <c r="R40" s="10">
         <f>(Q40-P40)/P40</f>
-        <v>-0.17573099289835697</v>
+        <v>-8.3362637200791498E-2</v>
       </c>
       <c r="S40" s="8">
         <v>11</v>
@@ -7394,7 +7389,7 @@
     </row>
     <row r="41" spans="1:24">
       <c r="A41" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B41" s="5">
         <v>20540</v>
@@ -7437,7 +7432,7 @@
         <v>551.75</v>
       </c>
       <c r="O41" s="4">
-        <v>528.25196296092702</v>
+        <v>513.70343622884798</v>
       </c>
       <c r="P41" s="9">
         <f>8*(N41/B41)^2</f>
@@ -7445,11 +7440,11 @@
       </c>
       <c r="Q41" s="9">
         <f>8*(O41/B41)^2</f>
-        <v>5.2914091936805113E-3</v>
+        <v>5.0039625419103125E-3</v>
       </c>
       <c r="R41" s="10">
         <f>(Q41-P41)/P41</f>
-        <v>-8.3362637200791498E-2</v>
+        <v>-0.13315737640538275</v>
       </c>
       <c r="S41" s="8">
         <v>11</v>
@@ -7476,170 +7471,29 @@
       </c>
     </row>
     <row r="42" spans="1:24">
-      <c r="A42" t="s">
-        <v>198</v>
-      </c>
-      <c r="B42" s="5">
-        <v>20540</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E42" s="18">
-        <v>6.6666666666666596E-2</v>
-      </c>
-      <c r="F42" s="5">
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="G42" s="18">
-        <v>7.9024239999999996E-2</v>
-      </c>
-      <c r="H42" s="13">
-        <v>2.2765490000000001E-3</v>
-      </c>
-      <c r="I42" s="19">
-        <f>E42/F42</f>
-        <v>1.7777777777777759</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="K42" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L42" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="M42" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="N42" s="12">
-        <v>551.75</v>
-      </c>
-      <c r="O42" s="4">
-        <v>513.70343622884798</v>
-      </c>
-      <c r="P42" s="9">
-        <f>8*(N42/B42)^2</f>
-        <v>5.772630931736967E-3</v>
-      </c>
-      <c r="Q42" s="9">
-        <f>8*(O42/B42)^2</f>
-        <v>5.0039625419103125E-3</v>
-      </c>
-      <c r="R42" s="10">
-        <f>(Q42-P42)/P42</f>
-        <v>-0.13315737640538275</v>
-      </c>
-      <c r="S42" s="8">
-        <v>11</v>
-      </c>
-      <c r="T42" s="4">
-        <f>B42/4*P42</f>
-        <v>29.642459834469324</v>
-      </c>
-      <c r="U42" s="8">
-        <f>E42*N42</f>
-        <v>36.783333333333296</v>
-      </c>
-      <c r="V42" s="8">
-        <f>F42*N42</f>
-        <v>20.690625000000001</v>
-      </c>
-      <c r="W42" s="8">
-        <f>G42*N42</f>
-        <v>43.60162442</v>
-      </c>
-      <c r="X42" s="8">
-        <f>H42*N42</f>
-        <v>1.25608591075</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24">
-      <c r="A43" t="s">
-        <v>195</v>
-      </c>
-      <c r="B43" s="5">
-        <v>20540</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E43" s="18">
-        <v>6.6666666666666596E-2</v>
-      </c>
-      <c r="F43" s="5">
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="G43" s="18">
-        <v>7.9024239999999996E-2</v>
-      </c>
-      <c r="H43" s="13">
-        <v>2.2765490000000001E-3</v>
-      </c>
-      <c r="I43" s="19">
-        <f>E43/F43</f>
-        <v>1.7777777777777759</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="K43" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L43" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="M43" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="N43" s="12">
-        <v>551.75</v>
-      </c>
-      <c r="O43" s="4">
-        <v>530.67093902860302</v>
-      </c>
-      <c r="P43" s="9">
-        <f>8*(N43/B43)^2</f>
-        <v>5.772630931736967E-3</v>
-      </c>
-      <c r="Q43" s="9">
-        <f>8*(O43/B43)^2</f>
-        <v>5.3399810857480785E-3</v>
-      </c>
-      <c r="R43" s="10">
-        <f>(Q43-P43)/P43</f>
-        <v>-7.4948468229668289E-2</v>
-      </c>
-      <c r="S43" s="8">
-        <v>11</v>
-      </c>
-      <c r="T43" s="4">
-        <f>B43/4*P43</f>
-        <v>29.642459834469324</v>
-      </c>
-      <c r="U43" s="8">
-        <f>E43*N43</f>
-        <v>36.783333333333296</v>
-      </c>
-      <c r="V43" s="8">
-        <f>F43*N43</f>
-        <v>20.690625000000001</v>
-      </c>
-      <c r="W43" s="8">
-        <f>G43*N43</f>
-        <v>43.60162442</v>
-      </c>
-      <c r="X43" s="8">
-        <f>H43*N43</f>
-        <v>1.25608591075</v>
-      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="8"/>
+      <c r="W42" s="8"/>
+      <c r="X42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add correc_1st_point and modify strain rate to use one-sided wall-normal derivative and average
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCE68F8-BBFA-46DC-93CE-699F04916750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C2A1CA-A6DE-4809-95A4-7F21FE694129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="203">
   <si>
     <t>nompi</t>
   </si>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:X59"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32:M33"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4364,7 +4364,7 @@
   <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5748,10 +5748,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3643DFC1-43AF-4E64-819A-C97D29654F85}">
-  <dimension ref="A1:X42"/>
+  <dimension ref="A1:X44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39:R41"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7700,7 +7700,7 @@
         <v>43.60162442</v>
       </c>
       <c r="X28" s="8">
-        <f t="shared" si="41"/>
+        <f>H28*N28</f>
         <v>1.25608591075</v>
       </c>
     </row>
@@ -7784,7 +7784,7 @@
         <v>17.879756694999998</v>
       </c>
       <c r="X29" s="8">
-        <f t="shared" si="41"/>
+        <f>H29*N29</f>
         <v>1.3024439457499999</v>
       </c>
     </row>
@@ -8657,6 +8657,92 @@
       <c r="W42" s="8"/>
       <c r="X42" s="8"/>
     </row>
+    <row r="44" spans="1:24">
+      <c r="A44" t="s">
+        <v>192</v>
+      </c>
+      <c r="B44" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E44" s="18">
+        <f>6.4/192</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F44" s="5">
+        <f>2.4/128</f>
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="G44" s="18">
+        <v>3.9572349999999999E-2</v>
+      </c>
+      <c r="H44" s="13">
+        <v>1.094476E-3</v>
+      </c>
+      <c r="I44" s="19">
+        <f t="shared" ref="I44" si="62">E44/F44</f>
+        <v>1.7777777777777779</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L44" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M44" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N44" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O44" s="4">
+        <v>549.31194168112302</v>
+      </c>
+      <c r="P44" s="9">
+        <f t="shared" ref="P44" si="63">8*(N44/B44)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q44" s="9">
+        <f t="shared" ref="Q44" si="64">8*(O44/B44)^2</f>
+        <v>5.721727747572799E-3</v>
+      </c>
+      <c r="R44" s="10">
+        <f t="shared" ref="R44" si="65">(Q44-P44)/P44</f>
+        <v>-8.8180215860173463E-3</v>
+      </c>
+      <c r="S44" s="8">
+        <f>200*2*O44/B44</f>
+        <v>10.69740879612703</v>
+      </c>
+      <c r="T44" s="4">
+        <f t="shared" ref="T44" si="66">B44/4*P44</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U44" s="8">
+        <f t="shared" ref="U44" si="67">E44*N44</f>
+        <v>18.391666666666666</v>
+      </c>
+      <c r="V44" s="8">
+        <f t="shared" ref="V44" si="68">F44*N44</f>
+        <v>10.3453125</v>
+      </c>
+      <c r="W44" s="8">
+        <f t="shared" ref="W44" si="69">G44*N44</f>
+        <v>21.834044112499999</v>
+      </c>
+      <c r="X44" s="8">
+        <f t="shared" ref="X44" si="70">H44*N44</f>
+        <v>0.60387713300000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -8669,8 +8755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BFF680-E330-4D55-9962-B9A4D02270CE}">
   <dimension ref="A1:X35"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:S31"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10634,7 +10720,7 @@
     </row>
     <row r="35" spans="1:24">
       <c r="A35" t="s">
-        <v>142</v>
+        <v>192</v>
       </c>
       <c r="B35" s="5">
         <v>40582</v>

</xml_diff>

<commit_message>
second-order approxiamation of strain rate at the first layer
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5257739-5797-49E0-8996-8737FE9E0D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B6E3D0-EB46-4AE6-88F5-F9E613B82C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="5" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="206">
   <si>
     <t>nompi</t>
   </si>
@@ -681,6 +681,9 @@
   </si>
   <si>
     <t>WM+SMAG+SMALL</t>
+  </si>
+  <si>
+    <t>WM+SMAG+SMALL+ONESIDE</t>
   </si>
 </sst>
 </file>
@@ -10820,8 +10823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42F51E-90FA-449F-904F-669D9897EDC7}">
   <dimension ref="A1:X103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S93" sqref="S93"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R92" sqref="R92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -16200,22 +16203,24 @@
       <c r="N89" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O89" s="16"/>
+      <c r="O89" s="16">
+        <v>5163.6548122326203</v>
+      </c>
       <c r="P89">
         <f>8*(N89/B89)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
       <c r="Q89" s="9">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>3.412906370546317E-3</v>
       </c>
       <c r="R89" s="10">
         <f t="shared" si="68"/>
-        <v>-1</v>
+        <v>-8.5595566832998744E-3</v>
       </c>
       <c r="S89" s="8">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>20.65461924893048</v>
       </c>
       <c r="T89" s="4">
         <f t="shared" si="70"/>
@@ -16227,7 +16232,7 @@
       </c>
       <c r="V89" s="8">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>170.40060880367648</v>
       </c>
       <c r="W89" s="8">
         <f t="shared" si="66"/>
@@ -16238,6 +16243,350 @@
         <v>42.783650250000001</v>
       </c>
     </row>
+    <row r="92" spans="1:24">
+      <c r="A92" t="s">
+        <v>205</v>
+      </c>
+      <c r="B92" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E92" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F92" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G92">
+        <f>F92</f>
+        <v>0.1</v>
+      </c>
+      <c r="H92" s="5">
+        <f>0.25*G92</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I92" s="5">
+        <v>1</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K92" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L92">
+        <v>0.1</v>
+      </c>
+      <c r="M92" s="8">
+        <f>L92/H92</f>
+        <v>4</v>
+      </c>
+      <c r="N92" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O92" s="16">
+        <v>5161.2796463928098</v>
+      </c>
+      <c r="P92">
+        <f>8*(N92/B92)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q92" s="9">
+        <f>8*(O92/B92)^2</f>
+        <v>3.4097673712983915E-3</v>
+      </c>
+      <c r="R92" s="10">
+        <f>(Q92-P92)/P92</f>
+        <v>-9.4714278183512142E-3</v>
+      </c>
+      <c r="S92" s="8">
+        <f>500*2*O92/B92</f>
+        <v>20.64511858557124</v>
+      </c>
+      <c r="T92" s="4">
+        <f>B92/4*P92</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U92" s="8">
+        <f t="shared" ref="U92:U95" si="72">E92*N92</f>
+        <v>518.58969999999999</v>
+      </c>
+      <c r="V92" s="8">
+        <f t="shared" ref="V92:V95" si="73">F92*O92</f>
+        <v>516.127964639281</v>
+      </c>
+      <c r="W92" s="8">
+        <f t="shared" ref="W92:W95" si="74">G92*N92</f>
+        <v>518.58969999999999</v>
+      </c>
+      <c r="X92" s="4">
+        <f t="shared" ref="X92:X95" si="75">H92*N92</f>
+        <v>129.647425</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24">
+      <c r="A93" t="s">
+        <v>205</v>
+      </c>
+      <c r="B93" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E93" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F93" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G93">
+        <f>F93</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H93" s="5">
+        <f>0.25*G93</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I93" s="5">
+        <v>1</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K93" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L93">
+        <v>0.1</v>
+      </c>
+      <c r="M93" s="8">
+        <f>L93/H93</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N93" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O93" s="16">
+        <v>5137.6418223186201</v>
+      </c>
+      <c r="P93">
+        <f>8*(N93/B93)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q93" s="9">
+        <f>8*(O93/B93)^2</f>
+        <v>3.3786065272879864E-3</v>
+      </c>
+      <c r="R93" s="10">
+        <f t="shared" ref="R93:R95" si="76">(Q93-P93)/P93</f>
+        <v>-1.8523572133360134E-2</v>
+      </c>
+      <c r="S93" s="8">
+        <f t="shared" ref="S93:S95" si="77">500*2*O93/B93</f>
+        <v>20.550567289274479</v>
+      </c>
+      <c r="T93" s="4">
+        <f t="shared" ref="T93:T95" si="78">B93/4*P93</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U93" s="8">
+        <f t="shared" si="72"/>
+        <v>347.45509900000002</v>
+      </c>
+      <c r="V93" s="8">
+        <f t="shared" si="73"/>
+        <v>344.22200209534759</v>
+      </c>
+      <c r="W93" s="8">
+        <f t="shared" si="74"/>
+        <v>347.45509900000002</v>
+      </c>
+      <c r="X93" s="4">
+        <f t="shared" si="75"/>
+        <v>86.863774750000005</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24">
+      <c r="A94" t="s">
+        <v>205</v>
+      </c>
+      <c r="B94" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E94" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F94" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G94">
+        <f>F94</f>
+        <v>0.05</v>
+      </c>
+      <c r="H94" s="5">
+        <f>0.25*G94</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I94" s="5">
+        <v>1</v>
+      </c>
+      <c r="J94" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K94" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L94">
+        <v>0.1</v>
+      </c>
+      <c r="M94" s="8">
+        <f>L94/H94</f>
+        <v>8</v>
+      </c>
+      <c r="N94" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O94" s="16">
+        <v>5175.4405682218103</v>
+      </c>
+      <c r="P94">
+        <f>8*(N94/B94)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q94" s="9">
+        <f t="shared" ref="Q94:Q95" si="79">8*(O94/B94)^2</f>
+        <v>3.4285036896251008E-3</v>
+      </c>
+      <c r="R94" s="10">
+        <f t="shared" si="76"/>
+        <v>-4.0285759697721007E-3</v>
+      </c>
+      <c r="S94" s="8">
+        <f t="shared" si="77"/>
+        <v>20.70176227288724</v>
+      </c>
+      <c r="T94" s="4">
+        <f t="shared" si="78"/>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U94" s="8">
+        <f t="shared" si="72"/>
+        <v>259.29485</v>
+      </c>
+      <c r="V94" s="8">
+        <f t="shared" si="73"/>
+        <v>258.7720284110905</v>
+      </c>
+      <c r="W94" s="8">
+        <f t="shared" si="74"/>
+        <v>259.29485</v>
+      </c>
+      <c r="X94" s="4">
+        <f t="shared" si="75"/>
+        <v>64.823712499999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24">
+      <c r="A95" t="s">
+        <v>205</v>
+      </c>
+      <c r="B95" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E95" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F95" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G95">
+        <f>F95</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H95" s="5">
+        <f>0.25*G95</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I95" s="5">
+        <v>1</v>
+      </c>
+      <c r="J95" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K95" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L95">
+        <v>0.1</v>
+      </c>
+      <c r="M95" s="8">
+        <f>L95/H95</f>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N95" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O95" s="16">
+        <v>5160.3492684698103</v>
+      </c>
+      <c r="P95">
+        <f>8*(N95/B95)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q95" s="9">
+        <f t="shared" si="79"/>
+        <v>3.4085381852924043E-3</v>
+      </c>
+      <c r="R95" s="10">
+        <f t="shared" si="76"/>
+        <v>-9.8285031630521037E-3</v>
+      </c>
+      <c r="S95" s="8">
+        <f t="shared" si="77"/>
+        <v>20.641397073879244</v>
+      </c>
+      <c r="T95" s="4">
+        <f t="shared" si="78"/>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U95" s="8">
+        <f t="shared" si="72"/>
+        <v>171.134601</v>
+      </c>
+      <c r="V95" s="8">
+        <f t="shared" si="73"/>
+        <v>170.29152585950374</v>
+      </c>
+      <c r="W95" s="8">
+        <f t="shared" si="74"/>
+        <v>171.134601</v>
+      </c>
+      <c r="X95" s="4">
+        <f t="shared" si="75"/>
+        <v>42.783650250000001</v>
+      </c>
+    </row>
     <row r="100" spans="1:15">
       <c r="A100" s="5">
         <v>250000</v>
@@ -16345,7 +16694,7 @@
         <v>48</v>
       </c>
       <c r="D102" s="5">
-        <f t="shared" ref="D102:D103" si="72">E102*2</f>
+        <f t="shared" ref="D102:D103" si="80">E102*2</f>
         <v>0.1</v>
       </c>
       <c r="E102" s="5">
@@ -16394,7 +16743,7 @@
         <v>49</v>
       </c>
       <c r="D103" s="5">
-        <f t="shared" si="72"/>
+        <f t="shared" si="80"/>
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="E103" s="5">

</xml_diff>

<commit_message>
remove 2nd-order strain rate, and add note about the numerics for wall model implementation
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B6E3D0-EB46-4AE6-88F5-F9E613B82C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC0D622-53F8-49AA-A118-2B4C0B26A6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="5" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="207">
   <si>
     <t>nompi</t>
   </si>
@@ -684,6 +684,9 @@
   </si>
   <si>
     <t>WM+SMAG+SMALL+ONESIDE</t>
+  </si>
+  <si>
+    <t>WM+SMAG+SMALL+ONESIDE+2ND</t>
   </si>
 </sst>
 </file>
@@ -10821,15 +10824,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42F51E-90FA-449F-904F-669D9897EDC7}">
-  <dimension ref="A1:X103"/>
+  <dimension ref="A1:X113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R92" sqref="R92"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R101" sqref="R101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.7265625" customWidth="1"/>
+    <col min="1" max="1" width="29.54296875" customWidth="1"/>
     <col min="2" max="2" width="12.6328125" customWidth="1"/>
     <col min="3" max="3" width="12.08984375" customWidth="1"/>
     <col min="4" max="4" width="12.81640625" customWidth="1"/>
@@ -16587,197 +16590,541 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="100" spans="1:15">
-      <c r="A100" s="5">
+    <row r="98" spans="1:24">
+      <c r="A98" t="s">
+        <v>206</v>
+      </c>
+      <c r="B98" s="5">
         <v>250000</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="C98" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="D98" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E98" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F98" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G98">
+        <f>F98</f>
+        <v>0.1</v>
+      </c>
+      <c r="H98" s="5">
+        <f>0.25*G98</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I98" s="5">
+        <v>1</v>
+      </c>
+      <c r="J98" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K98" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L98">
+        <v>0.1</v>
+      </c>
+      <c r="M98" s="8">
+        <f>L98/H98</f>
+        <v>4</v>
+      </c>
+      <c r="N98" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O98" s="16">
+        <v>5150.2287556594101</v>
+      </c>
+      <c r="P98">
+        <f>8*(N98/B98)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q98" s="9">
+        <f>8*(O98/B98)^2</f>
+        <v>3.3951815981594973E-3</v>
+      </c>
+      <c r="R98" s="10">
+        <f>(Q98-P98)/P98</f>
+        <v>-1.3708557061550242E-2</v>
+      </c>
+      <c r="S98" s="8">
+        <f>500*2*O98/B98</f>
+        <v>20.60091502263764</v>
+      </c>
+      <c r="T98" s="4">
+        <f>B98/4*P98</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U98" s="8">
+        <f t="shared" ref="U98:U101" si="80">E98*N98</f>
+        <v>518.58969999999999</v>
+      </c>
+      <c r="V98" s="8">
+        <f t="shared" ref="V98:V101" si="81">F98*O98</f>
+        <v>515.02287556594104</v>
+      </c>
+      <c r="W98" s="8">
+        <f t="shared" ref="W98:W101" si="82">G98*N98</f>
+        <v>518.58969999999999</v>
+      </c>
+      <c r="X98" s="4">
+        <f t="shared" ref="X98:X101" si="83">H98*N98</f>
+        <v>129.647425</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24">
+      <c r="A99" t="s">
+        <v>206</v>
+      </c>
+      <c r="B99" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E99" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F99" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G99">
+        <f>F99</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H99" s="5">
+        <f>0.25*G99</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I99" s="5">
+        <v>1</v>
+      </c>
+      <c r="J99" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K99" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L99">
+        <v>0.1</v>
+      </c>
+      <c r="M99" s="8">
+        <f>L99/H99</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N99" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O99" s="16">
+        <v>5138.61073565483</v>
+      </c>
+      <c r="P99">
+        <f>8*(N99/B99)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q99" s="9">
+        <f>8*(O99/B99)^2</f>
+        <v>3.3798809974511447E-3</v>
+      </c>
+      <c r="R99" s="10">
+        <f t="shared" ref="R99:R101" si="84">(Q99-P99)/P99</f>
+        <v>-1.8153341858524522E-2</v>
+      </c>
+      <c r="S99" s="8">
+        <f t="shared" ref="S99:S101" si="85">500*2*O99/B99</f>
+        <v>20.554442942619321</v>
+      </c>
+      <c r="T99" s="4">
+        <f t="shared" ref="T99:T101" si="86">B99/4*P99</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U99" s="8">
+        <f t="shared" si="80"/>
+        <v>347.45509900000002</v>
+      </c>
+      <c r="V99" s="8">
+        <f t="shared" si="81"/>
+        <v>344.28691928887361</v>
+      </c>
+      <c r="W99" s="8">
+        <f t="shared" si="82"/>
+        <v>347.45509900000002</v>
+      </c>
+      <c r="X99" s="4">
+        <f t="shared" si="83"/>
+        <v>86.863774750000005</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24">
+      <c r="A100" t="s">
+        <v>206</v>
+      </c>
+      <c r="B100" s="5">
+        <v>250000</v>
+      </c>
       <c r="C100" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E100" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F100" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G100">
+        <f>F100</f>
+        <v>0.05</v>
+      </c>
+      <c r="H100" s="5">
+        <f>0.25*G100</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I100" s="5">
+        <v>1</v>
+      </c>
+      <c r="J100" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K100" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L100">
+        <v>0.1</v>
+      </c>
+      <c r="M100" s="8">
+        <f>L100/H100</f>
+        <v>8</v>
+      </c>
+      <c r="N100" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O100" s="16">
+        <v>5163.2875780213199</v>
+      </c>
+      <c r="P100">
+        <f>8*(N100/B100)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q100" s="9">
+        <f t="shared" ref="Q100:Q101" si="87">8*(O100/B100)^2</f>
+        <v>3.4124209425087063E-3</v>
+      </c>
+      <c r="R100" s="10">
+        <f t="shared" si="84"/>
+        <v>-8.7005722684212698E-3</v>
+      </c>
+      <c r="S100" s="8">
+        <f t="shared" si="85"/>
+        <v>20.653150312085277</v>
+      </c>
+      <c r="T100" s="4">
+        <f t="shared" si="86"/>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U100" s="8">
+        <f t="shared" si="80"/>
+        <v>259.29485</v>
+      </c>
+      <c r="V100" s="8">
+        <f t="shared" si="81"/>
+        <v>258.16437890106602</v>
+      </c>
+      <c r="W100" s="8">
+        <f t="shared" si="82"/>
+        <v>259.29485</v>
+      </c>
+      <c r="X100" s="4">
+        <f t="shared" si="83"/>
+        <v>64.823712499999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24">
+      <c r="A101" t="s">
+        <v>206</v>
+      </c>
+      <c r="B101" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E101" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F101" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G101">
+        <f>F101</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H101" s="5">
+        <f>0.25*G101</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I101" s="5">
+        <v>1</v>
+      </c>
+      <c r="J101" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K101" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L101">
+        <v>0.1</v>
+      </c>
+      <c r="M101" s="8">
+        <f>L101/H101</f>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N101" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O101" s="16">
+        <v>5149.6803129002901</v>
+      </c>
+      <c r="P101">
+        <f>8*(N101/B101)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q101" s="9">
+        <f t="shared" si="87"/>
+        <v>3.394458537609322E-3</v>
+      </c>
+      <c r="R101" s="10">
+        <f t="shared" si="84"/>
+        <v>-1.391860427485715E-2</v>
+      </c>
+      <c r="S101" s="8">
+        <f t="shared" si="85"/>
+        <v>20.598721251601159</v>
+      </c>
+      <c r="T101" s="4">
+        <f t="shared" si="86"/>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U101" s="8">
+        <f t="shared" si="80"/>
+        <v>171.134601</v>
+      </c>
+      <c r="V101" s="8">
+        <f t="shared" si="81"/>
+        <v>169.93945032570957</v>
+      </c>
+      <c r="W101" s="8">
+        <f t="shared" si="82"/>
+        <v>171.134601</v>
+      </c>
+      <c r="X101" s="4">
+        <f t="shared" si="83"/>
+        <v>42.783650250000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:24">
+      <c r="A110" s="5">
+        <v>250000</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C110" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D100" s="5">
+      <c r="D110" s="5">
         <v>0.2</v>
       </c>
-      <c r="E100" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F100">
-        <v>0.1</v>
-      </c>
-      <c r="G100" s="5">
-        <f>0.25*F100</f>
+      <c r="E110" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F110">
+        <v>0.1</v>
+      </c>
+      <c r="G110" s="5">
+        <f>0.25*F110</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H100" s="5">
+      <c r="H110" s="5">
         <v>2</v>
       </c>
-      <c r="I100" s="5" t="s">
+      <c r="I110" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J100" s="5" t="s">
+      <c r="J110" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K100">
-        <v>0.1</v>
-      </c>
-      <c r="L100" s="8">
-        <f>K100/G100</f>
+      <c r="K110">
+        <v>0.1</v>
+      </c>
+      <c r="L110" s="8">
+        <f>K110/G110</f>
         <v>4</v>
       </c>
-      <c r="M100" s="8">
+      <c r="M110" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O100">
-        <f>8*(M100/A100)^2</f>
+      <c r="O110">
+        <f>8*(M110/A110)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:15">
-      <c r="A101" s="5">
+    <row r="111" spans="1:24">
+      <c r="A111" s="5">
         <v>250000</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B111" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C101" s="5" t="s">
+      <c r="C111" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D101" s="5">
-        <f>E101*2</f>
+      <c r="D111" s="5">
+        <f>E111*2</f>
         <v>0.13400000000000001</v>
       </c>
-      <c r="E101" s="5">
+      <c r="E111" s="5">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="F101">
-        <f>E101</f>
+      <c r="F111">
+        <f>E111</f>
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="G101" s="5">
-        <f>0.25*F101</f>
+      <c r="G111" s="5">
+        <f>0.25*F111</f>
         <v>1.6750000000000001E-2</v>
       </c>
-      <c r="H101" s="5">
+      <c r="H111" s="5">
         <v>2</v>
       </c>
-      <c r="I101" s="5" t="s">
+      <c r="I111" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J101" s="5" t="s">
+      <c r="J111" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K101">
-        <v>0.1</v>
-      </c>
-      <c r="L101" s="8">
-        <f>K101/G101</f>
+      <c r="K111">
+        <v>0.1</v>
+      </c>
+      <c r="L111" s="8">
+        <f>K111/G111</f>
         <v>5.9701492537313436</v>
       </c>
-      <c r="M101" s="8">
+      <c r="M111" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O101">
-        <f>8*(M101/A101)^2</f>
+      <c r="O111">
+        <f>8*(M111/A111)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:15">
-      <c r="A102" s="5">
+    <row r="112" spans="1:24">
+      <c r="A112" s="5">
         <v>250000</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B112" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C112" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D102" s="5">
-        <f t="shared" ref="D102:D103" si="80">E102*2</f>
-        <v>0.1</v>
-      </c>
-      <c r="E102" s="5">
+      <c r="D112" s="5">
+        <f t="shared" ref="D112:D113" si="88">E112*2</f>
+        <v>0.1</v>
+      </c>
+      <c r="E112" s="5">
         <v>0.05</v>
       </c>
-      <c r="F102">
-        <f>E102</f>
+      <c r="F112">
+        <f>E112</f>
         <v>0.05</v>
       </c>
-      <c r="G102" s="5">
-        <f>0.25*F102</f>
+      <c r="G112" s="5">
+        <f>0.25*F112</f>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="H102" s="5">
+      <c r="H112" s="5">
         <v>2</v>
       </c>
-      <c r="I102" s="5" t="s">
+      <c r="I112" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J102" s="5" t="s">
+      <c r="J112" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K102">
-        <v>0.1</v>
-      </c>
-      <c r="L102" s="8">
-        <f>K102/G102</f>
+      <c r="K112">
+        <v>0.1</v>
+      </c>
+      <c r="L112" s="8">
+        <f>K112/G112</f>
         <v>8</v>
       </c>
-      <c r="M102" s="8">
+      <c r="M112" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O102">
-        <f>8*(M102/A102)^2</f>
+      <c r="O112">
+        <f>8*(M112/A112)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:15">
-      <c r="A103" s="5">
+    <row r="113" spans="1:15">
+      <c r="A113" s="5">
         <v>250000</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B113" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C103" s="5" t="s">
+      <c r="C113" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D103" s="5">
-        <f t="shared" si="80"/>
+      <c r="D113" s="5">
+        <f t="shared" si="88"/>
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="E103" s="5">
+      <c r="E113" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F103">
-        <f>E103</f>
+      <c r="F113">
+        <f>E113</f>
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="G103" s="5">
-        <f>0.25*F103</f>
+      <c r="G113" s="5">
+        <f>0.25*F113</f>
         <v>8.2500000000000004E-3</v>
       </c>
-      <c r="H103" s="5">
+      <c r="H113" s="5">
         <v>2</v>
       </c>
-      <c r="I103" s="5" t="s">
+      <c r="I113" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J103" s="5" t="s">
+      <c r="J113" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K103">
-        <v>0.1</v>
-      </c>
-      <c r="L103" s="8">
-        <f>K103/G103</f>
+      <c r="K113">
+        <v>0.1</v>
+      </c>
+      <c r="L113" s="8">
+        <f>K113/G113</f>
         <v>12.121212121212121</v>
       </c>
-      <c r="M103" s="8">
+      <c r="M113" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O103">
-        <f>8*(M103/A103)^2</f>
+      <c r="O113">
+        <f>8*(M113/A113)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some output modifications for square duct
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC0D622-53F8-49AA-A118-2B4C0B26A6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3F6792-AB8D-4938-8F9F-2EB49880FDEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="5" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="213">
   <si>
     <t>nompi</t>
   </si>
@@ -688,6 +688,24 @@
   <si>
     <t>WM+SMAG+SMALL+ONESIDE+2ND</t>
   </si>
+  <si>
+    <t>ONESIDE</t>
+  </si>
+  <si>
+    <t>64×24×32</t>
+  </si>
+  <si>
+    <t>96×36×48</t>
+  </si>
+  <si>
+    <t>128×48×64</t>
+  </si>
+  <si>
+    <t>192×72×96</t>
+  </si>
+  <si>
+    <t>WM+DSMAG+SMALL</t>
+  </si>
 </sst>
 </file>
 
@@ -699,7 +717,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -733,6 +751,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4375,8 +4399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B745900-CF34-4783-B8B3-D2DA1ADCC55F}">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5760,10 +5784,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3643DFC1-43AF-4E64-819A-C97D29654F85}">
-  <dimension ref="A1:X44"/>
+  <dimension ref="A1:X58"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C21" sqref="C21:R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -8697,7 +8721,7 @@
         <v>1.094476E-3</v>
       </c>
       <c r="I44" s="19">
-        <f t="shared" ref="I44" si="62">E44/F44</f>
+        <f t="shared" ref="I44:I45" si="62">E44/F44</f>
         <v>1.7777777777777779</v>
       </c>
       <c r="J44" s="5" t="s">
@@ -8719,15 +8743,15 @@
         <v>549.31194168112302</v>
       </c>
       <c r="P44" s="9">
-        <f t="shared" ref="P44" si="63">8*(N44/B44)^2</f>
+        <f t="shared" ref="P44:P45" si="63">8*(N44/B44)^2</f>
         <v>5.772630931736967E-3</v>
       </c>
       <c r="Q44" s="9">
-        <f t="shared" ref="Q44" si="64">8*(O44/B44)^2</f>
+        <f t="shared" ref="Q44:Q45" si="64">8*(O44/B44)^2</f>
         <v>5.721727747572799E-3</v>
       </c>
       <c r="R44" s="10">
-        <f t="shared" ref="R44" si="65">(Q44-P44)/P44</f>
+        <f t="shared" ref="R44:R45" si="65">(Q44-P44)/P44</f>
         <v>-8.8180215860173463E-3</v>
       </c>
       <c r="S44" s="8">
@@ -8735,24 +8759,785 @@
         <v>10.69740879612703</v>
       </c>
       <c r="T44" s="4">
-        <f t="shared" ref="T44" si="66">B44/4*P44</f>
+        <f t="shared" ref="T44:T45" si="66">B44/4*P44</f>
         <v>29.642459834469324</v>
       </c>
       <c r="U44" s="8">
-        <f t="shared" ref="U44" si="67">E44*N44</f>
+        <f t="shared" ref="U44:U45" si="67">E44*N44</f>
         <v>18.391666666666666</v>
       </c>
       <c r="V44" s="8">
-        <f t="shared" ref="V44" si="68">F44*N44</f>
+        <f t="shared" ref="V44:V45" si="68">F44*N44</f>
         <v>10.3453125</v>
       </c>
       <c r="W44" s="8">
-        <f t="shared" ref="W44" si="69">G44*N44</f>
+        <f t="shared" ref="W44:W45" si="69">G44*N44</f>
         <v>21.834044112499999</v>
       </c>
       <c r="X44" s="8">
-        <f t="shared" ref="X44" si="70">H44*N44</f>
+        <f t="shared" ref="X44:X45" si="70">H44*N44</f>
         <v>0.60387713300000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24">
+      <c r="A45" t="s">
+        <v>192</v>
+      </c>
+      <c r="B45" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E45" s="18">
+        <f>6.4/384</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F45" s="5">
+        <f>2.4/256</f>
+        <v>9.3749999999999997E-3</v>
+      </c>
+      <c r="G45" s="18">
+        <v>1.9793720000000001E-2</v>
+      </c>
+      <c r="H45" s="13">
+        <v>5.3669989999999995E-4</v>
+      </c>
+      <c r="I45" s="19">
+        <f>E45/F45</f>
+        <v>1.7777777777777779</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M45" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N45" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O45" s="4">
+        <v>544.25273791426696</v>
+      </c>
+      <c r="P45" s="9">
+        <f>8*(N45/B45)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q45" s="9">
+        <f>8*(O45/B45)^2</f>
+        <v>5.6168180210684595E-3</v>
+      </c>
+      <c r="R45" s="10">
+        <f>(Q45-P45)/P45</f>
+        <v>-2.6991663335321516E-2</v>
+      </c>
+      <c r="S45" s="8">
+        <f>200*2*O45/B45</f>
+        <v>10.59888486687959</v>
+      </c>
+      <c r="T45" s="4">
+        <f>B45/4*P45</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U45" s="8">
+        <f>E45*N45</f>
+        <v>9.1958333333333329</v>
+      </c>
+      <c r="V45" s="8">
+        <f>F45*N45</f>
+        <v>5.1726562500000002</v>
+      </c>
+      <c r="W45" s="8">
+        <f>G45*N45</f>
+        <v>10.92118501</v>
+      </c>
+      <c r="X45" s="8">
+        <f>H45*N45</f>
+        <v>0.29612416982499995</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24">
+      <c r="A48" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24">
+      <c r="A49" t="s">
+        <v>204</v>
+      </c>
+      <c r="B49" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E49" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F49" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G49">
+        <f>F49</f>
+        <v>0.1</v>
+      </c>
+      <c r="H49" s="5">
+        <f>0.25*G49</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I49" s="5">
+        <v>1</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L49">
+        <v>0.1</v>
+      </c>
+      <c r="M49" s="8">
+        <f>L49/H49</f>
+        <v>4</v>
+      </c>
+      <c r="N49" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O49" s="4"/>
+      <c r="P49" s="9">
+        <f>8*(N49/B49)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q49" s="9">
+        <f>8*(O49/B49)^2</f>
+        <v>0</v>
+      </c>
+      <c r="R49" s="10">
+        <f>(Q49-P49)/P49</f>
+        <v>-1</v>
+      </c>
+      <c r="S49" s="8">
+        <v>10.7</v>
+      </c>
+      <c r="T49" s="4">
+        <f>B49/4*P49</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U49" s="8">
+        <f>E49*N49</f>
+        <v>55.175000000000004</v>
+      </c>
+      <c r="V49" s="8">
+        <f>F49*N49</f>
+        <v>55.175000000000004</v>
+      </c>
+      <c r="W49" s="8">
+        <f>G49*N49</f>
+        <v>55.175000000000004</v>
+      </c>
+      <c r="X49" s="8">
+        <f>H49*N49</f>
+        <v>13.793750000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24">
+      <c r="A50" t="s">
+        <v>204</v>
+      </c>
+      <c r="B50" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E50" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F50" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G50">
+        <f>F50</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H50" s="5">
+        <f>0.25*G50</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I50" s="5">
+        <v>1</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L50">
+        <v>0.1</v>
+      </c>
+      <c r="M50" s="8">
+        <f t="shared" ref="M50:M52" si="71">L50/H50</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N50" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O50" s="4"/>
+      <c r="P50" s="9">
+        <f>8*(N50/B50)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q50" s="9">
+        <f t="shared" ref="Q50:Q52" si="72">8*(O50/B50)^2</f>
+        <v>0</v>
+      </c>
+      <c r="R50" s="10">
+        <f t="shared" ref="R50:R52" si="73">(Q50-P50)/P50</f>
+        <v>-1</v>
+      </c>
+      <c r="S50" s="8">
+        <f t="shared" ref="S50:S52" si="74">200*2*O50/B50</f>
+        <v>0</v>
+      </c>
+      <c r="T50" s="4">
+        <f t="shared" ref="T50:T52" si="75">B50/4*P50</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U50" s="8">
+        <f t="shared" ref="U50:U52" si="76">E50*N50</f>
+        <v>36.96725</v>
+      </c>
+      <c r="V50" s="8">
+        <f t="shared" ref="V50:V52" si="77">F50*N50</f>
+        <v>36.96725</v>
+      </c>
+      <c r="W50" s="8">
+        <f t="shared" ref="W50:W52" si="78">G50*N50</f>
+        <v>36.96725</v>
+      </c>
+      <c r="X50" s="8">
+        <f t="shared" ref="X50:X52" si="79">H50*N50</f>
+        <v>9.2418125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24">
+      <c r="A51" t="s">
+        <v>204</v>
+      </c>
+      <c r="B51" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E51" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F51" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G51">
+        <f>F51</f>
+        <v>0.05</v>
+      </c>
+      <c r="H51" s="5">
+        <f>0.25*G51</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I51" s="5">
+        <v>1</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L51">
+        <v>0.1</v>
+      </c>
+      <c r="M51" s="8">
+        <f t="shared" si="71"/>
+        <v>8</v>
+      </c>
+      <c r="N51" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O51" s="4"/>
+      <c r="P51" s="9">
+        <f>8*(N51/B51)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q51" s="9">
+        <f t="shared" si="72"/>
+        <v>0</v>
+      </c>
+      <c r="R51" s="10">
+        <f t="shared" si="73"/>
+        <v>-1</v>
+      </c>
+      <c r="S51" s="8">
+        <f t="shared" si="74"/>
+        <v>0</v>
+      </c>
+      <c r="T51" s="4">
+        <f t="shared" si="75"/>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U51" s="8">
+        <f t="shared" si="76"/>
+        <v>27.587500000000002</v>
+      </c>
+      <c r="V51" s="8">
+        <f t="shared" si="77"/>
+        <v>27.587500000000002</v>
+      </c>
+      <c r="W51" s="8">
+        <f t="shared" si="78"/>
+        <v>27.587500000000002</v>
+      </c>
+      <c r="X51" s="8">
+        <f t="shared" si="79"/>
+        <v>6.8968750000000005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24">
+      <c r="A52" t="s">
+        <v>204</v>
+      </c>
+      <c r="B52" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E52" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F52" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G52">
+        <f>F52</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H52" s="5">
+        <f>0.25*G52</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I52" s="5">
+        <v>1</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L52">
+        <v>0.1</v>
+      </c>
+      <c r="M52" s="8">
+        <f t="shared" si="71"/>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N52" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O52" s="4"/>
+      <c r="P52" s="9">
+        <f>8*(N52/B52)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q52" s="9">
+        <f t="shared" si="72"/>
+        <v>0</v>
+      </c>
+      <c r="R52" s="10">
+        <f t="shared" si="73"/>
+        <v>-1</v>
+      </c>
+      <c r="S52" s="8">
+        <f t="shared" si="74"/>
+        <v>0</v>
+      </c>
+      <c r="T52" s="4">
+        <f t="shared" si="75"/>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U52" s="8">
+        <f t="shared" si="76"/>
+        <v>18.207750000000001</v>
+      </c>
+      <c r="V52" s="8">
+        <f t="shared" si="77"/>
+        <v>18.207750000000001</v>
+      </c>
+      <c r="W52" s="8">
+        <f t="shared" si="78"/>
+        <v>18.207750000000001</v>
+      </c>
+      <c r="X52" s="8">
+        <f t="shared" si="79"/>
+        <v>4.5519375000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24">
+      <c r="A55" t="s">
+        <v>212</v>
+      </c>
+      <c r="B55" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E55" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F55" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G55">
+        <f>F55</f>
+        <v>0.1</v>
+      </c>
+      <c r="H55" s="5">
+        <f>0.25*G55</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I55" s="5">
+        <v>1</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L55">
+        <v>0.1</v>
+      </c>
+      <c r="M55" s="8">
+        <f>L55/H55</f>
+        <v>4</v>
+      </c>
+      <c r="N55" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O55" s="4"/>
+      <c r="P55" s="9">
+        <f>8*(N55/B55)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q55" s="9">
+        <f>8*(O55/B55)^2</f>
+        <v>0</v>
+      </c>
+      <c r="R55" s="10">
+        <f>(Q55-P55)/P55</f>
+        <v>-1</v>
+      </c>
+      <c r="S55" s="8">
+        <v>10.7</v>
+      </c>
+      <c r="T55" s="4">
+        <f>B55/4*P55</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U55" s="8">
+        <f>E55*N55</f>
+        <v>55.175000000000004</v>
+      </c>
+      <c r="V55" s="8">
+        <f>F55*N55</f>
+        <v>55.175000000000004</v>
+      </c>
+      <c r="W55" s="8">
+        <f>G55*N55</f>
+        <v>55.175000000000004</v>
+      </c>
+      <c r="X55" s="8">
+        <f>H55*N55</f>
+        <v>13.793750000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24">
+      <c r="A56" t="s">
+        <v>212</v>
+      </c>
+      <c r="B56" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E56" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F56" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G56">
+        <f>F56</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H56" s="5">
+        <f>0.25*G56</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I56" s="5">
+        <v>1</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K56" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L56">
+        <v>0.1</v>
+      </c>
+      <c r="M56" s="8">
+        <f t="shared" ref="M56:M58" si="80">L56/H56</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N56" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O56" s="4"/>
+      <c r="P56" s="9">
+        <f>8*(N56/B56)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q56" s="9">
+        <f t="shared" ref="Q56:Q58" si="81">8*(O56/B56)^2</f>
+        <v>0</v>
+      </c>
+      <c r="R56" s="10">
+        <f t="shared" ref="R56:R58" si="82">(Q56-P56)/P56</f>
+        <v>-1</v>
+      </c>
+      <c r="S56" s="8">
+        <f t="shared" ref="S56:S58" si="83">200*2*O56/B56</f>
+        <v>0</v>
+      </c>
+      <c r="T56" s="4">
+        <f t="shared" ref="T56:T58" si="84">B56/4*P56</f>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U56" s="8">
+        <f t="shared" ref="U56:U58" si="85">E56*N56</f>
+        <v>36.96725</v>
+      </c>
+      <c r="V56" s="8">
+        <f t="shared" ref="V56:V58" si="86">F56*N56</f>
+        <v>36.96725</v>
+      </c>
+      <c r="W56" s="8">
+        <f t="shared" ref="W56:W58" si="87">G56*N56</f>
+        <v>36.96725</v>
+      </c>
+      <c r="X56" s="8">
+        <f t="shared" ref="X56:X58" si="88">H56*N56</f>
+        <v>9.2418125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24">
+      <c r="A57" t="s">
+        <v>212</v>
+      </c>
+      <c r="B57" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E57" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F57" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G57">
+        <f>F57</f>
+        <v>0.05</v>
+      </c>
+      <c r="H57" s="5">
+        <f>0.25*G57</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I57" s="5">
+        <v>1</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K57" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L57">
+        <v>0.1</v>
+      </c>
+      <c r="M57" s="8">
+        <f t="shared" si="80"/>
+        <v>8</v>
+      </c>
+      <c r="N57" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O57" s="4"/>
+      <c r="P57" s="9">
+        <f>8*(N57/B57)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q57" s="9">
+        <f t="shared" si="81"/>
+        <v>0</v>
+      </c>
+      <c r="R57" s="10">
+        <f t="shared" si="82"/>
+        <v>-1</v>
+      </c>
+      <c r="S57" s="8">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="T57" s="4">
+        <f t="shared" si="84"/>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U57" s="8">
+        <f t="shared" si="85"/>
+        <v>27.587500000000002</v>
+      </c>
+      <c r="V57" s="8">
+        <f t="shared" si="86"/>
+        <v>27.587500000000002</v>
+      </c>
+      <c r="W57" s="8">
+        <f t="shared" si="87"/>
+        <v>27.587500000000002</v>
+      </c>
+      <c r="X57" s="8">
+        <f t="shared" si="88"/>
+        <v>6.8968750000000005</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24">
+      <c r="A58" t="s">
+        <v>212</v>
+      </c>
+      <c r="B58" s="5">
+        <v>20540</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E58" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F58" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G58">
+        <f>F58</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H58" s="5">
+        <f>0.25*G58</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I58" s="5">
+        <v>1</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K58" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L58">
+        <v>0.1</v>
+      </c>
+      <c r="M58" s="8">
+        <f t="shared" si="80"/>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N58" s="12">
+        <v>551.75</v>
+      </c>
+      <c r="O58" s="4"/>
+      <c r="P58" s="9">
+        <f>8*(N58/B58)^2</f>
+        <v>5.772630931736967E-3</v>
+      </c>
+      <c r="Q58" s="9">
+        <f t="shared" si="81"/>
+        <v>0</v>
+      </c>
+      <c r="R58" s="10">
+        <f t="shared" si="82"/>
+        <v>-1</v>
+      </c>
+      <c r="S58" s="8">
+        <f t="shared" si="83"/>
+        <v>0</v>
+      </c>
+      <c r="T58" s="4">
+        <f t="shared" si="84"/>
+        <v>29.642459834469324</v>
+      </c>
+      <c r="U58" s="8">
+        <f t="shared" si="85"/>
+        <v>18.207750000000001</v>
+      </c>
+      <c r="V58" s="8">
+        <f t="shared" si="86"/>
+        <v>18.207750000000001</v>
+      </c>
+      <c r="W58" s="8">
+        <f t="shared" si="87"/>
+        <v>18.207750000000001</v>
+      </c>
+      <c r="X58" s="8">
+        <f t="shared" si="88"/>
+        <v>4.5519375000000002</v>
       </c>
     </row>
   </sheetData>
@@ -8768,7 +9553,7 @@
   <dimension ref="A1:X35"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -10824,10 +11609,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42F51E-90FA-449F-904F-669D9897EDC7}">
-  <dimension ref="A1:X113"/>
+  <dimension ref="A1:X134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R101" sqref="R101"/>
+    <sheetView topLeftCell="A52" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S110" sqref="S110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -14572,19 +15357,19 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U62" s="8">
-        <f t="shared" ref="U62:U77" si="48">E62*N62</f>
+        <f t="shared" ref="U62:U71" si="48">E62*N62</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V62" s="8">
-        <f t="shared" ref="V62:V77" si="49">F62*O62</f>
+        <f t="shared" ref="V62:V71" si="49">F62*O62</f>
         <v>486.30764273383807</v>
       </c>
       <c r="W62" s="8">
-        <f t="shared" ref="W62:W77" si="50">G62*N62</f>
+        <f t="shared" ref="W62:W71" si="50">G62*N62</f>
         <v>518.58969999999999</v>
       </c>
       <c r="X62" s="4">
-        <f t="shared" ref="X62:X77" si="51">H62*N62</f>
+        <f t="shared" ref="X62:X71" si="51">H62*N62</f>
         <v>129.647425</v>
       </c>
     </row>
@@ -15284,19 +16069,19 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U74" s="8">
-        <f t="shared" si="48"/>
+        <f>E74*N74</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V74" s="8">
-        <f t="shared" si="49"/>
+        <f>F74*O74</f>
         <v>269.73210756077401</v>
       </c>
       <c r="W74" s="8">
-        <f t="shared" si="50"/>
+        <f>G74*N74</f>
         <v>518.58969999999999</v>
       </c>
       <c r="X74" s="4">
-        <f t="shared" si="51"/>
+        <f>H74*N74</f>
         <v>129.647425</v>
       </c>
     </row>
@@ -15370,19 +16155,19 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U75" s="8">
-        <f t="shared" si="48"/>
+        <f>E75*N75</f>
         <v>347.45509900000002</v>
       </c>
       <c r="V75" s="8">
-        <f t="shared" si="49"/>
+        <f>F75*O75</f>
         <v>214.63903361563635</v>
       </c>
       <c r="W75" s="8">
-        <f t="shared" si="50"/>
+        <f>G75*N75</f>
         <v>347.45509900000002</v>
       </c>
       <c r="X75" s="4">
-        <f t="shared" si="51"/>
+        <f>H75*N75</f>
         <v>86.863774750000005</v>
       </c>
     </row>
@@ -15456,19 +16241,19 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U76" s="8">
-        <f t="shared" si="48"/>
+        <f>E76*N76</f>
         <v>259.29485</v>
       </c>
       <c r="V76" s="8">
-        <f t="shared" si="49"/>
+        <f>F76*O76</f>
         <v>179.50305675292401</v>
       </c>
       <c r="W76" s="8">
-        <f t="shared" si="50"/>
+        <f>G76*N76</f>
         <v>259.29485</v>
       </c>
       <c r="X76" s="4">
-        <f t="shared" si="51"/>
+        <f>H76*N76</f>
         <v>64.823712499999999</v>
       </c>
     </row>
@@ -15542,19 +16327,19 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U77" s="8">
-        <f t="shared" si="48"/>
+        <f>E77*N77</f>
         <v>171.134601</v>
       </c>
       <c r="V77" s="8">
-        <f t="shared" si="49"/>
+        <f>F77*O77</f>
         <v>136.72786348482526</v>
       </c>
       <c r="W77" s="8">
-        <f t="shared" si="50"/>
+        <f>G77*N77</f>
         <v>171.134601</v>
       </c>
       <c r="X77" s="4">
-        <f t="shared" si="51"/>
+        <f>H77*N77</f>
         <v>42.783650250000001</v>
       </c>
     </row>
@@ -15628,19 +16413,19 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U80" s="8">
-        <f t="shared" ref="U80:U83" si="56">E80*N80</f>
+        <f>E80*N80</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V80" s="8">
-        <f t="shared" ref="V80:V83" si="57">F80*O80</f>
+        <f>F80*O80</f>
         <v>493.64000411562006</v>
       </c>
       <c r="W80" s="8">
-        <f t="shared" ref="W80:W83" si="58">G80*N80</f>
+        <f>G80*N80</f>
         <v>518.58969999999999</v>
       </c>
       <c r="X80" s="4">
-        <f t="shared" ref="X80:X83" si="59">H80*N80</f>
+        <f>H80*N80</f>
         <v>129.647425</v>
       </c>
     </row>
@@ -15702,31 +16487,31 @@
         <v>3.3161899397384782E-3</v>
       </c>
       <c r="R81" s="10">
-        <f t="shared" ref="R81:R83" si="60">(Q81-P81)/P81</f>
+        <f>(Q81-P81)/P81</f>
         <v>-3.6655428830177257E-2</v>
       </c>
       <c r="S81" s="8">
-        <f t="shared" ref="S81:S83" si="61">500*2*O81/B81</f>
+        <f>500*2*O81/B81</f>
         <v>20.359856150457201</v>
       </c>
       <c r="T81" s="4">
-        <f t="shared" ref="T81:T83" si="62">B81/4*P81</f>
+        <f>B81/4*P81</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U81" s="8">
-        <f t="shared" si="56"/>
+        <f>E81*N81</f>
         <v>347.45509900000002</v>
       </c>
       <c r="V81" s="8">
-        <f t="shared" si="57"/>
+        <f>F81*O81</f>
         <v>341.02759052015813</v>
       </c>
       <c r="W81" s="8">
-        <f t="shared" si="58"/>
+        <f>G81*N81</f>
         <v>347.45509900000002</v>
       </c>
       <c r="X81" s="4">
-        <f t="shared" si="59"/>
+        <f>H81*N81</f>
         <v>86.863774750000005</v>
       </c>
     </row>
@@ -15784,35 +16569,35 @@
         <v>3.4423715449099523E-3</v>
       </c>
       <c r="Q82" s="9">
-        <f t="shared" ref="Q82:Q83" si="63">8*(O82/B82)^2</f>
+        <f>8*(O82/B82)^2</f>
         <v>3.3629192338376869E-3</v>
       </c>
       <c r="R82" s="10">
-        <f t="shared" si="60"/>
+        <f>(Q82-P82)/P82</f>
         <v>-2.308069016830773E-2</v>
       </c>
       <c r="S82" s="8">
-        <f t="shared" si="61"/>
+        <f>500*2*O82/B82</f>
         <v>20.502802350647361</v>
       </c>
       <c r="T82" s="4">
-        <f t="shared" si="62"/>
+        <f>B82/4*P82</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U82" s="8">
-        <f t="shared" si="56"/>
+        <f>E82*N82</f>
         <v>259.29485</v>
       </c>
       <c r="V82" s="8">
-        <f t="shared" si="57"/>
+        <f>F82*O82</f>
         <v>256.28502938309197</v>
       </c>
       <c r="W82" s="8">
-        <f t="shared" si="58"/>
+        <f>G82*N82</f>
         <v>259.29485</v>
       </c>
       <c r="X82" s="4">
-        <f t="shared" si="59"/>
+        <f>H82*N82</f>
         <v>64.823712499999999</v>
       </c>
     </row>
@@ -15870,35 +16655,35 @@
         <v>3.4423715449099523E-3</v>
       </c>
       <c r="Q83" s="9">
-        <f t="shared" si="63"/>
+        <f>8*(O83/B83)^2</f>
         <v>3.3838565303621103E-3</v>
       </c>
       <c r="R83" s="10">
-        <f t="shared" si="60"/>
+        <f>(Q83-P83)/P83</f>
         <v>-1.699845986536954E-2</v>
       </c>
       <c r="S83" s="8">
-        <f t="shared" si="61"/>
+        <f>500*2*O83/B83</f>
         <v>20.566527813300521</v>
       </c>
       <c r="T83" s="4">
-        <f t="shared" si="62"/>
+        <f>B83/4*P83</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U83" s="8">
-        <f t="shared" si="56"/>
+        <f>E83*N83</f>
         <v>171.134601</v>
       </c>
       <c r="V83" s="8">
-        <f t="shared" si="57"/>
+        <f>F83*O83</f>
         <v>169.67385445972928</v>
       </c>
       <c r="W83" s="8">
-        <f t="shared" si="58"/>
+        <f>G83*N83</f>
         <v>171.134601</v>
       </c>
       <c r="X83" s="4">
-        <f t="shared" si="59"/>
+        <f>H83*N83</f>
         <v>42.783650250000001</v>
       </c>
     </row>
@@ -15972,19 +16757,19 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U86" s="8">
-        <f t="shared" ref="U86:U89" si="64">E86*N86</f>
+        <f>E86*N86</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V86" s="8">
-        <f t="shared" ref="V86:V89" si="65">F86*O86</f>
+        <f>F86*O86</f>
         <v>490.28200076165808</v>
       </c>
       <c r="W86" s="8">
-        <f t="shared" ref="W86:W89" si="66">G86*N86</f>
+        <f>G86*N86</f>
         <v>518.58969999999999</v>
       </c>
       <c r="X86" s="4">
-        <f t="shared" ref="X86:X89" si="67">H86*N86</f>
+        <f>H86*N86</f>
         <v>129.647425</v>
       </c>
     </row>
@@ -16046,31 +16831,31 @@
         <v>3.300080223724636E-3</v>
       </c>
       <c r="R87" s="10">
-        <f t="shared" ref="R87:R89" si="68">(Q87-P87)/P87</f>
+        <f>(Q87-P87)/P87</f>
         <v>-4.1335259523544096E-2</v>
       </c>
       <c r="S87" s="8">
-        <f t="shared" ref="S87:S89" si="69">500*2*O87/B87</f>
+        <f>500*2*O87/B87</f>
         <v>20.310342881536481</v>
       </c>
       <c r="T87" s="4">
-        <f t="shared" ref="T87:T89" si="70">B87/4*P87</f>
+        <f>B87/4*P87</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U87" s="8">
-        <f t="shared" si="64"/>
+        <f>E87*N87</f>
         <v>347.45509900000002</v>
       </c>
       <c r="V87" s="8">
-        <f t="shared" si="65"/>
+        <f>F87*O87</f>
         <v>340.19824326573604</v>
       </c>
       <c r="W87" s="8">
-        <f t="shared" si="66"/>
+        <f>G87*N87</f>
         <v>347.45509900000002</v>
       </c>
       <c r="X87" s="4">
-        <f t="shared" si="67"/>
+        <f>H87*N87</f>
         <v>86.863774750000005</v>
       </c>
     </row>
@@ -16128,35 +16913,35 @@
         <v>3.4423715449099523E-3</v>
       </c>
       <c r="Q88" s="9">
-        <f t="shared" ref="Q88:Q89" si="71">8*(O88/B88)^2</f>
+        <f>8*(O88/B88)^2</f>
         <v>3.3519760489614161E-3</v>
       </c>
       <c r="R88" s="10">
-        <f t="shared" si="68"/>
+        <f>(Q88-P88)/P88</f>
         <v>-2.6259656974622368E-2</v>
       </c>
       <c r="S88" s="8">
-        <f t="shared" si="69"/>
+        <f>500*2*O88/B88</f>
         <v>20.469416360027878</v>
       </c>
       <c r="T88" s="4">
-        <f t="shared" si="70"/>
+        <f>B88/4*P88</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U88" s="8">
-        <f t="shared" si="64"/>
+        <f>E88*N88</f>
         <v>259.29485</v>
       </c>
       <c r="V88" s="8">
-        <f t="shared" si="65"/>
+        <f>F88*O88</f>
         <v>255.86770450034851</v>
       </c>
       <c r="W88" s="8">
-        <f t="shared" si="66"/>
+        <f>G88*N88</f>
         <v>259.29485</v>
       </c>
       <c r="X88" s="4">
-        <f t="shared" si="67"/>
+        <f>H88*N88</f>
         <v>64.823712499999999</v>
       </c>
     </row>
@@ -16214,35 +16999,35 @@
         <v>3.4423715449099523E-3</v>
       </c>
       <c r="Q89" s="9">
-        <f t="shared" si="71"/>
+        <f>8*(O89/B89)^2</f>
         <v>3.412906370546317E-3</v>
       </c>
       <c r="R89" s="10">
-        <f t="shared" si="68"/>
+        <f>(Q89-P89)/P89</f>
         <v>-8.5595566832998744E-3</v>
       </c>
       <c r="S89" s="8">
-        <f t="shared" si="69"/>
+        <f>500*2*O89/B89</f>
         <v>20.65461924893048</v>
       </c>
       <c r="T89" s="4">
-        <f t="shared" si="70"/>
+        <f>B89/4*P89</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U89" s="8">
-        <f t="shared" si="64"/>
+        <f>E89*N89</f>
         <v>171.134601</v>
       </c>
       <c r="V89" s="8">
-        <f t="shared" si="65"/>
+        <f>F89*O89</f>
         <v>170.40060880367648</v>
       </c>
       <c r="W89" s="8">
-        <f t="shared" si="66"/>
+        <f>G89*N89</f>
         <v>171.134601</v>
       </c>
       <c r="X89" s="4">
-        <f t="shared" si="67"/>
+        <f>H89*N89</f>
         <v>42.783650250000001</v>
       </c>
     </row>
@@ -16316,19 +17101,19 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U92" s="8">
-        <f t="shared" ref="U92:U95" si="72">E92*N92</f>
+        <f>E92*N92</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V92" s="8">
-        <f t="shared" ref="V92:V95" si="73">F92*O92</f>
+        <f>F92*O92</f>
         <v>516.127964639281</v>
       </c>
       <c r="W92" s="8">
-        <f t="shared" ref="W92:W95" si="74">G92*N92</f>
+        <f>G92*N92</f>
         <v>518.58969999999999</v>
       </c>
       <c r="X92" s="4">
-        <f t="shared" ref="X92:X95" si="75">H92*N92</f>
+        <f>H92*N92</f>
         <v>129.647425</v>
       </c>
     </row>
@@ -16390,31 +17175,31 @@
         <v>3.3786065272879864E-3</v>
       </c>
       <c r="R93" s="10">
-        <f t="shared" ref="R93:R95" si="76">(Q93-P93)/P93</f>
+        <f>(Q93-P93)/P93</f>
         <v>-1.8523572133360134E-2</v>
       </c>
       <c r="S93" s="8">
-        <f t="shared" ref="S93:S95" si="77">500*2*O93/B93</f>
+        <f>500*2*O93/B93</f>
         <v>20.550567289274479</v>
       </c>
       <c r="T93" s="4">
-        <f t="shared" ref="T93:T95" si="78">B93/4*P93</f>
+        <f>B93/4*P93</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U93" s="8">
-        <f t="shared" si="72"/>
+        <f>E93*N93</f>
         <v>347.45509900000002</v>
       </c>
       <c r="V93" s="8">
-        <f t="shared" si="73"/>
+        <f>F93*O93</f>
         <v>344.22200209534759</v>
       </c>
       <c r="W93" s="8">
-        <f t="shared" si="74"/>
+        <f>G93*N93</f>
         <v>347.45509900000002</v>
       </c>
       <c r="X93" s="4">
-        <f t="shared" si="75"/>
+        <f>H93*N93</f>
         <v>86.863774750000005</v>
       </c>
     </row>
@@ -16472,35 +17257,35 @@
         <v>3.4423715449099523E-3</v>
       </c>
       <c r="Q94" s="9">
-        <f t="shared" ref="Q94:Q95" si="79">8*(O94/B94)^2</f>
+        <f>8*(O94/B94)^2</f>
         <v>3.4285036896251008E-3</v>
       </c>
       <c r="R94" s="10">
-        <f t="shared" si="76"/>
+        <f>(Q94-P94)/P94</f>
         <v>-4.0285759697721007E-3</v>
       </c>
       <c r="S94" s="8">
-        <f t="shared" si="77"/>
+        <f>500*2*O94/B94</f>
         <v>20.70176227288724</v>
       </c>
       <c r="T94" s="4">
-        <f t="shared" si="78"/>
+        <f>B94/4*P94</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U94" s="8">
-        <f t="shared" si="72"/>
+        <f>E94*N94</f>
         <v>259.29485</v>
       </c>
       <c r="V94" s="8">
-        <f t="shared" si="73"/>
+        <f>F94*O94</f>
         <v>258.7720284110905</v>
       </c>
       <c r="W94" s="8">
-        <f t="shared" si="74"/>
+        <f>G94*N94</f>
         <v>259.29485</v>
       </c>
       <c r="X94" s="4">
-        <f t="shared" si="75"/>
+        <f>H94*N94</f>
         <v>64.823712499999999</v>
       </c>
     </row>
@@ -16558,35 +17343,35 @@
         <v>3.4423715449099523E-3</v>
       </c>
       <c r="Q95" s="9">
-        <f t="shared" si="79"/>
+        <f>8*(O95/B95)^2</f>
         <v>3.4085381852924043E-3</v>
       </c>
       <c r="R95" s="10">
-        <f t="shared" si="76"/>
+        <f>(Q95-P95)/P95</f>
         <v>-9.8285031630521037E-3</v>
       </c>
       <c r="S95" s="8">
-        <f t="shared" si="77"/>
+        <f>500*2*O95/B95</f>
         <v>20.641397073879244</v>
       </c>
       <c r="T95" s="4">
-        <f t="shared" si="78"/>
+        <f>B95/4*P95</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U95" s="8">
-        <f t="shared" si="72"/>
+        <f>E95*N95</f>
         <v>171.134601</v>
       </c>
       <c r="V95" s="8">
-        <f t="shared" si="73"/>
+        <f>F95*O95</f>
         <v>170.29152585950374</v>
       </c>
       <c r="W95" s="8">
-        <f t="shared" si="74"/>
+        <f>G95*N95</f>
         <v>171.134601</v>
       </c>
       <c r="X95" s="4">
-        <f t="shared" si="75"/>
+        <f>H95*N95</f>
         <v>42.783650250000001</v>
       </c>
     </row>
@@ -16660,19 +17445,19 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U98" s="8">
-        <f t="shared" ref="U98:U101" si="80">E98*N98</f>
+        <f>E98*N98</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V98" s="8">
-        <f t="shared" ref="V98:V101" si="81">F98*O98</f>
+        <f>F98*O98</f>
         <v>515.02287556594104</v>
       </c>
       <c r="W98" s="8">
-        <f t="shared" ref="W98:W101" si="82">G98*N98</f>
+        <f>G98*N98</f>
         <v>518.58969999999999</v>
       </c>
       <c r="X98" s="4">
-        <f t="shared" ref="X98:X101" si="83">H98*N98</f>
+        <f>H98*N98</f>
         <v>129.647425</v>
       </c>
     </row>
@@ -16734,31 +17519,31 @@
         <v>3.3798809974511447E-3</v>
       </c>
       <c r="R99" s="10">
-        <f t="shared" ref="R99:R101" si="84">(Q99-P99)/P99</f>
+        <f>(Q99-P99)/P99</f>
         <v>-1.8153341858524522E-2</v>
       </c>
       <c r="S99" s="8">
-        <f t="shared" ref="S99:S101" si="85">500*2*O99/B99</f>
+        <f>500*2*O99/B99</f>
         <v>20.554442942619321</v>
       </c>
       <c r="T99" s="4">
-        <f t="shared" ref="T99:T101" si="86">B99/4*P99</f>
+        <f>B99/4*P99</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U99" s="8">
-        <f t="shared" si="80"/>
+        <f>E99*N99</f>
         <v>347.45509900000002</v>
       </c>
       <c r="V99" s="8">
-        <f t="shared" si="81"/>
+        <f>F99*O99</f>
         <v>344.28691928887361</v>
       </c>
       <c r="W99" s="8">
-        <f t="shared" si="82"/>
+        <f>G99*N99</f>
         <v>347.45509900000002</v>
       </c>
       <c r="X99" s="4">
-        <f t="shared" si="83"/>
+        <f>H99*N99</f>
         <v>86.863774750000005</v>
       </c>
     </row>
@@ -16816,35 +17601,35 @@
         <v>3.4423715449099523E-3</v>
       </c>
       <c r="Q100" s="9">
-        <f t="shared" ref="Q100:Q101" si="87">8*(O100/B100)^2</f>
+        <f>8*(O100/B100)^2</f>
         <v>3.4124209425087063E-3</v>
       </c>
       <c r="R100" s="10">
-        <f t="shared" si="84"/>
+        <f>(Q100-P100)/P100</f>
         <v>-8.7005722684212698E-3</v>
       </c>
       <c r="S100" s="8">
-        <f t="shared" si="85"/>
+        <f>500*2*O100/B100</f>
         <v>20.653150312085277</v>
       </c>
       <c r="T100" s="4">
-        <f t="shared" si="86"/>
+        <f>B100/4*P100</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U100" s="8">
-        <f t="shared" si="80"/>
+        <f>E100*N100</f>
         <v>259.29485</v>
       </c>
       <c r="V100" s="8">
-        <f t="shared" si="81"/>
+        <f>F100*O100</f>
         <v>258.16437890106602</v>
       </c>
       <c r="W100" s="8">
-        <f t="shared" si="82"/>
+        <f>G100*N100</f>
         <v>259.29485</v>
       </c>
       <c r="X100" s="4">
-        <f t="shared" si="83"/>
+        <f>H100*N100</f>
         <v>64.823712499999999</v>
       </c>
     </row>
@@ -16902,233 +17687,927 @@
         <v>3.4423715449099523E-3</v>
       </c>
       <c r="Q101" s="9">
-        <f t="shared" si="87"/>
+        <f>8*(O101/B101)^2</f>
         <v>3.394458537609322E-3</v>
       </c>
       <c r="R101" s="10">
-        <f t="shared" si="84"/>
+        <f>(Q101-P101)/P101</f>
         <v>-1.391860427485715E-2</v>
       </c>
       <c r="S101" s="8">
-        <f t="shared" si="85"/>
+        <f>500*2*O101/B101</f>
         <v>20.598721251601159</v>
       </c>
       <c r="T101" s="4">
-        <f t="shared" si="86"/>
+        <f>B101/4*P101</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U101" s="8">
-        <f t="shared" si="80"/>
+        <f>E101*N101</f>
         <v>171.134601</v>
       </c>
       <c r="V101" s="8">
-        <f t="shared" si="81"/>
+        <f>F101*O101</f>
         <v>169.93945032570957</v>
       </c>
       <c r="W101" s="8">
-        <f t="shared" si="82"/>
+        <f>G101*N101</f>
         <v>171.134601</v>
       </c>
       <c r="X101" s="4">
-        <f t="shared" si="83"/>
+        <f>H101*N101</f>
         <v>42.783650250000001</v>
       </c>
     </row>
+    <row r="103" spans="1:24">
+      <c r="A103" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="104" spans="1:24">
+      <c r="A104" t="s">
+        <v>204</v>
+      </c>
+      <c r="B104" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E104" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F104" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G104">
+        <f>F104</f>
+        <v>0.1</v>
+      </c>
+      <c r="H104" s="5">
+        <f>0.25*G104</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I104" s="5">
+        <v>1</v>
+      </c>
+      <c r="J104" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K104" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L104">
+        <v>0.1</v>
+      </c>
+      <c r="M104" s="8">
+        <f>L104/H104</f>
+        <v>4</v>
+      </c>
+      <c r="N104" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O104" s="16">
+        <v>5223.4826079345203</v>
+      </c>
+      <c r="P104">
+        <f>8*(N104/B104)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q104" s="9">
+        <f>8*(O104/B104)^2</f>
+        <v>3.4924506310904852E-3</v>
+      </c>
+      <c r="R104" s="10">
+        <f>(Q104-P104)/P104</f>
+        <v>1.4547844567964248E-2</v>
+      </c>
+      <c r="S104" s="8">
+        <f>500*2*O104/B104</f>
+        <v>20.893930431738081</v>
+      </c>
+      <c r="T104" s="4">
+        <f>B104/4*P104</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U104" s="8">
+        <f>E104*N104</f>
+        <v>518.58969999999999</v>
+      </c>
+      <c r="V104" s="8">
+        <f>F104*O104</f>
+        <v>522.34826079345203</v>
+      </c>
+      <c r="W104" s="8">
+        <f>G104*N104</f>
+        <v>518.58969999999999</v>
+      </c>
+      <c r="X104" s="4">
+        <f>H104*N104</f>
+        <v>129.647425</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24">
+      <c r="A105" t="s">
+        <v>204</v>
+      </c>
+      <c r="B105" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E105" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F105" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G105">
+        <f>F105</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H105" s="5">
+        <f>0.25*G105</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I105" s="5">
+        <v>1</v>
+      </c>
+      <c r="J105" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K105" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L105">
+        <v>0.1</v>
+      </c>
+      <c r="M105" s="8">
+        <f>L105/H105</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N105" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O105" s="16">
+        <v>5221.7433220266303</v>
+      </c>
+      <c r="P105">
+        <f>8*(N105/B105)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q105" s="9">
+        <f>8*(O105/B105)^2</f>
+        <v>3.4901252251046027E-3</v>
+      </c>
+      <c r="R105" s="10">
+        <f>(Q105-P105)/P105</f>
+        <v>1.3872320164062809E-2</v>
+      </c>
+      <c r="S105" s="8">
+        <f>500*2*O105/B105</f>
+        <v>20.886973288106521</v>
+      </c>
+      <c r="T105" s="4">
+        <f>B105/4*P105</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U105" s="8">
+        <f>E105*N105</f>
+        <v>347.45509900000002</v>
+      </c>
+      <c r="V105" s="8">
+        <f>F105*O105</f>
+        <v>349.85680257578423</v>
+      </c>
+      <c r="W105" s="8">
+        <f>G105*N105</f>
+        <v>347.45509900000002</v>
+      </c>
+      <c r="X105" s="4">
+        <f>H105*N105</f>
+        <v>86.863774750000005</v>
+      </c>
+    </row>
+    <row r="106" spans="1:24">
+      <c r="A106" t="s">
+        <v>204</v>
+      </c>
+      <c r="B106" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E106" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F106" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G106">
+        <f>F106</f>
+        <v>0.05</v>
+      </c>
+      <c r="H106" s="5">
+        <f>0.25*G106</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I106" s="5">
+        <v>1</v>
+      </c>
+      <c r="J106" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K106" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L106">
+        <v>0.1</v>
+      </c>
+      <c r="M106" s="8">
+        <f>L106/H106</f>
+        <v>8</v>
+      </c>
+      <c r="N106" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O106" s="16">
+        <v>5237.8650971100296</v>
+      </c>
+      <c r="P106">
+        <f>8*(N106/B106)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q106" s="9">
+        <f>8*(O106/B106)^2</f>
+        <v>3.511709539267003E-3</v>
+      </c>
+      <c r="R106" s="10">
+        <f>(Q106-P106)/P106</f>
+        <v>2.0142507411664224E-2</v>
+      </c>
+      <c r="S106" s="8">
+        <f>500*2*O106/B106</f>
+        <v>20.951460388440118</v>
+      </c>
+      <c r="T106" s="4">
+        <f>B106/4*P106</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U106" s="8">
+        <f>E106*N106</f>
+        <v>259.29485</v>
+      </c>
+      <c r="V106" s="8">
+        <f>F106*O106</f>
+        <v>261.89325485550148</v>
+      </c>
+      <c r="W106" s="8">
+        <f>G106*N106</f>
+        <v>259.29485</v>
+      </c>
+      <c r="X106" s="4">
+        <f>H106*N106</f>
+        <v>64.823712499999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24">
+      <c r="A107" t="s">
+        <v>204</v>
+      </c>
+      <c r="B107" s="5">
+        <v>250000</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E107" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F107" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G107">
+        <f>F107</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H107" s="5">
+        <f>0.25*G107</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I107" s="5">
+        <v>1</v>
+      </c>
+      <c r="J107" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K107" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L107">
+        <v>0.1</v>
+      </c>
+      <c r="M107" s="8">
+        <f>L107/H107</f>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N107" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O107" s="16">
+        <v>5211.7641765039198</v>
+      </c>
+      <c r="P107">
+        <f>8*(N107/B107)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q107" s="9">
+        <f>8*(O107/B107)^2</f>
+        <v>3.4767981864306666E-3</v>
+      </c>
+      <c r="R107" s="10">
+        <f>(Q107-P107)/P107</f>
+        <v>1.0000850016210226E-2</v>
+      </c>
+      <c r="S107" s="8">
+        <f>500*2*O107/B107</f>
+        <v>20.847056706015682</v>
+      </c>
+      <c r="T107" s="4">
+        <f>B107/4*P107</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U107" s="8">
+        <f>E107*N107</f>
+        <v>171.134601</v>
+      </c>
+      <c r="V107" s="8">
+        <f>F107*O107</f>
+        <v>171.98821782462937</v>
+      </c>
+      <c r="W107" s="8">
+        <f>G107*N107</f>
+        <v>171.134601</v>
+      </c>
+      <c r="X107" s="4">
+        <f>H107*N107</f>
+        <v>42.783650250000001</v>
+      </c>
+    </row>
     <row r="110" spans="1:24">
-      <c r="A110" s="5">
+      <c r="A110" t="s">
+        <v>161</v>
+      </c>
+      <c r="B110" s="5">
         <v>250000</v>
       </c>
-      <c r="B110" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C110" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D110" s="5">
-        <v>0.2</v>
+        <v>158</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="E110" s="5">
         <v>0.1</v>
       </c>
-      <c r="F110">
-        <v>0.1</v>
-      </c>
-      <c r="G110" s="5">
-        <f>0.25*F110</f>
+      <c r="F110" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G110">
+        <f>F110</f>
+        <v>0.1</v>
+      </c>
+      <c r="H110" s="5">
+        <f>0.25*G110</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="H110" s="5">
-        <v>2</v>
-      </c>
-      <c r="I110" s="5" t="s">
+      <c r="I110" s="5">
+        <v>1</v>
+      </c>
+      <c r="J110" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J110" s="5" t="s">
+      <c r="K110" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K110">
-        <v>0.1</v>
-      </c>
-      <c r="L110" s="8">
-        <f>K110/G110</f>
+      <c r="L110">
+        <v>0.1</v>
+      </c>
+      <c r="M110" s="8">
+        <f>L110/H110</f>
         <v>4</v>
       </c>
-      <c r="M110" s="8">
+      <c r="N110" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O110">
-        <f>8*(M110/A110)^2</f>
+      <c r="O110" s="16">
+        <v>2743.1537675531599</v>
+      </c>
+      <c r="P110">
+        <f>8*(N110/B110)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
+      <c r="Q110" s="9">
+        <f>8*(O110/B110)^2</f>
+        <v>9.6318625183246015E-4</v>
+      </c>
+      <c r="R110" s="10">
+        <f>(Q110-P110)/P110</f>
+        <v>-0.72019689354663896</v>
+      </c>
+      <c r="S110" s="8">
+        <f>500*2*O110/B110</f>
+        <v>10.97261507021264</v>
+      </c>
+      <c r="T110" s="4">
+        <f>B110/4*P110</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U110" s="8">
+        <f t="shared" ref="U110:U113" si="56">E110*N110</f>
+        <v>518.58969999999999</v>
+      </c>
+      <c r="V110" s="8">
+        <f t="shared" ref="V110:V113" si="57">F110*O110</f>
+        <v>274.31537675531598</v>
+      </c>
+      <c r="W110" s="8">
+        <f t="shared" ref="W110:W113" si="58">G110*N110</f>
+        <v>518.58969999999999</v>
+      </c>
+      <c r="X110" s="4">
+        <f t="shared" ref="X110:X113" si="59">H110*N110</f>
+        <v>129.647425</v>
+      </c>
     </row>
     <row r="111" spans="1:24">
-      <c r="A111" s="5">
+      <c r="A111" t="s">
+        <v>161</v>
+      </c>
+      <c r="B111" s="5">
         <v>250000</v>
       </c>
-      <c r="B111" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C111" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D111" s="5">
-        <f>E111*2</f>
-        <v>0.13400000000000001</v>
+        <v>158</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>209</v>
       </c>
       <c r="E111" s="5">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="F111">
-        <f>E111</f>
+      <c r="F111" s="5">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="G111" s="5">
-        <f>0.25*F111</f>
+      <c r="G111">
+        <f>F111</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H111" s="5">
+        <f>0.25*G111</f>
         <v>1.6750000000000001E-2</v>
       </c>
-      <c r="H111" s="5">
-        <v>2</v>
-      </c>
-      <c r="I111" s="5" t="s">
+      <c r="I111" s="5">
+        <v>1</v>
+      </c>
+      <c r="J111" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J111" s="5" t="s">
+      <c r="K111" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K111">
-        <v>0.1</v>
-      </c>
-      <c r="L111" s="8">
-        <f>K111/G111</f>
+      <c r="L111">
+        <v>0.1</v>
+      </c>
+      <c r="M111" s="8">
+        <f>L111/H111</f>
         <v>5.9701492537313436</v>
       </c>
-      <c r="M111" s="8">
+      <c r="N111" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O111">
-        <f>8*(M111/A111)^2</f>
+      <c r="O111" s="16">
+        <v>3268.0035118168398</v>
+      </c>
+      <c r="P111">
+        <f>8*(N111/B111)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
+      <c r="Q111" s="9">
+        <f>8*(O111/B111)^2</f>
+        <v>1.3670204100156415E-3</v>
+      </c>
+      <c r="R111" s="10">
+        <f>(Q111-P111)/P111</f>
+        <v>-0.60288411864286395</v>
+      </c>
+      <c r="S111" s="8">
+        <f>500*2*O111/B111</f>
+        <v>13.072014047267359</v>
+      </c>
+      <c r="T111" s="4">
+        <f>B111/4*P111</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U111" s="8">
+        <f t="shared" si="56"/>
+        <v>347.45509900000002</v>
+      </c>
+      <c r="V111" s="8">
+        <f t="shared" si="57"/>
+        <v>218.95623529172829</v>
+      </c>
+      <c r="W111" s="8">
+        <f t="shared" si="58"/>
+        <v>347.45509900000002</v>
+      </c>
+      <c r="X111" s="4">
+        <f t="shared" si="59"/>
+        <v>86.863774750000005</v>
+      </c>
     </row>
     <row r="112" spans="1:24">
-      <c r="A112" s="5">
+      <c r="A112" t="s">
+        <v>161</v>
+      </c>
+      <c r="B112" s="5">
         <v>250000</v>
       </c>
-      <c r="B112" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C112" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D112" s="5">
-        <f t="shared" ref="D112:D113" si="88">E112*2</f>
-        <v>0.1</v>
+        <v>158</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>210</v>
       </c>
       <c r="E112" s="5">
         <v>0.05</v>
       </c>
-      <c r="F112">
-        <f>E112</f>
+      <c r="F112" s="5">
         <v>0.05</v>
       </c>
-      <c r="G112" s="5">
-        <f>0.25*F112</f>
+      <c r="G112">
+        <f>F112</f>
+        <v>0.05</v>
+      </c>
+      <c r="H112" s="5">
+        <f>0.25*G112</f>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="H112" s="5">
-        <v>2</v>
-      </c>
-      <c r="I112" s="5" t="s">
+      <c r="I112" s="5">
+        <v>1</v>
+      </c>
+      <c r="J112" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J112" s="5" t="s">
+      <c r="K112" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K112">
-        <v>0.1</v>
-      </c>
-      <c r="L112" s="8">
-        <f>K112/G112</f>
+      <c r="L112">
+        <v>0.1</v>
+      </c>
+      <c r="M112" s="8">
+        <f>L112/H112</f>
         <v>8</v>
       </c>
-      <c r="M112" s="8">
+      <c r="N112" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O112">
-        <f>8*(M112/A112)^2</f>
+      <c r="O112" s="16">
+        <v>3655.12521174326</v>
+      </c>
+      <c r="P112">
+        <f>8*(N112/B112)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
-    </row>
-    <row r="113" spans="1:15">
-      <c r="A113" s="5">
+      <c r="Q112" s="9">
+        <f>8*(O112/B112)^2</f>
+        <v>1.7100723601307152E-3</v>
+      </c>
+      <c r="R112" s="10">
+        <f>(Q112-P112)/P112</f>
+        <v>-0.50322841743817393</v>
+      </c>
+      <c r="S112" s="8">
+        <f>500*2*O112/B112</f>
+        <v>14.620500846973039</v>
+      </c>
+      <c r="T112" s="4">
+        <f>B112/4*P112</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U112" s="8">
+        <f t="shared" si="56"/>
+        <v>259.29485</v>
+      </c>
+      <c r="V112" s="8">
+        <f t="shared" si="57"/>
+        <v>182.75626058716301</v>
+      </c>
+      <c r="W112" s="8">
+        <f t="shared" si="58"/>
+        <v>259.29485</v>
+      </c>
+      <c r="X112" s="4">
+        <f t="shared" si="59"/>
+        <v>64.823712499999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24">
+      <c r="A113" t="s">
+        <v>161</v>
+      </c>
+      <c r="B113" s="5">
         <v>250000</v>
       </c>
-      <c r="B113" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C113" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D113" s="5">
-        <f t="shared" si="88"/>
-        <v>6.6000000000000003E-2</v>
+        <v>158</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>211</v>
       </c>
       <c r="E113" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="F113">
-        <f>E113</f>
+      <c r="F113" s="5">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="G113" s="5">
-        <f>0.25*F113</f>
+      <c r="G113">
+        <f>F113</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H113" s="5">
+        <f>0.25*G113</f>
         <v>8.2500000000000004E-3</v>
       </c>
-      <c r="H113" s="5">
+      <c r="I113" s="5">
+        <v>1</v>
+      </c>
+      <c r="J113" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K113" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L113">
+        <v>0.1</v>
+      </c>
+      <c r="M113" s="8">
+        <f>L113/H113</f>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N113" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O113" s="16">
+        <v>4182.8312077934797</v>
+      </c>
+      <c r="P113">
+        <f>8*(N113/B113)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q113" s="9">
+        <f>8*(O113/B113)^2</f>
+        <v>2.2394978448500562E-3</v>
+      </c>
+      <c r="R113" s="10">
+        <f>(Q113-P113)/P113</f>
+        <v>-0.34943168811586306</v>
+      </c>
+      <c r="S113" s="8">
+        <f>500*2*O113/B113</f>
+        <v>16.731324831173918</v>
+      </c>
+      <c r="T113" s="4">
+        <f>B113/4*P113</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U113" s="8">
+        <f t="shared" si="56"/>
+        <v>171.134601</v>
+      </c>
+      <c r="V113" s="8">
+        <f t="shared" si="57"/>
+        <v>138.03342985718484</v>
+      </c>
+      <c r="W113" s="8">
+        <f t="shared" si="58"/>
+        <v>171.134601</v>
+      </c>
+      <c r="X113" s="4">
+        <f t="shared" si="59"/>
+        <v>42.783650250000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15">
+      <c r="A131" s="5">
+        <v>250000</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D131" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E131" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F131">
+        <v>0.1</v>
+      </c>
+      <c r="G131" s="5">
+        <f>0.25*F131</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H131" s="5">
         <v>2</v>
       </c>
-      <c r="I113" s="5" t="s">
+      <c r="I131" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J113" s="5" t="s">
+      <c r="J131" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K113">
-        <v>0.1</v>
-      </c>
-      <c r="L113" s="8">
-        <f>K113/G113</f>
+      <c r="K131">
+        <v>0.1</v>
+      </c>
+      <c r="L131" s="8">
+        <f>K131/G131</f>
+        <v>4</v>
+      </c>
+      <c r="M131" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O131">
+        <f>8*(M131/A131)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15">
+      <c r="A132" s="5">
+        <v>250000</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D132" s="5">
+        <f>E132*2</f>
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="E132" s="5">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F132">
+        <f>E132</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G132" s="5">
+        <f>0.25*F132</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="H132" s="5">
+        <v>2</v>
+      </c>
+      <c r="I132" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J132" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K132">
+        <v>0.1</v>
+      </c>
+      <c r="L132" s="8">
+        <f>K132/G132</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="M132" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O132">
+        <f>8*(M132/A132)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15">
+      <c r="A133" s="5">
+        <v>250000</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D133" s="5">
+        <f t="shared" ref="D133:D134" si="60">E133*2</f>
+        <v>0.1</v>
+      </c>
+      <c r="E133" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F133">
+        <f>E133</f>
+        <v>0.05</v>
+      </c>
+      <c r="G133" s="5">
+        <f>0.25*F133</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="H133" s="5">
+        <v>2</v>
+      </c>
+      <c r="I133" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J133" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K133">
+        <v>0.1</v>
+      </c>
+      <c r="L133" s="8">
+        <f>K133/G133</f>
+        <v>8</v>
+      </c>
+      <c r="M133" s="8">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O133">
+        <f>8*(M133/A133)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15">
+      <c r="A134" s="5">
+        <v>250000</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D134" s="5">
+        <f t="shared" si="60"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="E134" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F134">
+        <f>E134</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G134" s="5">
+        <f>0.25*F134</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="H134" s="5">
+        <v>2</v>
+      </c>
+      <c r="I134" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J134" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K134">
+        <v>0.1</v>
+      </c>
+      <c r="L134" s="8">
+        <f>K134/G134</f>
         <v>12.121212121212121</v>
       </c>
-      <c r="M113" s="8">
+      <c r="M134" s="8">
         <v>5185.8969999999999</v>
       </c>
-      <c r="O113">
-        <f>8*(M113/A113)^2</f>
+      <c r="O134">
+        <f>8*(M134/A134)^2</f>
         <v>3.4423715449099523E-3</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
postprocessing codes added to utils
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCFC761-1F09-4012-8DD2-872D2F7FA2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8ECCC7-B46A-449C-8531-639A60FC0344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="7" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="4" activeTab="8" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="CHA_RETAU1000" sheetId="4" r:id="rId6"/>
     <sheet name="CHA_RETAU5200" sheetId="6" r:id="rId7"/>
     <sheet name="DUC_RETAU150" sheetId="11" r:id="rId8"/>
+    <sheet name="DUC_RETAU1000" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="221">
   <si>
     <t>nompi</t>
   </si>
@@ -692,6 +693,42 @@
   </si>
   <si>
     <t>WM+DSMAG+SMALL</t>
+  </si>
+  <si>
+    <t>DNS+SMALL</t>
+  </si>
+  <si>
+    <t>12.8×2.0×2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 384×128×128</t>
+  </si>
+  <si>
+    <t>dz_w=dy</t>
+  </si>
+  <si>
+    <t>uniform</t>
+  </si>
+  <si>
+    <t>6.4×2.0×2.0</t>
+  </si>
+  <si>
+    <t>DNS+REFINE</t>
+  </si>
+  <si>
+    <t>256×80×80</t>
+  </si>
+  <si>
+    <t>128×80×80</t>
+  </si>
+  <si>
+    <t>64×80×80</t>
+  </si>
+  <si>
+    <t>384×120×120</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 576×192×192</t>
   </si>
 </sst>
 </file>
@@ -1930,7 +1967,7 @@
   <dimension ref="A1:X59"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4409,7 +4446,7 @@
   <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5796,7 +5833,7 @@
   <dimension ref="A1:X58"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:R23"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11620,8 +11657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42F51E-90FA-449F-904F-669D9897EDC7}">
   <dimension ref="A1:X134"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N90" sqref="N90"/>
+    <sheetView topLeftCell="A49" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18623,14 +18660,798 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455609CC-CB8B-4322-BCD1-DB060831DD3C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" customWidth="1"/>
+    <col min="10" max="10" width="13.36328125" customWidth="1"/>
+    <col min="18" max="18" width="12.26953125" customWidth="1"/>
+    <col min="19" max="19" width="14.90625" customWidth="1"/>
+    <col min="24" max="24" width="10.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="4">
+        <v>4410</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2" s="17">
+        <f>12.8/384</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F2" s="17">
+        <f>2/128</f>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="G2" s="17">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="H2" s="17">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="I2" s="18">
+        <f>E2/F2</f>
+        <v>2.1333333333333333</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="N2" s="11">
+        <v>150</v>
+      </c>
+      <c r="O2" s="3">
+        <v>148.846405200954</v>
+      </c>
+      <c r="P2" s="8">
+        <f>8*(N2/B2)^2</f>
+        <v>9.2554028414086748E-3</v>
+      </c>
+      <c r="Q2" s="8">
+        <f>8*(O2/B2)^2</f>
+        <v>9.1135904653911019E-3</v>
+      </c>
+      <c r="R2" s="9">
+        <f>(Q2-P2)/P2</f>
+        <v>-1.5322118166818652E-2</v>
+      </c>
+      <c r="S2" s="7">
+        <f>3300*2*O2/B2</f>
+        <v>222.76332751163184</v>
+      </c>
+      <c r="T2" s="3">
+        <f>B2/4*P2</f>
+        <v>10.204081632653065</v>
+      </c>
+      <c r="U2" s="7">
+        <f>E2*N2</f>
+        <v>5</v>
+      </c>
+      <c r="V2" s="7">
+        <f>F2*N2</f>
+        <v>2.34375</v>
+      </c>
+      <c r="W2" s="7">
+        <f>G2*N2</f>
+        <v>2.34375</v>
+      </c>
+      <c r="X2" s="7">
+        <f>H2*N2</f>
+        <v>2.34375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" s="4">
+        <v>4410</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E3" s="17">
+        <f>12.8/576</f>
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="F3" s="17">
+        <f>2/192</f>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="G3" s="17">
+        <f>2/192</f>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H3" s="17">
+        <f>2/192</f>
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="I3" s="18">
+        <f>E3/F3</f>
+        <v>2.1333333333333337</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="N3" s="11">
+        <v>150</v>
+      </c>
+      <c r="O3" s="3">
+        <v>149.041431015104</v>
+      </c>
+      <c r="P3" s="8">
+        <f>8*(N3/B3)^2</f>
+        <v>9.2554028414086748E-3</v>
+      </c>
+      <c r="Q3" s="8">
+        <f>8*(O3/B3)^2</f>
+        <v>9.1374882519238403E-3</v>
+      </c>
+      <c r="R3" s="9">
+        <f>(Q3-P3)/P3</f>
+        <v>-1.2740081820888932E-2</v>
+      </c>
+      <c r="S3" s="7">
+        <f>700*2*O3/B3</f>
+        <v>47.31474000479492</v>
+      </c>
+      <c r="T3" s="3">
+        <f>B3/4*P3</f>
+        <v>10.204081632653065</v>
+      </c>
+      <c r="U3" s="7">
+        <f>E3*N3</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="V3" s="7">
+        <f>F3*N3</f>
+        <v>1.5625</v>
+      </c>
+      <c r="W3" s="7">
+        <f>G3*N3</f>
+        <v>1.5625</v>
+      </c>
+      <c r="X3" s="7">
+        <f>H3*N3</f>
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" s="4">
+        <v>4410</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E4" s="17">
+        <f>12.8/384</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F4" s="17">
+        <f>2/128</f>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="G4" s="17">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="H4" s="17">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="I4" s="18">
+        <f>E4/F4</f>
+        <v>2.1333333333333333</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="N4" s="11">
+        <v>150</v>
+      </c>
+      <c r="O4" s="3">
+        <v>148.48689957656501</v>
+      </c>
+      <c r="P4" s="8">
+        <f>8*(N4/B4)^2</f>
+        <v>9.2554028414086748E-3</v>
+      </c>
+      <c r="Q4" s="8">
+        <f>8*(O4/B4)^2</f>
+        <v>9.0696198994702441E-3</v>
+      </c>
+      <c r="R4" s="9">
+        <f>(Q4-P4)/P4</f>
+        <v>-2.0072917961737737E-2</v>
+      </c>
+      <c r="S4" s="7">
+        <f>4500*2*O4/B4</f>
+        <v>303.03448893176534</v>
+      </c>
+      <c r="T4" s="3">
+        <f>B4/4*P4</f>
+        <v>10.204081632653065</v>
+      </c>
+      <c r="U4" s="7">
+        <f>E4*N4</f>
+        <v>5</v>
+      </c>
+      <c r="V4" s="7">
+        <f>F4*N4</f>
+        <v>2.34375</v>
+      </c>
+      <c r="W4" s="7">
+        <f>G4*N4</f>
+        <v>2.34375</v>
+      </c>
+      <c r="X4" s="7">
+        <f>H4*N4</f>
+        <v>2.34375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE85DC12-DB96-414E-A0EA-58380D3D2CE8}">
+  <dimension ref="A1:X5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
+    <col min="18" max="18" width="13.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="4">
+        <v>40000</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" s="17">
+        <f>6.4/256</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F2" s="4">
+        <f>2/80</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G2" s="17">
+        <f>2/80</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H2" s="17">
+        <f>2/80</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I2" s="18">
+        <v>1</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="N2" s="11">
+        <v>1055</v>
+      </c>
+      <c r="O2" s="3">
+        <v>1038.48230917147</v>
+      </c>
+      <c r="P2" s="8">
+        <f>8*(N2/B2)^2</f>
+        <v>5.5651249999999998E-3</v>
+      </c>
+      <c r="Q2" s="8">
+        <f>8*(O2/B2)^2</f>
+        <v>5.3922275323105423E-3</v>
+      </c>
+      <c r="R2" s="9">
+        <f>(Q2-P2)/P2</f>
+        <v>-3.106802950328294E-2</v>
+      </c>
+      <c r="S2" s="7">
+        <f>1700*O2/B2</f>
+        <v>44.135498139787479</v>
+      </c>
+      <c r="T2" s="3">
+        <f>B2/4*P2</f>
+        <v>55.651249999999997</v>
+      </c>
+      <c r="U2" s="7">
+        <f>E2*N2</f>
+        <v>26.375</v>
+      </c>
+      <c r="V2" s="7">
+        <f>F2*N2</f>
+        <v>26.375</v>
+      </c>
+      <c r="W2" s="7">
+        <f>G2*N2</f>
+        <v>26.375</v>
+      </c>
+      <c r="X2" s="7">
+        <f>H2*N2</f>
+        <v>26.375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="4">
+        <v>40000</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="17">
+        <f>6.4/128</f>
+        <v>0.05</v>
+      </c>
+      <c r="F3" s="4">
+        <f>2/80</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G3" s="17">
+        <f>2/80</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H3" s="17">
+        <f>2/80</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I3" s="18">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="N3" s="11">
+        <v>1055</v>
+      </c>
+      <c r="O3" s="3">
+        <v>1046.3668774222201</v>
+      </c>
+      <c r="P3" s="8">
+        <f>8*(N3/B3)^2</f>
+        <v>5.5651249999999998E-3</v>
+      </c>
+      <c r="Q3" s="8">
+        <f>8*(O3/B3)^2</f>
+        <v>5.4744182108316369E-3</v>
+      </c>
+      <c r="R3" s="9">
+        <f>(Q3-P3)/P3</f>
+        <v>-1.6299146769994007E-2</v>
+      </c>
+      <c r="S3" s="7">
+        <f>1700*O3/B3</f>
+        <v>44.470592290444351</v>
+      </c>
+      <c r="T3" s="3">
+        <f>B3/4*P3</f>
+        <v>55.651249999999997</v>
+      </c>
+      <c r="U3" s="7">
+        <f>E3*N3</f>
+        <v>52.75</v>
+      </c>
+      <c r="V3" s="7">
+        <f>F3*N3</f>
+        <v>26.375</v>
+      </c>
+      <c r="W3" s="7">
+        <f>G3*N3</f>
+        <v>26.375</v>
+      </c>
+      <c r="X3" s="7">
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="4">
+        <v>40000</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E4" s="17">
+        <f>6.4/64</f>
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="4">
+        <f>2/80</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G4" s="17">
+        <f>2/80</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H4" s="17">
+        <f>2/80</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I4" s="18">
+        <v>4</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="N4" s="11">
+        <v>1055</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1065.6540405542701</v>
+      </c>
+      <c r="P4" s="8">
+        <f>8*(N4/B4)^2</f>
+        <v>5.5651249999999998E-3</v>
+      </c>
+      <c r="Q4" s="8">
+        <f>8*(O4/B4)^2</f>
+        <v>5.6780926707482096E-3</v>
+      </c>
+      <c r="R4" s="9">
+        <f>(Q4-P4)/P4</f>
+        <v>2.0299215336261067E-2</v>
+      </c>
+      <c r="S4" s="7">
+        <f>1700*O4/B4</f>
+        <v>45.29029672355648</v>
+      </c>
+      <c r="T4" s="3">
+        <f>B4/4*P4</f>
+        <v>55.651249999999997</v>
+      </c>
+      <c r="U4" s="7">
+        <f>E4*N4</f>
+        <v>105.5</v>
+      </c>
+      <c r="V4" s="7">
+        <f>F4*N4</f>
+        <v>26.375</v>
+      </c>
+      <c r="W4" s="7">
+        <f>G4*N4</f>
+        <v>26.375</v>
+      </c>
+      <c r="X4" s="7">
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="4">
+        <v>40000</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E5" s="17">
+        <f>6.4/384</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="F5" s="17">
+        <f>2/120</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="G5" s="17">
+        <f>2/120</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="H5" s="17">
+        <f>2/120</f>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="I5" s="18">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="N5" s="11">
+        <v>1055</v>
+      </c>
+      <c r="O5" s="3">
+        <v>1043.4815598084899</v>
+      </c>
+      <c r="P5" s="8">
+        <f>8*(N5/B5)^2</f>
+        <v>5.5651249999999998E-3</v>
+      </c>
+      <c r="Q5" s="8">
+        <f>8*(O5/B5)^2</f>
+        <v>5.4442688283017964E-3</v>
+      </c>
+      <c r="R5" s="9">
+        <f>(Q5-P5)/P5</f>
+        <v>-2.1716703883237719E-2</v>
+      </c>
+      <c r="S5" s="7">
+        <f>1700*O5/B5</f>
+        <v>44.347966291860821</v>
+      </c>
+      <c r="T5" s="3">
+        <f>B5/4*P5</f>
+        <v>55.651249999999997</v>
+      </c>
+      <c r="U5" s="7">
+        <f>E5*N5</f>
+        <v>17.583333333333332</v>
+      </c>
+      <c r="V5" s="7">
+        <f>F5*N5</f>
+        <v>17.583333333333332</v>
+      </c>
+      <c r="W5" s="7">
+        <f>G5*N5</f>
+        <v>17.583333333333332</v>
+      </c>
+      <c r="X5" s="7">
+        <f>H5*N5</f>
+        <v>17.583333333333332</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
multiple moving walls supported
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maoch\OneDrive - uniroma1.it\Documents\code\CaNS\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mchao\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7600AB8-D293-4ABF-9BDA-320015F38BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976C446C-A481-4511-8075-CE0FB29D73A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="6" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="3" activeTab="6" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="223">
   <si>
     <t>nompi</t>
   </si>
@@ -732,6 +732,9 @@
   </si>
   <si>
     <t>512×160×160</t>
+  </si>
+  <si>
+    <t>WM+SMAG+SMALL+MOV</t>
   </si>
 </sst>
 </file>
@@ -1970,12 +1973,13 @@
   <dimension ref="A1:X59"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
     <col min="3" max="3" width="15.6328125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="11.08984375" customWidth="1"/>
@@ -8770,7 +8774,7 @@
         <v>1.094476E-3</v>
       </c>
       <c r="I44" s="18">
-        <f t="shared" ref="I44:I45" si="62">E44/F44</f>
+        <f t="shared" ref="I44" si="62">E44/F44</f>
         <v>1.7777777777777779</v>
       </c>
       <c r="J44" s="4" t="s">
@@ -8792,15 +8796,15 @@
         <v>549.31194168112302</v>
       </c>
       <c r="P44" s="8">
-        <f t="shared" ref="P44:P45" si="63">8*(N44/B44)^2</f>
+        <f t="shared" ref="P44" si="63">8*(N44/B44)^2</f>
         <v>5.772630931736967E-3</v>
       </c>
       <c r="Q44" s="8">
-        <f t="shared" ref="Q44:Q45" si="64">8*(O44/B44)^2</f>
+        <f t="shared" ref="Q44" si="64">8*(O44/B44)^2</f>
         <v>5.721727747572799E-3</v>
       </c>
       <c r="R44" s="9">
-        <f t="shared" ref="R44:R45" si="65">(Q44-P44)/P44</f>
+        <f t="shared" ref="R44" si="65">(Q44-P44)/P44</f>
         <v>-8.8180215860173463E-3</v>
       </c>
       <c r="S44" s="7">
@@ -8808,23 +8812,23 @@
         <v>10.69740879612703</v>
       </c>
       <c r="T44" s="3">
-        <f t="shared" ref="T44:T45" si="66">B44/4*P44</f>
+        <f t="shared" ref="T44" si="66">B44/4*P44</f>
         <v>29.642459834469324</v>
       </c>
       <c r="U44" s="7">
-        <f t="shared" ref="U44:U45" si="67">E44*N44</f>
+        <f t="shared" ref="U44" si="67">E44*N44</f>
         <v>18.391666666666666</v>
       </c>
       <c r="V44" s="7">
-        <f t="shared" ref="V44:V45" si="68">F44*N44</f>
+        <f t="shared" ref="V44" si="68">F44*N44</f>
         <v>10.3453125</v>
       </c>
       <c r="W44" s="7">
-        <f t="shared" ref="W44:W45" si="69">G44*N44</f>
+        <f t="shared" ref="W44" si="69">G44*N44</f>
         <v>21.834044112499999</v>
       </c>
       <c r="X44" s="7">
-        <f t="shared" ref="X44:X45" si="70">H44*N44</f>
+        <f t="shared" ref="X44" si="70">H44*N44</f>
         <v>0.60387713300000001</v>
       </c>
     </row>
@@ -11661,7 +11665,7 @@
   <dimension ref="A1:X134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q96" sqref="Q96"/>
+      <selection activeCell="O125" sqref="O125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16118,11 +16122,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U74" s="7">
-        <f>E74*N74</f>
+        <f t="shared" ref="U74:V77" si="56">E74*N74</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V74" s="7">
-        <f>F74*O74</f>
+        <f t="shared" si="56"/>
         <v>269.73210756077401</v>
       </c>
       <c r="W74" s="7">
@@ -16204,11 +16208,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U75" s="7">
-        <f>E75*N75</f>
+        <f t="shared" si="56"/>
         <v>347.45509900000002</v>
       </c>
       <c r="V75" s="7">
-        <f>F75*O75</f>
+        <f t="shared" si="56"/>
         <v>214.63903361563635</v>
       </c>
       <c r="W75" s="7">
@@ -16290,11 +16294,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U76" s="7">
-        <f>E76*N76</f>
+        <f t="shared" si="56"/>
         <v>259.29485</v>
       </c>
       <c r="V76" s="7">
-        <f>F76*O76</f>
+        <f t="shared" si="56"/>
         <v>179.50305675292401</v>
       </c>
       <c r="W76" s="7">
@@ -16376,11 +16380,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U77" s="7">
-        <f>E77*N77</f>
+        <f t="shared" si="56"/>
         <v>171.134601</v>
       </c>
       <c r="V77" s="7">
-        <f>F77*O77</f>
+        <f t="shared" si="56"/>
         <v>136.72786348482526</v>
       </c>
       <c r="W77" s="7">
@@ -16462,11 +16466,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U80" s="7">
-        <f>E80*N80</f>
+        <f t="shared" ref="U80:V83" si="57">E80*N80</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V80" s="7">
-        <f>F80*O80</f>
+        <f t="shared" si="57"/>
         <v>493.64000411562006</v>
       </c>
       <c r="W80" s="7">
@@ -16548,11 +16552,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U81" s="7">
-        <f>E81*N81</f>
+        <f t="shared" si="57"/>
         <v>347.45509900000002</v>
       </c>
       <c r="V81" s="7">
-        <f>F81*O81</f>
+        <f t="shared" si="57"/>
         <v>341.02759052015813</v>
       </c>
       <c r="W81" s="7">
@@ -16634,11 +16638,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U82" s="7">
-        <f>E82*N82</f>
+        <f t="shared" si="57"/>
         <v>259.29485</v>
       </c>
       <c r="V82" s="7">
-        <f>F82*O82</f>
+        <f t="shared" si="57"/>
         <v>256.28502938309197</v>
       </c>
       <c r="W82" s="7">
@@ -16720,11 +16724,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U83" s="7">
-        <f>E83*N83</f>
+        <f t="shared" si="57"/>
         <v>171.134601</v>
       </c>
       <c r="V83" s="7">
-        <f>F83*O83</f>
+        <f t="shared" si="57"/>
         <v>169.67385445972928</v>
       </c>
       <c r="W83" s="7">
@@ -16806,11 +16810,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U86" s="7">
-        <f>E86*N86</f>
+        <f t="shared" ref="U86:V89" si="58">E86*N86</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V86" s="7">
-        <f>F86*O86</f>
+        <f t="shared" si="58"/>
         <v>490.28200076165808</v>
       </c>
       <c r="W86" s="7">
@@ -16892,11 +16896,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U87" s="7">
-        <f>E87*N87</f>
+        <f t="shared" si="58"/>
         <v>347.45509900000002</v>
       </c>
       <c r="V87" s="7">
-        <f>F87*O87</f>
+        <f t="shared" si="58"/>
         <v>340.19824326573604</v>
       </c>
       <c r="W87" s="7">
@@ -16978,11 +16982,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U88" s="7">
-        <f>E88*N88</f>
+        <f t="shared" si="58"/>
         <v>259.29485</v>
       </c>
       <c r="V88" s="7">
-        <f>F88*O88</f>
+        <f t="shared" si="58"/>
         <v>255.86770450034851</v>
       </c>
       <c r="W88" s="7">
@@ -17064,11 +17068,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U89" s="7">
-        <f>E89*N89</f>
+        <f t="shared" si="58"/>
         <v>171.134601</v>
       </c>
       <c r="V89" s="7">
-        <f>F89*O89</f>
+        <f t="shared" si="58"/>
         <v>170.40060880367648</v>
       </c>
       <c r="W89" s="7">
@@ -17150,11 +17154,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U92" s="7">
-        <f>E92*N92</f>
+        <f t="shared" ref="U92:V95" si="59">E92*N92</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V92" s="7">
-        <f>F92*O92</f>
+        <f t="shared" si="59"/>
         <v>516.127964639281</v>
       </c>
       <c r="W92" s="7">
@@ -17236,11 +17240,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U93" s="7">
-        <f>E93*N93</f>
+        <f t="shared" si="59"/>
         <v>347.45509900000002</v>
       </c>
       <c r="V93" s="7">
-        <f>F93*O93</f>
+        <f t="shared" si="59"/>
         <v>344.22200209534759</v>
       </c>
       <c r="W93" s="7">
@@ -17322,11 +17326,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U94" s="7">
-        <f>E94*N94</f>
+        <f t="shared" si="59"/>
         <v>259.29485</v>
       </c>
       <c r="V94" s="7">
-        <f>F94*O94</f>
+        <f t="shared" si="59"/>
         <v>258.7720284110905</v>
       </c>
       <c r="W94" s="7">
@@ -17408,11 +17412,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U95" s="7">
-        <f>E95*N95</f>
+        <f t="shared" si="59"/>
         <v>171.134601</v>
       </c>
       <c r="V95" s="7">
-        <f>F95*O95</f>
+        <f t="shared" si="59"/>
         <v>170.29152585950374</v>
       </c>
       <c r="W95" s="7">
@@ -17494,11 +17498,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U98" s="7">
-        <f>E98*N98</f>
+        <f t="shared" ref="U98:V101" si="60">E98*N98</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V98" s="7">
-        <f>F98*O98</f>
+        <f t="shared" si="60"/>
         <v>515.02287556594104</v>
       </c>
       <c r="W98" s="7">
@@ -17580,11 +17584,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U99" s="7">
-        <f>E99*N99</f>
+        <f t="shared" si="60"/>
         <v>347.45509900000002</v>
       </c>
       <c r="V99" s="7">
-        <f>F99*O99</f>
+        <f t="shared" si="60"/>
         <v>344.28691928887361</v>
       </c>
       <c r="W99" s="7">
@@ -17666,11 +17670,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U100" s="7">
-        <f>E100*N100</f>
+        <f t="shared" si="60"/>
         <v>259.29485</v>
       </c>
       <c r="V100" s="7">
-        <f>F100*O100</f>
+        <f t="shared" si="60"/>
         <v>258.16437890106602</v>
       </c>
       <c r="W100" s="7">
@@ -17752,11 +17756,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U101" s="7">
-        <f>E101*N101</f>
+        <f t="shared" si="60"/>
         <v>171.134601</v>
       </c>
       <c r="V101" s="7">
-        <f>F101*O101</f>
+        <f t="shared" si="60"/>
         <v>169.93945032570957</v>
       </c>
       <c r="W101" s="7">
@@ -17775,7 +17779,7 @@
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B104" s="4">
         <v>250000</v>
@@ -17843,11 +17847,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U104" s="7">
-        <f>E104*N104</f>
+        <f t="shared" ref="U104:V107" si="61">E104*N104</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V104" s="7">
-        <f>F104*O104</f>
+        <f t="shared" si="61"/>
         <v>522.34826079345203</v>
       </c>
       <c r="W104" s="7">
@@ -17861,7 +17865,7 @@
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B105" s="4">
         <v>250000</v>
@@ -17929,11 +17933,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U105" s="7">
-        <f>E105*N105</f>
+        <f t="shared" si="61"/>
         <v>347.45509900000002</v>
       </c>
       <c r="V105" s="7">
-        <f>F105*O105</f>
+        <f t="shared" si="61"/>
         <v>349.85680257578423</v>
       </c>
       <c r="W105" s="7">
@@ -17947,7 +17951,7 @@
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B106" s="4">
         <v>250000</v>
@@ -18015,11 +18019,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U106" s="7">
-        <f>E106*N106</f>
+        <f t="shared" si="61"/>
         <v>259.29485</v>
       </c>
       <c r="V106" s="7">
-        <f>F106*O106</f>
+        <f t="shared" si="61"/>
         <v>261.89325485550148</v>
       </c>
       <c r="W106" s="7">
@@ -18033,7 +18037,7 @@
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B107" s="4">
         <v>250000</v>
@@ -18101,11 +18105,11 @@
         <v>215.14822155687202</v>
       </c>
       <c r="U107" s="7">
-        <f>E107*N107</f>
+        <f t="shared" si="61"/>
         <v>171.134601</v>
       </c>
       <c r="V107" s="7">
-        <f>F107*O107</f>
+        <f t="shared" si="61"/>
         <v>171.98821782462937</v>
       </c>
       <c r="W107" s="7">
@@ -18119,7 +18123,7 @@
     </row>
     <row r="110" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>157</v>
+        <v>200</v>
       </c>
       <c r="B110" s="4">
         <v>250000</v>
@@ -18164,7 +18168,7 @@
         <v>5185.8969999999999</v>
       </c>
       <c r="O110" s="15">
-        <v>2743.1537675531599</v>
+        <v>5151.0393081271804</v>
       </c>
       <c r="P110">
         <f>8*(N110/B110)^2</f>
@@ -18172,40 +18176,40 @@
       </c>
       <c r="Q110" s="8">
         <f>8*(O110/B110)^2</f>
-        <v>9.6318625183246015E-4</v>
+        <v>3.3962503620955319E-3</v>
       </c>
       <c r="R110" s="9">
         <f>(Q110-P110)/P110</f>
-        <v>-0.72019689354663896</v>
+        <v>-1.3398083911836091E-2</v>
       </c>
       <c r="S110" s="7">
         <f>500*2*O110/B110</f>
-        <v>10.97261507021264</v>
+        <v>20.604157232508722</v>
       </c>
       <c r="T110" s="3">
         <f>B110/4*P110</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U110" s="7">
-        <f t="shared" ref="U110:U113" si="56">E110*N110</f>
+        <f t="shared" ref="U110:U113" si="62">E110*N110</f>
         <v>518.58969999999999</v>
       </c>
       <c r="V110" s="7">
-        <f t="shared" ref="V110:V113" si="57">F110*O110</f>
-        <v>274.31537675531598</v>
+        <f t="shared" ref="V110:V113" si="63">F110*O110</f>
+        <v>515.10393081271809</v>
       </c>
       <c r="W110" s="7">
-        <f t="shared" ref="W110:W113" si="58">G110*N110</f>
+        <f>G110*N110</f>
         <v>518.58969999999999</v>
       </c>
       <c r="X110" s="3">
-        <f t="shared" ref="X110:X113" si="59">H110*N110</f>
+        <f>H110*N110</f>
         <v>129.647425</v>
       </c>
     </row>
     <row r="111" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>157</v>
+        <v>200</v>
       </c>
       <c r="B111" s="4">
         <v>250000</v>
@@ -18250,7 +18254,7 @@
         <v>5185.8969999999999</v>
       </c>
       <c r="O111" s="15">
-        <v>3268.0035118168398</v>
+        <v>5156.7697362610397</v>
       </c>
       <c r="P111">
         <f>8*(N111/B111)^2</f>
@@ -18258,40 +18262,40 @@
       </c>
       <c r="Q111" s="8">
         <f>8*(O111/B111)^2</f>
-        <v>1.3670204100156415E-3</v>
+        <v>3.403811086440672E-3</v>
       </c>
       <c r="R111" s="9">
         <f>(Q111-P111)/P111</f>
-        <v>-0.60288411864286395</v>
+        <v>-1.1201713111502323E-2</v>
       </c>
       <c r="S111" s="7">
         <f>500*2*O111/B111</f>
-        <v>13.072014047267359</v>
+        <v>20.627078945044161</v>
       </c>
       <c r="T111" s="3">
         <f>B111/4*P111</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U111" s="7">
-        <f t="shared" si="56"/>
+        <f t="shared" si="62"/>
         <v>347.45509900000002</v>
       </c>
       <c r="V111" s="7">
-        <f t="shared" si="57"/>
-        <v>218.95623529172829</v>
+        <f t="shared" si="63"/>
+        <v>345.50357232948966</v>
       </c>
       <c r="W111" s="7">
-        <f t="shared" si="58"/>
+        <f>G111*N111</f>
         <v>347.45509900000002</v>
       </c>
       <c r="X111" s="3">
-        <f t="shared" si="59"/>
+        <f>H111*N111</f>
         <v>86.863774750000005</v>
       </c>
     </row>
     <row r="112" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>157</v>
+        <v>200</v>
       </c>
       <c r="B112" s="4">
         <v>250000</v>
@@ -18336,7 +18340,7 @@
         <v>5185.8969999999999</v>
       </c>
       <c r="O112" s="15">
-        <v>3655.12521174326</v>
+        <v>5163.6698001868599</v>
       </c>
       <c r="P112">
         <f>8*(N112/B112)^2</f>
@@ -18344,40 +18348,40 @@
       </c>
       <c r="Q112" s="8">
         <f>8*(O112/B112)^2</f>
-        <v>1.7100723601307152E-3</v>
+        <v>3.4129261830863106E-3</v>
       </c>
       <c r="R112" s="9">
         <f>(Q112-P112)/P112</f>
-        <v>-0.50322841743817393</v>
+        <v>-8.5538011918501224E-3</v>
       </c>
       <c r="S112" s="7">
         <f>500*2*O112/B112</f>
-        <v>14.620500846973039</v>
+        <v>20.654679200747438</v>
       </c>
       <c r="T112" s="3">
         <f>B112/4*P112</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U112" s="7">
-        <f t="shared" si="56"/>
+        <f t="shared" si="62"/>
         <v>259.29485</v>
       </c>
       <c r="V112" s="7">
-        <f t="shared" si="57"/>
-        <v>182.75626058716301</v>
+        <f t="shared" si="63"/>
+        <v>258.18349000934302</v>
       </c>
       <c r="W112" s="7">
-        <f t="shared" si="58"/>
+        <f>G112*N112</f>
         <v>259.29485</v>
       </c>
       <c r="X112" s="3">
-        <f t="shared" si="59"/>
+        <f>H112*N112</f>
         <v>64.823712499999999</v>
       </c>
     </row>
     <row r="113" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>157</v>
+        <v>200</v>
       </c>
       <c r="B113" s="4">
         <v>250000</v>
@@ -18422,7 +18426,7 @@
         <v>5185.8969999999999</v>
       </c>
       <c r="O113" s="15">
-        <v>4182.8312077934797</v>
+        <v>5154.3938959526904</v>
       </c>
       <c r="P113">
         <f>8*(N113/B113)^2</f>
@@ -18430,34 +18434,722 @@
       </c>
       <c r="Q113" s="8">
         <f>8*(O113/B113)^2</f>
-        <v>2.2394978448500562E-3</v>
+        <v>3.4006753836331978E-3</v>
       </c>
       <c r="R113" s="9">
         <f>(Q113-P113)/P113</f>
-        <v>-0.34943168811586306</v>
+        <v>-1.2112626639157621E-2</v>
       </c>
       <c r="S113" s="7">
         <f>500*2*O113/B113</f>
-        <v>16.731324831173918</v>
+        <v>20.617575583810762</v>
       </c>
       <c r="T113" s="3">
         <f>B113/4*P113</f>
         <v>215.14822155687202</v>
       </c>
       <c r="U113" s="7">
-        <f t="shared" si="56"/>
+        <f t="shared" si="62"/>
         <v>171.134601</v>
       </c>
       <c r="V113" s="7">
-        <f t="shared" si="57"/>
+        <f t="shared" si="63"/>
+        <v>170.09499856643879</v>
+      </c>
+      <c r="W113" s="7">
+        <f>G113*N113</f>
+        <v>171.134601</v>
+      </c>
+      <c r="X113" s="3">
+        <f>H113*N113</f>
+        <v>42.783650250000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>157</v>
+      </c>
+      <c r="B116" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E116" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="F116" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G116">
+        <f>F116</f>
+        <v>0.1</v>
+      </c>
+      <c r="H116" s="4">
+        <f>0.25*G116</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I116" s="4">
+        <v>1</v>
+      </c>
+      <c r="J116" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K116" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L116">
+        <v>0.1</v>
+      </c>
+      <c r="M116" s="7">
+        <f>L116/H116</f>
+        <v>4</v>
+      </c>
+      <c r="N116" s="7">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O116" s="15">
+        <v>2743.1537675531599</v>
+      </c>
+      <c r="P116">
+        <f>8*(N116/B116)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q116" s="8">
+        <f>8*(O116/B116)^2</f>
+        <v>9.6318625183246015E-4</v>
+      </c>
+      <c r="R116" s="9">
+        <f>(Q116-P116)/P116</f>
+        <v>-0.72019689354663896</v>
+      </c>
+      <c r="S116" s="7">
+        <f>500*2*O116/B116</f>
+        <v>10.97261507021264</v>
+      </c>
+      <c r="T116" s="3">
+        <f>B116/4*P116</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U116" s="7">
+        <f t="shared" ref="U116:U119" si="64">E116*N116</f>
+        <v>518.58969999999999</v>
+      </c>
+      <c r="V116" s="7">
+        <f t="shared" ref="V116:V119" si="65">F116*O116</f>
+        <v>274.31537675531598</v>
+      </c>
+      <c r="W116" s="7">
+        <f t="shared" ref="W116:W119" si="66">G116*N116</f>
+        <v>518.58969999999999</v>
+      </c>
+      <c r="X116" s="3">
+        <f t="shared" ref="X116:X119" si="67">H116*N116</f>
+        <v>129.647425</v>
+      </c>
+    </row>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>157</v>
+      </c>
+      <c r="B117" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E117" s="4">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F117" s="4">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G117">
+        <f>F117</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H117" s="4">
+        <f>0.25*G117</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I117" s="4">
+        <v>1</v>
+      </c>
+      <c r="J117" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K117" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L117">
+        <v>0.1</v>
+      </c>
+      <c r="M117" s="7">
+        <f>L117/H117</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N117" s="7">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O117" s="15">
+        <v>3268.0035118168398</v>
+      </c>
+      <c r="P117">
+        <f>8*(N117/B117)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q117" s="8">
+        <f>8*(O117/B117)^2</f>
+        <v>1.3670204100156415E-3</v>
+      </c>
+      <c r="R117" s="9">
+        <f>(Q117-P117)/P117</f>
+        <v>-0.60288411864286395</v>
+      </c>
+      <c r="S117" s="7">
+        <f>500*2*O117/B117</f>
+        <v>13.072014047267359</v>
+      </c>
+      <c r="T117" s="3">
+        <f>B117/4*P117</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U117" s="7">
+        <f t="shared" si="64"/>
+        <v>347.45509900000002</v>
+      </c>
+      <c r="V117" s="7">
+        <f t="shared" si="65"/>
+        <v>218.95623529172829</v>
+      </c>
+      <c r="W117" s="7">
+        <f t="shared" si="66"/>
+        <v>347.45509900000002</v>
+      </c>
+      <c r="X117" s="3">
+        <f t="shared" si="67"/>
+        <v>86.863774750000005</v>
+      </c>
+    </row>
+    <row r="118" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>157</v>
+      </c>
+      <c r="B118" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E118" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F118" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="G118">
+        <f>F118</f>
+        <v>0.05</v>
+      </c>
+      <c r="H118" s="4">
+        <f>0.25*G118</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I118" s="4">
+        <v>1</v>
+      </c>
+      <c r="J118" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K118" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L118">
+        <v>0.1</v>
+      </c>
+      <c r="M118" s="7">
+        <f>L118/H118</f>
+        <v>8</v>
+      </c>
+      <c r="N118" s="7">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O118" s="15">
+        <v>3655.12521174326</v>
+      </c>
+      <c r="P118">
+        <f>8*(N118/B118)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q118" s="8">
+        <f>8*(O118/B118)^2</f>
+        <v>1.7100723601307152E-3</v>
+      </c>
+      <c r="R118" s="9">
+        <f>(Q118-P118)/P118</f>
+        <v>-0.50322841743817393</v>
+      </c>
+      <c r="S118" s="7">
+        <f>500*2*O118/B118</f>
+        <v>14.620500846973039</v>
+      </c>
+      <c r="T118" s="3">
+        <f>B118/4*P118</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U118" s="7">
+        <f t="shared" si="64"/>
+        <v>259.29485</v>
+      </c>
+      <c r="V118" s="7">
+        <f t="shared" si="65"/>
+        <v>182.75626058716301</v>
+      </c>
+      <c r="W118" s="7">
+        <f t="shared" si="66"/>
+        <v>259.29485</v>
+      </c>
+      <c r="X118" s="3">
+        <f t="shared" si="67"/>
+        <v>64.823712499999999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>157</v>
+      </c>
+      <c r="B119" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E119" s="4">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F119" s="4">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G119">
+        <f>F119</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H119" s="4">
+        <f>0.25*G119</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I119" s="4">
+        <v>1</v>
+      </c>
+      <c r="J119" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K119" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L119">
+        <v>0.1</v>
+      </c>
+      <c r="M119" s="7">
+        <f>L119/H119</f>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N119" s="7">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O119" s="15">
+        <v>4182.8312077934797</v>
+      </c>
+      <c r="P119">
+        <f>8*(N119/B119)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q119" s="8">
+        <f>8*(O119/B119)^2</f>
+        <v>2.2394978448500562E-3</v>
+      </c>
+      <c r="R119" s="9">
+        <f>(Q119-P119)/P119</f>
+        <v>-0.34943168811586306</v>
+      </c>
+      <c r="S119" s="7">
+        <f>500*2*O119/B119</f>
+        <v>16.731324831173918</v>
+      </c>
+      <c r="T119" s="3">
+        <f>B119/4*P119</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U119" s="7">
+        <f t="shared" si="64"/>
+        <v>171.134601</v>
+      </c>
+      <c r="V119" s="7">
+        <f t="shared" si="65"/>
         <v>138.03342985718484</v>
       </c>
-      <c r="W113" s="7">
-        <f t="shared" si="58"/>
+      <c r="W119" s="7">
+        <f t="shared" si="66"/>
         <v>171.134601</v>
       </c>
-      <c r="X113" s="3">
-        <f t="shared" si="59"/>
+      <c r="X119" s="3">
+        <f t="shared" si="67"/>
+        <v>42.783650250000001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>222</v>
+      </c>
+      <c r="B122" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E122" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="F122" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G122">
+        <f>F122</f>
+        <v>0.1</v>
+      </c>
+      <c r="H122" s="4">
+        <f>0.25*G122</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I122" s="4">
+        <v>1</v>
+      </c>
+      <c r="J122" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K122" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L122">
+        <v>0.1</v>
+      </c>
+      <c r="M122" s="7">
+        <f>L122/H122</f>
+        <v>4</v>
+      </c>
+      <c r="N122" s="7">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O122" s="15">
+        <v>4960.6637403888799</v>
+      </c>
+      <c r="P122">
+        <f>8*(N122/B122)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q122" s="8">
+        <f>8*(O122/B122)^2</f>
+        <v>3.1498476473867513E-3</v>
+      </c>
+      <c r="R122" s="9">
+        <f>(Q122-P122)/P122</f>
+        <v>-8.4977433059409344E-2</v>
+      </c>
+      <c r="S122" s="7">
+        <f>500*2*O122/B122</f>
+        <v>19.842654961555517</v>
+      </c>
+      <c r="T122" s="3">
+        <f>B122/4*P122</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U122" s="7">
+        <f t="shared" ref="U122:U125" si="68">E122*N122</f>
+        <v>518.58969999999999</v>
+      </c>
+      <c r="V122" s="7">
+        <f t="shared" ref="V122:V125" si="69">F122*O122</f>
+        <v>496.066374038888</v>
+      </c>
+      <c r="W122" s="7">
+        <f>G122*N122</f>
+        <v>518.58969999999999</v>
+      </c>
+      <c r="X122" s="3">
+        <f>H122*N122</f>
+        <v>129.647425</v>
+      </c>
+    </row>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>222</v>
+      </c>
+      <c r="B123" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="E123" s="4">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="F123" s="4">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="G123">
+        <f>F123</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H123" s="4">
+        <f>0.25*G123</f>
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="I123" s="4">
+        <v>1</v>
+      </c>
+      <c r="J123" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K123" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L123">
+        <v>0.1</v>
+      </c>
+      <c r="M123" s="7">
+        <f>L123/H123</f>
+        <v>5.9701492537313436</v>
+      </c>
+      <c r="N123" s="7">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O123" s="15">
+        <v>5047.2924706829599</v>
+      </c>
+      <c r="P123">
+        <f>8*(N123/B123)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q123" s="8">
+        <f>8*(O123/B123)^2</f>
+        <v>3.2608206444304506E-3</v>
+      </c>
+      <c r="R123" s="9">
+        <f>(Q123-P123)/P123</f>
+        <v>-5.2740065420291748E-2</v>
+      </c>
+      <c r="S123" s="7">
+        <f>500*2*O123/B123</f>
+        <v>20.189169882731839</v>
+      </c>
+      <c r="T123" s="3">
+        <f>B123/4*P123</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U123" s="7">
+        <f t="shared" si="68"/>
+        <v>347.45509900000002</v>
+      </c>
+      <c r="V123" s="7">
+        <f t="shared" si="69"/>
+        <v>338.16859553575836</v>
+      </c>
+      <c r="W123" s="7">
+        <f>G123*N123</f>
+        <v>347.45509900000002</v>
+      </c>
+      <c r="X123" s="3">
+        <f>H123*N123</f>
+        <v>86.863774750000005</v>
+      </c>
+    </row>
+    <row r="124" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>222</v>
+      </c>
+      <c r="B124" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E124" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F124" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="G124">
+        <f>F124</f>
+        <v>0.05</v>
+      </c>
+      <c r="H124" s="4">
+        <f>0.25*G124</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="I124" s="4">
+        <v>1</v>
+      </c>
+      <c r="J124" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K124" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L124">
+        <v>0.1</v>
+      </c>
+      <c r="M124" s="7">
+        <f>L124/H124</f>
+        <v>8</v>
+      </c>
+      <c r="N124" s="7">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O124" s="15">
+        <v>5090.5135219019503</v>
+      </c>
+      <c r="P124">
+        <f>8*(N124/B124)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q124" s="8">
+        <f>8*(O124/B124)^2</f>
+        <v>3.3169059733333243E-3</v>
+      </c>
+      <c r="R124" s="9">
+        <f>(Q124-P124)/P124</f>
+        <v>-3.6447422929156821E-2</v>
+      </c>
+      <c r="S124" s="7">
+        <f>500*2*O124/B124</f>
+        <v>20.362054087607802</v>
+      </c>
+      <c r="T124" s="3">
+        <f>B124/4*P124</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U124" s="7">
+        <f t="shared" si="68"/>
+        <v>259.29485</v>
+      </c>
+      <c r="V124" s="7">
+        <f t="shared" si="69"/>
+        <v>254.52567609509754</v>
+      </c>
+      <c r="W124" s="7">
+        <f>G124*N124</f>
+        <v>259.29485</v>
+      </c>
+      <c r="X124" s="3">
+        <f>H124*N124</f>
+        <v>64.823712499999999</v>
+      </c>
+    </row>
+    <row r="125" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>222</v>
+      </c>
+      <c r="B125" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E125" s="4">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F125" s="4">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="G125">
+        <f>F125</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H125" s="4">
+        <f>0.25*G125</f>
+        <v>8.2500000000000004E-3</v>
+      </c>
+      <c r="I125" s="4">
+        <v>1</v>
+      </c>
+      <c r="J125" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K125" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L125">
+        <v>0.1</v>
+      </c>
+      <c r="M125" s="7">
+        <f>L125/H125</f>
+        <v>12.121212121212121</v>
+      </c>
+      <c r="N125" s="7">
+        <v>5185.8969999999999</v>
+      </c>
+      <c r="O125" s="15">
+        <v>5182.0467619173896</v>
+      </c>
+      <c r="P125">
+        <f>8*(N125/B125)^2</f>
+        <v>3.4423715449099523E-3</v>
+      </c>
+      <c r="Q125" s="8">
+        <f>8*(O125/B125)^2</f>
+        <v>3.4372619062654083E-3</v>
+      </c>
+      <c r="R125" s="9">
+        <f>(Q125-P125)/P125</f>
+        <v>-1.4843367654776779E-3</v>
+      </c>
+      <c r="S125" s="7">
+        <f>500*2*O125/B125</f>
+        <v>20.728187047669561</v>
+      </c>
+      <c r="T125" s="3">
+        <f>B125/4*P125</f>
+        <v>215.14822155687202</v>
+      </c>
+      <c r="U125" s="7">
+        <f t="shared" si="68"/>
+        <v>171.134601</v>
+      </c>
+      <c r="V125" s="7">
+        <f t="shared" si="69"/>
+        <v>171.00754314327386</v>
+      </c>
+      <c r="W125" s="7">
+        <f>G125*N125</f>
+        <v>171.134601</v>
+      </c>
+      <c r="X125" s="3">
+        <f>H125*N125</f>
         <v>42.783650250000001</v>
       </c>
     </row>
@@ -18568,7 +19260,7 @@
         <v>44</v>
       </c>
       <c r="D133" s="4">
-        <f t="shared" ref="D133:D134" si="60">E133*2</f>
+        <f t="shared" ref="D133:D134" si="70">E133*2</f>
         <v>0.1</v>
       </c>
       <c r="E133" s="4">
@@ -18617,7 +19309,7 @@
         <v>45</v>
       </c>
       <c r="D134" s="4">
-        <f t="shared" si="60"/>
+        <f t="shared" si="70"/>
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="E134" s="4">
@@ -19026,7 +19718,7 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19128,15 +19820,15 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="F2" s="4">
-        <f>2/80</f>
+        <f t="shared" ref="F2:H4" si="0">2/80</f>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G2" s="17">
-        <f>2/80</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="H2" s="17">
-        <f>2/80</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="I2" s="18">
@@ -19215,15 +19907,15 @@
         <v>0.05</v>
       </c>
       <c r="F3" s="4">
-        <f>2/80</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G3" s="17">
-        <f>2/80</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="H3" s="17">
-        <f>2/80</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="I3" s="18">
@@ -19301,15 +19993,15 @@
         <v>0.1</v>
       </c>
       <c r="F4" s="4">
-        <f>2/80</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G4" s="17">
-        <f>2/80</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="H4" s="17">
-        <f>2/80</f>
+        <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="I4" s="18">
@@ -19503,22 +20195,24 @@
       <c r="N6" s="11">
         <v>1055</v>
       </c>
-      <c r="O6" s="3"/>
+      <c r="O6" s="3">
+        <v>1043.2289674921899</v>
+      </c>
       <c r="P6" s="8">
         <f>8*(N6/B6)^2</f>
         <v>5.5651249999999998E-3</v>
       </c>
       <c r="Q6" s="8">
         <f>8*(O6/B6)^2</f>
-        <v>0</v>
+        <v>5.4416333930741032E-3</v>
       </c>
       <c r="R6" s="9">
         <f>(Q6-P6)/P6</f>
-        <v>-1</v>
+        <v>-2.219026651259344E-2</v>
       </c>
       <c r="S6" s="7">
         <f>1700*O6/B6</f>
-        <v>0</v>
+        <v>44.337231118418075</v>
       </c>
       <c r="T6" s="3">
         <f>B6/4*P6</f>

</xml_diff>

<commit_message>
alph2=2.52 for the first off-wall layers
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mchao\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B4A03E-02CE-4468-AD91-EB6645FA30B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF181F5-53D8-4862-B052-E8DE7C8C2A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="6" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
@@ -767,7 +767,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -910,9 +910,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -950,7 +950,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1056,7 +1056,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1198,7 +1198,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1208,21 +1208,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760F17C5-A88B-45BD-B60F-0BA67AB143DF}">
   <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A86" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" customWidth="1"/>
-    <col min="2" max="2" width="64.28515625" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="43.26953125" customWidth="1"/>
+    <col min="2" max="2" width="64.26953125" customWidth="1"/>
+    <col min="3" max="3" width="40.7265625" customWidth="1"/>
+    <col min="4" max="4" width="38.26953125" customWidth="1"/>
+    <col min="5" max="5" width="38.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>4</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="13.7" customHeight="1">
+    <row r="12" spans="1:5" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>5</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>6</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>1</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>4</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="57.95">
+    <row r="16" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>5</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>6</v>
       </c>
@@ -1410,12 +1410,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1480,182 +1480,182 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="2:2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="2:2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="2:2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="2:2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="2:2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="2:2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="2:2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="2:2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="2:2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="2:2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="2:2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="2:2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B51" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="2:2">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="2:2">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="2:2">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="2:2">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="2:2">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="2:2">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="2:2">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:2">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="2:2">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="2:2">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>56</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>59</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>60</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>61</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>59</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>60</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>62</v>
       </c>
@@ -1717,17 +1717,17 @@
         <v>63</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>66</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>70</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="14" t="s">
         <v>72</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="14" t="s">
         <v>73</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>74</v>
       </c>
@@ -1791,12 +1791,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>77</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
         <v>80</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
         <v>81</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
         <v>82</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>83</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>84</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>85</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>0.72123728255822872</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>86</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>1.6227838857560142</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>87</v>
       </c>
@@ -1886,13 +1886,13 @@
         <v>19.835640030216698</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C118">
         <f>SUM(C115:C117)/2857</f>
         <v>7.7632695829649772E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>88</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>93</v>
       </c>
@@ -1926,12 +1926,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>11</v>
       </c>
@@ -1948,12 +1948,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>101</v>
       </c>
@@ -1961,17 +1961,17 @@
         <v>102</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>105</v>
       </c>
@@ -1990,23 +1990,23 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="95.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="95.81640625" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="57.95">
+    <row r="2" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -2024,32 +2024,32 @@
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" customWidth="1"/>
+    <col min="7" max="7" width="14.26953125" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" customWidth="1"/>
+    <col min="10" max="10" width="20.7265625" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" customWidth="1"/>
+    <col min="15" max="15" width="11.453125" customWidth="1"/>
+    <col min="16" max="16" width="12.54296875" customWidth="1"/>
+    <col min="18" max="18" width="14.1796875" customWidth="1"/>
+    <col min="19" max="19" width="16.1796875" customWidth="1"/>
     <col min="20" max="20" width="13" customWidth="1"/>
-    <col min="21" max="21" width="12.140625" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" customWidth="1"/>
+    <col min="21" max="21" width="12.1796875" customWidth="1"/>
+    <col min="22" max="22" width="11.7265625" customWidth="1"/>
     <col min="23" max="23" width="13" customWidth="1"/>
-    <col min="24" max="24" width="13.42578125" customWidth="1"/>
+    <col min="24" max="24" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>109</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>4.5150460941314252</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>3.0250808830680551</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>2.2575230470657126</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>1.4899652110633703</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>2.7253667052842979E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>4.5150460941314252</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>3.0250808830680551</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>141</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>2.2575230470657126</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>1.4899652110633703</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>4.5150460941314252</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>142</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>3.0250808830680551</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>142</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>2.2575230470657126</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -3239,10 +3239,10 @@
         <v>1.4899652110633703</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="V19" s="7"/>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3267,7 +3267,7 @@
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>4.5150460941314252</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>143</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>3.0250808830680551</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>143</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>2.2575230470657126</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>143</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>1.4899652110633703</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>144</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>4.5150460941314252</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>144</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>3.0250808830680551</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>144</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>2.2575230470657126</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -3951,13 +3951,13 @@
         <v>1.4899652110633703</v>
       </c>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="S32" s="7"/>
     </row>
-    <row r="33" spans="1:24">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="S33" s="7"/>
     </row>
-    <row r="34" spans="1:24">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>4.5150460941314252</v>
       </c>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>146</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>3.0250808830680551</v>
       </c>
     </row>
-    <row r="36" spans="1:24">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>146</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>2.2575230470657126</v>
       </c>
     </row>
-    <row r="37" spans="1:24">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>146</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>1.4899652110633703</v>
       </c>
     </row>
-    <row r="38" spans="1:24">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -4319,7 +4319,7 @@
       <c r="W38" s="7"/>
       <c r="X38" s="7"/>
     </row>
-    <row r="39" spans="1:24">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
@@ -4341,7 +4341,7 @@
       <c r="W39" s="7"/>
       <c r="X39" s="7"/>
     </row>
-    <row r="40" spans="1:24">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -4363,12 +4363,12 @@
       <c r="W40" s="7"/>
       <c r="X40" s="7"/>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>109</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
         <v>5714</v>
       </c>
@@ -4481,12 +4481,12 @@
         <v>11.416529916489431</v>
       </c>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>153</v>
       </c>
@@ -4504,33 +4504,33 @@
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.81640625" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" customWidth="1"/>
+    <col min="9" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" customWidth="1"/>
-    <col min="16" max="17" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26953125" customWidth="1"/>
+    <col min="16" max="17" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1796875" customWidth="1"/>
+    <col min="19" max="19" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>109</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>154</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>1.2224732270400001</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="21" t="s">
         <v>154</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>0.89295357976000012</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>154</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>0.78681422024000014</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
         <v>154</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>0.57990212888000003</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="21"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -4971,7 +4971,7 @@
       <c r="W6" s="21"/>
       <c r="X6" s="21"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
         <v>161</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>0.89295357976000012</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="21" t="s">
         <v>162</v>
       </c>
@@ -5143,7 +5143,7 @@
         <v>0.89295357976000012</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="21" t="s">
         <v>163</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>0.89295357976000012</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -5255,7 +5255,7 @@
       <c r="W10" s="21"/>
       <c r="X10" s="21"/>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="21" t="s">
         <v>164</v>
       </c>
@@ -5341,7 +5341,7 @@
         <v>1.2224732270400001</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
         <v>164</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>0.89295357976000012</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="21" t="s">
         <v>164</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>0.78681422024000014</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
         <v>164</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>0.57990212888000003</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -5622,7 +5622,7 @@
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -5645,15 +5645,15 @@
       <c r="W16" s="7"/>
       <c r="X16" s="7"/>
     </row>
-    <row r="18" spans="2:24">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.35">
       <c r="W18" s="7"/>
       <c r="X18" s="7"/>
     </row>
-    <row r="19" spans="2:24">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.35">
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
     </row>
-    <row r="20" spans="2:24">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -5678,7 +5678,7 @@
       <c r="W20" s="7"/>
       <c r="X20" s="7"/>
     </row>
-    <row r="21" spans="2:24">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -5703,7 +5703,7 @@
       <c r="W21" s="7"/>
       <c r="X21" s="7"/>
     </row>
-    <row r="22" spans="2:24">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -5728,7 +5728,7 @@
       <c r="W22" s="7"/>
       <c r="X22" s="7"/>
     </row>
-    <row r="23" spans="2:24">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -5753,7 +5753,7 @@
       <c r="W23" s="7"/>
       <c r="X23" s="7"/>
     </row>
-    <row r="24" spans="2:24">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -5778,7 +5778,7 @@
       <c r="W24" s="7"/>
       <c r="X24" s="7"/>
     </row>
-    <row r="26" spans="2:24">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -5803,7 +5803,7 @@
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
     </row>
-    <row r="27" spans="2:24">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -5828,7 +5828,7 @@
       <c r="W27" s="7"/>
       <c r="X27" s="7"/>
     </row>
-    <row r="28" spans="2:24">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -5853,7 +5853,7 @@
       <c r="W28" s="7"/>
       <c r="X28" s="7"/>
     </row>
-    <row r="29" spans="2:24">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -5891,25 +5891,25 @@
       <selection activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" customWidth="1"/>
+    <col min="16" max="16" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.1796875" customWidth="1"/>
     <col min="19" max="19" width="15" customWidth="1"/>
-    <col min="20" max="20" width="12.140625" customWidth="1"/>
-    <col min="23" max="23" width="10.7109375" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" customWidth="1"/>
+    <col min="20" max="20" width="12.1796875" customWidth="1"/>
+    <col min="23" max="23" width="10.7265625" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>109</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -6066,7 +6066,7 @@
         <v>13.793750000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>9.2418125</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -6238,7 +6238,7 @@
         <v>6.8968750000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -6324,7 +6324,7 @@
         <v>4.5519375000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -6339,7 +6339,7 @@
       <c r="P6" s="8"/>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -6354,7 +6354,7 @@
       <c r="P7" s="8"/>
       <c r="Q7" s="3"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>13.793750000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -6525,7 +6525,7 @@
         <v>9.2418125</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -6611,7 +6611,7 @@
         <v>6.8968750000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>141</v>
       </c>
@@ -6697,7 +6697,7 @@
         <v>4.5519375000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -6716,7 +6716,7 @@
       <c r="S12" s="7"/>
       <c r="T12" s="3"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -6735,7 +6735,7 @@
       <c r="S13" s="7"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>143</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>13.793750000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -6907,7 +6907,7 @@
         <v>9.2418125</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>6.8968750000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>143</v>
       </c>
@@ -7079,15 +7079,15 @@
         <v>4.5519375000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="W18" s="7"/>
       <c r="X18" s="7"/>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>146</v>
       </c>
@@ -7171,7 +7171,7 @@
         <v>0.60387713300000001</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>154</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>0.60387713300000001</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>167</v>
       </c>
@@ -7339,7 +7339,7 @@
         <v>0.60387713300000001</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>154</v>
       </c>
@@ -7422,7 +7422,7 @@
         <v>0.39739451665000003</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>161</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>0.60387713300000001</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>169</v>
       </c>
@@ -7590,7 +7590,7 @@
         <v>0.60387713300000001</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>170</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>0.60387713300000001</v>
       </c>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>171</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>0.60387713300000001</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>154</v>
       </c>
@@ -7841,7 +7841,7 @@
         <v>1.25608591075</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>154</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>1.3024439457499999</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>154</v>
       </c>
@@ -8011,7 +8011,7 @@
         <v>0.29612416982499995</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>154</v>
       </c>
@@ -8097,7 +8097,7 @@
         <v>0.60387713300000001</v>
       </c>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>154</v>
       </c>
@@ -8183,7 +8183,7 @@
         <v>0.1466359491</v>
       </c>
     </row>
-    <row r="33" spans="1:24">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>154</v>
       </c>
@@ -8269,7 +8269,7 @@
         <v>0.29612416982499995</v>
       </c>
     </row>
-    <row r="34" spans="1:24">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>177</v>
       </c>
@@ -8352,7 +8352,7 @@
         <v>1.25608591075</v>
       </c>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>177</v>
       </c>
@@ -8436,7 +8436,7 @@
         <v>0.60387713300000001</v>
       </c>
     </row>
-    <row r="38" spans="1:24">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>164</v>
       </c>
@@ -8520,7 +8520,7 @@
         <v>0.60387713300000001</v>
       </c>
     </row>
-    <row r="39" spans="1:24">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>164</v>
       </c>
@@ -8603,7 +8603,7 @@
         <v>1.25608591075</v>
       </c>
     </row>
-    <row r="40" spans="1:24">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>178</v>
       </c>
@@ -8686,7 +8686,7 @@
         <v>1.25608591075</v>
       </c>
     </row>
-    <row r="41" spans="1:24">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>179</v>
       </c>
@@ -8769,7 +8769,7 @@
         <v>1.25608591075</v>
       </c>
     </row>
-    <row r="42" spans="1:24">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
@@ -8794,7 +8794,7 @@
       <c r="W42" s="7"/>
       <c r="X42" s="7"/>
     </row>
-    <row r="44" spans="1:24">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>164</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>0.60387713300000001</v>
       </c>
     </row>
-    <row r="45" spans="1:24">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>164</v>
       </c>
@@ -8966,12 +8966,12 @@
         <v>0.29612416982499995</v>
       </c>
     </row>
-    <row r="48" spans="1:24">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>181</v>
       </c>
@@ -9054,7 +9054,7 @@
         <v>13.793750000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>181</v>
       </c>
@@ -9138,7 +9138,7 @@
         <v>9.2418125</v>
       </c>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>181</v>
       </c>
@@ -9222,7 +9222,7 @@
         <v>6.8968750000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:24">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>181</v>
       </c>
@@ -9306,7 +9306,7 @@
         <v>4.5519375000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:24">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>186</v>
       </c>
@@ -9389,7 +9389,7 @@
         <v>13.793750000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:24">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>186</v>
       </c>
@@ -9473,7 +9473,7 @@
         <v>9.2418125</v>
       </c>
     </row>
-    <row r="57" spans="1:24">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>186</v>
       </c>
@@ -9557,7 +9557,7 @@
         <v>6.8968750000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:24">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>186</v>
       </c>
@@ -9657,32 +9657,32 @@
       <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" customWidth="1"/>
-    <col min="18" max="18" width="15.85546875" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" customWidth="1"/>
-    <col min="23" max="23" width="10.28515625" customWidth="1"/>
-    <col min="24" max="24" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="7.26953125" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" customWidth="1"/>
+    <col min="11" max="11" width="12.453125" customWidth="1"/>
+    <col min="12" max="12" width="14.1796875" customWidth="1"/>
+    <col min="13" max="13" width="12.453125" customWidth="1"/>
+    <col min="14" max="14" width="12.1796875" customWidth="1"/>
+    <col min="15" max="15" width="10.54296875" customWidth="1"/>
+    <col min="17" max="17" width="10.54296875" customWidth="1"/>
+    <col min="18" max="18" width="15.81640625" customWidth="1"/>
+    <col min="19" max="19" width="15.54296875" customWidth="1"/>
+    <col min="20" max="20" width="11.1796875" customWidth="1"/>
+    <col min="23" max="23" width="10.26953125" customWidth="1"/>
+    <col min="24" max="24" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>109</v>
       </c>
@@ -9753,7 +9753,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -9839,7 +9839,7 @@
         <v>25.052500000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -9925,7 +9925,7 @@
         <v>16.785175000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -10011,7 +10011,7 @@
         <v>12.526250000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -10097,7 +10097,7 @@
         <v>8.2673250000000014</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
@@ -10112,7 +10112,7 @@
       <c r="W6" s="7"/>
       <c r="X6" s="3"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
@@ -10127,7 +10127,7 @@
       <c r="W7" s="7"/>
       <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -10213,7 +10213,7 @@
         <v>25.052500000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -10299,7 +10299,7 @@
         <v>16.785175000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -10385,7 +10385,7 @@
         <v>12.526250000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>141</v>
       </c>
@@ -10471,19 +10471,19 @@
         <v>8.2673250000000014</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U12" s="7"/>
       <c r="V12" s="7"/>
       <c r="W12" s="7"/>
       <c r="X12" s="3"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U13" s="7"/>
       <c r="V13" s="7"/>
       <c r="W13" s="7"/>
       <c r="X13" s="3"/>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>143</v>
       </c>
@@ -10569,7 +10569,7 @@
         <v>25.052500000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -10655,7 +10655,7 @@
         <v>16.785175000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -10741,7 +10741,7 @@
         <v>12.526250000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>143</v>
       </c>
@@ -10827,16 +10827,16 @@
         <v>8.2673250000000014</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
       <c r="W18" s="7"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="V19" s="7"/>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>146</v>
       </c>
@@ -10922,13 +10922,13 @@
         <v>0.70665296141</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U21" s="7"/>
       <c r="V21" s="7"/>
       <c r="W21" s="7"/>
       <c r="X21" s="3"/>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>146</v>
       </c>
@@ -11014,7 +11014,7 @@
         <v>2.5458651130000001</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>191</v>
       </c>
@@ -11100,7 +11100,7 @@
         <v>2.5458651130000001</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>192</v>
       </c>
@@ -11186,7 +11186,7 @@
         <v>2.5458651130000001</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>193</v>
       </c>
@@ -11272,7 +11272,7 @@
         <v>2.5458651130000001</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" s="21" t="s">
         <v>154</v>
       </c>
@@ -11358,7 +11358,7 @@
         <v>1.0967743996000001</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" s="21" t="s">
         <v>154</v>
       </c>
@@ -11444,7 +11444,7 @@
         <v>0.53782696979</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" s="21" t="s">
         <v>164</v>
       </c>
@@ -11530,7 +11530,7 @@
         <v>1.0967743996000001</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" s="21" t="s">
         <v>164</v>
       </c>
@@ -11616,7 +11616,7 @@
         <v>0.53782696979</v>
       </c>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>164</v>
       </c>
@@ -11712,38 +11712,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42F51E-90FA-449F-904F-669D9897EDC7}">
   <dimension ref="A1:X134"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R110" sqref="R110"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" customWidth="1"/>
+    <col min="12" max="12" width="8.81640625" customWidth="1"/>
+    <col min="13" max="13" width="14.81640625" customWidth="1"/>
+    <col min="14" max="14" width="12.1796875" customWidth="1"/>
+    <col min="15" max="15" width="8.54296875" customWidth="1"/>
+    <col min="16" max="16" width="10.81640625" customWidth="1"/>
+    <col min="17" max="17" width="15.453125" customWidth="1"/>
+    <col min="18" max="18" width="14.7265625" customWidth="1"/>
     <col min="19" max="19" width="19" customWidth="1"/>
-    <col min="20" max="20" width="14.85546875" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" customWidth="1"/>
+    <col min="20" max="20" width="14.81640625" customWidth="1"/>
+    <col min="21" max="21" width="14.1796875" customWidth="1"/>
     <col min="22" max="22" width="12" customWidth="1"/>
-    <col min="23" max="23" width="13.5703125" customWidth="1"/>
-    <col min="24" max="24" width="13.42578125" customWidth="1"/>
+    <col min="23" max="23" width="13.54296875" customWidth="1"/>
+    <col min="24" max="24" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>109</v>
       </c>
@@ -11814,7 +11814,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -11900,7 +11900,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -11986,7 +11986,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -12072,7 +12072,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -12158,7 +12158,7 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -12177,14 +12177,14 @@
       <c r="W6" s="7"/>
       <c r="X6" s="3"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="T7" s="5"/>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
       <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -12270,7 +12270,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -12356,7 +12356,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -12442,7 +12442,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>141</v>
       </c>
@@ -12528,19 +12528,19 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U12" s="7"/>
       <c r="V12" s="7"/>
       <c r="W12" s="7"/>
       <c r="X12" s="3"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U13" s="7"/>
       <c r="V13" s="7"/>
       <c r="W13" s="7"/>
       <c r="X13" s="3"/>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>196</v>
       </c>
@@ -12626,7 +12626,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>196</v>
       </c>
@@ -12712,7 +12712,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>196</v>
       </c>
@@ -12798,7 +12798,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>196</v>
       </c>
@@ -12884,19 +12884,19 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
       <c r="W18" s="7"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U19" s="7"/>
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>197</v>
       </c>
@@ -12982,7 +12982,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>197</v>
       </c>
@@ -13068,7 +13068,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>197</v>
       </c>
@@ -13154,7 +13154,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>197</v>
       </c>
@@ -13240,19 +13240,19 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U24" s="7"/>
       <c r="V24" s="7"/>
       <c r="W24" s="7"/>
       <c r="X24" s="3"/>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U25" s="7"/>
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>198</v>
       </c>
@@ -13338,7 +13338,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>198</v>
       </c>
@@ -13424,7 +13424,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>198</v>
       </c>
@@ -13510,7 +13510,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>198</v>
       </c>
@@ -13596,19 +13596,19 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U30" s="7"/>
       <c r="V30" s="7"/>
       <c r="W30" s="7"/>
       <c r="X30" s="3"/>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U31" s="7"/>
       <c r="V31" s="7"/>
       <c r="W31" s="7"/>
       <c r="X31" s="3"/>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>199</v>
       </c>
@@ -13694,7 +13694,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="33" spans="1:24">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>199</v>
       </c>
@@ -13780,7 +13780,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="34" spans="1:24">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>199</v>
       </c>
@@ -13866,7 +13866,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>199</v>
       </c>
@@ -13952,19 +13952,19 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="36" spans="1:24">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U36" s="7"/>
       <c r="V36" s="7"/>
       <c r="W36" s="7"/>
       <c r="X36" s="3"/>
     </row>
-    <row r="37" spans="1:24">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U37" s="7"/>
       <c r="V37" s="7"/>
       <c r="W37" s="7"/>
       <c r="X37" s="3"/>
     </row>
-    <row r="38" spans="1:24">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -14050,7 +14050,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="39" spans="1:24">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>143</v>
       </c>
@@ -14136,7 +14136,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="40" spans="1:24">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>143</v>
       </c>
@@ -14222,7 +14222,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="41" spans="1:24">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>143</v>
       </c>
@@ -14308,19 +14308,19 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="42" spans="1:24">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U42" s="7"/>
       <c r="V42" s="7"/>
       <c r="W42" s="7"/>
       <c r="X42" s="3"/>
     </row>
-    <row r="43" spans="1:24">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U43" s="7"/>
       <c r="V43" s="7"/>
       <c r="W43" s="7"/>
       <c r="X43" s="3"/>
     </row>
-    <row r="44" spans="1:24">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>200</v>
       </c>
@@ -14406,7 +14406,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="45" spans="1:24">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>200</v>
       </c>
@@ -14492,7 +14492,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="46" spans="1:24">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>200</v>
       </c>
@@ -14578,7 +14578,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="47" spans="1:24">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>200</v>
       </c>
@@ -14664,19 +14664,19 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="48" spans="1:24">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U48" s="7"/>
       <c r="V48" s="7"/>
       <c r="W48" s="7"/>
       <c r="X48" s="3"/>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U49" s="7"/>
       <c r="V49" s="7"/>
       <c r="W49" s="7"/>
       <c r="X49" s="3"/>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>201</v>
       </c>
@@ -14762,7 +14762,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>201</v>
       </c>
@@ -14848,7 +14848,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="52" spans="1:24">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>201</v>
       </c>
@@ -14934,7 +14934,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="53" spans="1:24">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>201</v>
       </c>
@@ -15020,19 +15020,19 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="54" spans="1:24">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U54" s="7"/>
       <c r="V54" s="7"/>
       <c r="W54" s="7"/>
       <c r="X54" s="3"/>
     </row>
-    <row r="55" spans="1:24">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U55" s="7"/>
       <c r="V55" s="7"/>
       <c r="W55" s="7"/>
       <c r="X55" s="3"/>
     </row>
-    <row r="56" spans="1:24">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>202</v>
       </c>
@@ -15118,7 +15118,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="57" spans="1:24">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>202</v>
       </c>
@@ -15204,7 +15204,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="58" spans="1:24">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>202</v>
       </c>
@@ -15290,7 +15290,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="59" spans="1:24">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>202</v>
       </c>
@@ -15376,19 +15376,19 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="60" spans="1:24">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U60" s="7"/>
       <c r="V60" s="7"/>
       <c r="W60" s="7"/>
       <c r="X60" s="3"/>
     </row>
-    <row r="61" spans="1:24">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U61" s="7"/>
       <c r="V61" s="7"/>
       <c r="W61" s="7"/>
       <c r="X61" s="3"/>
     </row>
-    <row r="62" spans="1:24">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>142</v>
       </c>
@@ -15474,7 +15474,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="63" spans="1:24">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>142</v>
       </c>
@@ -15560,7 +15560,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="64" spans="1:24">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>142</v>
       </c>
@@ -15646,7 +15646,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="65" spans="1:24">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>142</v>
       </c>
@@ -15732,19 +15732,19 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="66" spans="1:24">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U66" s="7"/>
       <c r="V66" s="7"/>
       <c r="W66" s="7"/>
       <c r="X66" s="3"/>
     </row>
-    <row r="67" spans="1:24">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U67" s="7"/>
       <c r="V67" s="7"/>
       <c r="W67" s="7"/>
       <c r="X67" s="3"/>
     </row>
-    <row r="68" spans="1:24">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>146</v>
       </c>
@@ -15830,7 +15830,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="69" spans="1:24">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>146</v>
       </c>
@@ -15916,7 +15916,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="70" spans="1:24">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>146</v>
       </c>
@@ -16002,7 +16002,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="71" spans="1:24">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>146</v>
       </c>
@@ -16088,19 +16088,19 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="72" spans="1:24">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U72" s="7"/>
       <c r="V72" s="7"/>
       <c r="W72" s="7"/>
       <c r="X72" s="3"/>
     </row>
-    <row r="73" spans="1:24">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.35">
       <c r="U73" s="7"/>
       <c r="V73" s="7"/>
       <c r="W73" s="7"/>
       <c r="X73" s="3"/>
     </row>
-    <row r="74" spans="1:24">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>144</v>
       </c>
@@ -16186,7 +16186,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="75" spans="1:24">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>144</v>
       </c>
@@ -16272,7 +16272,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="76" spans="1:24">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>144</v>
       </c>
@@ -16358,7 +16358,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="77" spans="1:24">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>144</v>
       </c>
@@ -16444,7 +16444,7 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="80" spans="1:24">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>208</v>
       </c>
@@ -16530,7 +16530,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="81" spans="1:24">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>208</v>
       </c>
@@ -16616,7 +16616,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="82" spans="1:24">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>208</v>
       </c>
@@ -16702,7 +16702,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="83" spans="1:24">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>208</v>
       </c>
@@ -16788,7 +16788,7 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="86" spans="1:24">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>181</v>
       </c>
@@ -16874,7 +16874,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="87" spans="1:24">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>181</v>
       </c>
@@ -16960,7 +16960,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="88" spans="1:24">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>181</v>
       </c>
@@ -17046,7 +17046,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="89" spans="1:24">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>181</v>
       </c>
@@ -17132,7 +17132,7 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="92" spans="1:24">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>209</v>
       </c>
@@ -17218,7 +17218,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="93" spans="1:24">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>209</v>
       </c>
@@ -17304,7 +17304,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="94" spans="1:24">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>209</v>
       </c>
@@ -17390,7 +17390,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="95" spans="1:24">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>209</v>
       </c>
@@ -17476,7 +17476,7 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="98" spans="1:24">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>210</v>
       </c>
@@ -17562,7 +17562,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="99" spans="1:24">
+    <row r="99" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>210</v>
       </c>
@@ -17648,7 +17648,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="100" spans="1:24">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>210</v>
       </c>
@@ -17734,7 +17734,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="101" spans="1:24">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>210</v>
       </c>
@@ -17820,12 +17820,12 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="103" spans="1:24">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="104" spans="1:24">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>186</v>
       </c>
@@ -17911,7 +17911,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="105" spans="1:24">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>186</v>
       </c>
@@ -17997,7 +17997,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="106" spans="1:24">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>186</v>
       </c>
@@ -18083,7 +18083,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="107" spans="1:24">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>186</v>
       </c>
@@ -18169,7 +18169,7 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="110" spans="1:24">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>181</v>
       </c>
@@ -18255,7 +18255,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="111" spans="1:24">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>181</v>
       </c>
@@ -18341,7 +18341,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="112" spans="1:24">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>181</v>
       </c>
@@ -18427,7 +18427,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="113" spans="1:24">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>181</v>
       </c>
@@ -18513,7 +18513,7 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="116" spans="1:24">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>154</v>
       </c>
@@ -18599,7 +18599,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="117" spans="1:24">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>154</v>
       </c>
@@ -18685,7 +18685,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="118" spans="1:24">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>154</v>
       </c>
@@ -18771,7 +18771,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="119" spans="1:24">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>154</v>
       </c>
@@ -18857,7 +18857,7 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="122" spans="1:24">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>211</v>
       </c>
@@ -18943,7 +18943,7 @@
         <v>129.647425</v>
       </c>
     </row>
-    <row r="123" spans="1:24">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>211</v>
       </c>
@@ -19029,7 +19029,7 @@
         <v>86.863774750000005</v>
       </c>
     </row>
-    <row r="124" spans="1:24">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>211</v>
       </c>
@@ -19115,7 +19115,7 @@
         <v>64.823712499999999</v>
       </c>
     </row>
-    <row r="125" spans="1:24">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>211</v>
       </c>
@@ -19201,7 +19201,7 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="131" spans="1:15">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A131" s="4">
         <v>250000</v>
       </c>
@@ -19248,7 +19248,7 @@
         <v>3.4423715449099523E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:15">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A132" s="4">
         <v>250000</v>
       </c>
@@ -19297,7 +19297,7 @@
         <v>3.4423715449099523E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:15">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A133" s="4">
         <v>250000</v>
       </c>
@@ -19346,7 +19346,7 @@
         <v>3.4423715449099523E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:15">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A134" s="4">
         <v>250000</v>
       </c>
@@ -19409,23 +19409,23 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" customWidth="1"/>
-    <col min="24" max="24" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" customWidth="1"/>
+    <col min="18" max="18" width="12.26953125" customWidth="1"/>
+    <col min="19" max="19" width="14.81640625" customWidth="1"/>
+    <col min="24" max="24" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>109</v>
       </c>
@@ -19496,7 +19496,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -19582,7 +19582,7 @@
         <v>2.34375</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>220</v>
       </c>
@@ -19670,7 +19670,7 @@
         <v>1.5625</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>222</v>
       </c>
@@ -19769,17 +19769,17 @@
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
+    <col min="18" max="18" width="13.453125" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>109</v>
       </c>
@@ -19850,7 +19850,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>181</v>
       </c>
@@ -19937,7 +19937,7 @@
         <v>26.375</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>181</v>
       </c>
@@ -20023,7 +20023,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>181</v>
       </c>
@@ -20109,7 +20109,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -20196,7 +20196,7 @@
         <v>17.583333333333332</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>181</v>
       </c>

</xml_diff>

<commit_message>
alph2=2.52 in the first off-wall layer applied to any numbers of walls
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mchao\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF181F5-53D8-4862-B052-E8DE7C8C2A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9698BB1A-205B-4775-BD57-4443AAC2A674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="6" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="225">
   <si>
     <t>channel, two walls</t>
   </si>
@@ -704,18 +704,6 @@
   </si>
   <si>
     <t>WM+SMAG+SMALL+MOV</t>
-  </si>
-  <si>
-    <t>64×48×32</t>
-  </si>
-  <si>
-    <t>96×72×48</t>
-  </si>
-  <si>
-    <t>128×96×64</t>
-  </si>
-  <si>
-    <t>192×144×96</t>
   </si>
   <si>
     <t>dz_w=dy</t>
@@ -11712,8 +11700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42F51E-90FA-449F-904F-669D9897EDC7}">
   <dimension ref="A1:X134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q133" sqref="Q133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19201,199 +19189,57 @@
         <v>42.783650250000001</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A131" s="4">
-        <v>250000</v>
-      </c>
-      <c r="B131" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="D131" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="E131" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="F131">
-        <v>0.1</v>
-      </c>
-      <c r="G131" s="4">
-        <f>0.25*F131</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H131" s="4">
-        <v>2</v>
-      </c>
-      <c r="I131" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="J131" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="K131">
-        <v>0.1</v>
-      </c>
-      <c r="L131" s="7">
-        <f>K131/G131</f>
-        <v>4</v>
-      </c>
-      <c r="M131" s="7">
-        <v>5185.8969999999999</v>
-      </c>
-      <c r="O131">
-        <f>8*(M131/A131)^2</f>
-        <v>3.4423715449099523E-3</v>
-      </c>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A132" s="4">
-        <v>250000</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C132" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D132" s="4">
-        <f>E132*2</f>
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="E132" s="4">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="F132">
-        <f>E132</f>
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="G132" s="4">
-        <f>0.25*F132</f>
-        <v>1.6750000000000001E-2</v>
-      </c>
-      <c r="H132" s="4">
-        <v>2</v>
-      </c>
-      <c r="I132" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="J132" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="K132">
-        <v>0.1</v>
-      </c>
-      <c r="L132" s="7">
-        <f>K132/G132</f>
-        <v>5.9701492537313436</v>
-      </c>
-      <c r="M132" s="7">
-        <v>5185.8969999999999</v>
-      </c>
-      <c r="O132">
-        <f>8*(M132/A132)^2</f>
-        <v>3.4423715449099523E-3</v>
-      </c>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A133" s="4">
-        <v>250000</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="D133" s="4">
-        <f t="shared" ref="D133:D134" si="70">E133*2</f>
-        <v>0.1</v>
-      </c>
-      <c r="E133" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="F133">
-        <f>E133</f>
-        <v>0.05</v>
-      </c>
-      <c r="G133" s="4">
-        <f>0.25*F133</f>
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="H133" s="4">
-        <v>2</v>
-      </c>
-      <c r="I133" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="J133" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="K133">
-        <v>0.1</v>
-      </c>
-      <c r="L133" s="7">
-        <f>K133/G133</f>
-        <v>8</v>
-      </c>
-      <c r="M133" s="7">
-        <v>5185.8969999999999</v>
-      </c>
-      <c r="O133">
-        <f>8*(M133/A133)^2</f>
-        <v>3.4423715449099523E-3</v>
-      </c>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A134" s="4">
-        <v>250000</v>
-      </c>
-      <c r="B134" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C134" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="D134" s="4">
-        <f t="shared" si="70"/>
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="E134" s="4">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="F134">
-        <f>E134</f>
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="G134" s="4">
-        <f>0.25*F134</f>
-        <v>8.2500000000000004E-3</v>
-      </c>
-      <c r="H134" s="4">
-        <v>2</v>
-      </c>
-      <c r="I134" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="J134" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="K134">
-        <v>0.1</v>
-      </c>
-      <c r="L134" s="7">
-        <f>K134/G134</f>
-        <v>12.121212121212121</v>
-      </c>
-      <c r="M134" s="7">
-        <v>5185.8969999999999</v>
-      </c>
-      <c r="O134">
-        <f>8*(M134/A134)^2</f>
-        <v>3.4423715449099523E-3</v>
-      </c>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A131" s="4"/>
+      <c r="B131" s="4"/>
+      <c r="C131" s="4"/>
+      <c r="D131" s="4"/>
+      <c r="E131" s="4"/>
+      <c r="G131" s="4"/>
+      <c r="H131" s="4"/>
+      <c r="I131" s="4"/>
+      <c r="J131" s="4"/>
+      <c r="L131" s="7"/>
+      <c r="M131" s="7"/>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A132" s="4"/>
+      <c r="B132" s="4"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="4"/>
+      <c r="G132" s="4"/>
+      <c r="H132" s="4"/>
+      <c r="I132" s="4"/>
+      <c r="J132" s="4"/>
+      <c r="L132" s="7"/>
+      <c r="M132" s="7"/>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A133" s="4"/>
+      <c r="B133" s="4"/>
+      <c r="C133" s="4"/>
+      <c r="D133" s="4"/>
+      <c r="E133" s="4"/>
+      <c r="G133" s="4"/>
+      <c r="H133" s="4"/>
+      <c r="I133" s="4"/>
+      <c r="J133" s="4"/>
+      <c r="L133" s="7"/>
+      <c r="M133" s="7"/>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A134" s="4"/>
+      <c r="B134" s="4"/>
+      <c r="C134" s="4"/>
+      <c r="D134" s="4"/>
+      <c r="E134" s="4"/>
+      <c r="G134" s="4"/>
+      <c r="H134" s="4"/>
+      <c r="I134" s="4"/>
+      <c r="J134" s="4"/>
+      <c r="L134" s="7"/>
+      <c r="M134" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -19445,7 +19291,7 @@
         <v>112</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>114</v>
@@ -19504,10 +19350,10 @@
         <v>4410</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E2" s="17">
         <f>12.8/384</f>
@@ -19528,7 +19374,7 @@
         <v>2.1333333333333333</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>134</v>
@@ -19584,16 +19430,16 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B3" s="4">
         <v>4410</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>217</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>221</v>
       </c>
       <c r="E3" s="17">
         <f>12.8/576</f>
@@ -19616,7 +19462,7 @@
         <v>2.1333333333333337</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>134</v>
@@ -19672,13 +19518,13 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B4" s="4">
         <v>4410</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>165</v>
@@ -19702,7 +19548,7 @@
         <v>2.1333333333333333</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>134</v>
@@ -19799,7 +19645,7 @@
         <v>112</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>114</v>
@@ -19858,10 +19704,10 @@
         <v>40000</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E2" s="17">
         <f>6.4/256</f>
@@ -19883,7 +19729,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>134</v>
@@ -19945,10 +19791,10 @@
         <v>40000</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E3" s="17">
         <f>6.4/128</f>
@@ -19970,7 +19816,7 @@
         <v>2</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>134</v>
@@ -20031,10 +19877,10 @@
         <v>40000</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E4" s="17">
         <f>6.4/64</f>
@@ -20056,7 +19902,7 @@
         <v>4</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>134</v>
@@ -20117,10 +19963,10 @@
         <v>40000</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>227</v>
       </c>
       <c r="E5" s="17">
         <f>6.4/384</f>
@@ -20142,7 +19988,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>134</v>
@@ -20204,10 +20050,10 @@
         <v>40000</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E6" s="17">
         <f>6.4/512</f>
@@ -20229,7 +20075,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>134</v>

</xml_diff>

<commit_message>
_CHANNEL, _DUCT, _CAVITY predefined
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mchao\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9698BB1A-205B-4775-BD57-4443AAC2A674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D71E91-E6F7-43B0-AC9D-E86F0C7B01BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="6" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="3" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
@@ -4488,9 +4488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B745900-CF34-4783-B8B3-D2DA1ADCC55F}">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4507,7 +4505,7 @@
     <col min="11" max="11" width="8.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6328125" customWidth="1"/>
     <col min="15" max="15" width="11.26953125" customWidth="1"/>
     <col min="16" max="17" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.1796875" customWidth="1"/>
@@ -11700,8 +11698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42F51E-90FA-449F-904F-669D9897EDC7}">
   <dimension ref="A1:X134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q133" sqref="Q133"/>
+    <sheetView topLeftCell="A52" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E117" sqref="E117:F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19612,7 +19610,7 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19707,11 +19705,11 @@
         <v>219</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E2" s="17">
-        <f>6.4/256</f>
-        <v>2.5000000000000001E-2</v>
+        <f>6.4/64</f>
+        <v>0.1</v>
       </c>
       <c r="F2" s="4">
         <f t="shared" ref="F2:H4" si="0">2/80</f>
@@ -19726,7 +19724,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="I2" s="18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>215</v>
@@ -19744,7 +19742,7 @@
         <v>1055</v>
       </c>
       <c r="O2" s="3">
-        <v>1038.48230917147</v>
+        <v>1065.6540405542701</v>
       </c>
       <c r="P2" s="8">
         <f>8*(N2/B2)^2</f>
@@ -19752,15 +19750,15 @@
       </c>
       <c r="Q2" s="8">
         <f>8*(O2/B2)^2</f>
-        <v>5.3922275323105423E-3</v>
+        <v>5.6780926707482096E-3</v>
       </c>
       <c r="R2" s="9">
         <f>(Q2-P2)/P2</f>
-        <v>-3.106802950328294E-2</v>
+        <v>2.0299215336261067E-2</v>
       </c>
       <c r="S2" s="7">
         <f>1700*O2/B2</f>
-        <v>44.135498139787479</v>
+        <v>45.29029672355648</v>
       </c>
       <c r="T2" s="3">
         <f>B2/4*P2</f>
@@ -19768,7 +19766,7 @@
       </c>
       <c r="U2" s="7">
         <f>E2*N2</f>
-        <v>26.375</v>
+        <v>105.5</v>
       </c>
       <c r="V2" s="7">
         <f>F2*N2</f>
@@ -19779,8 +19777,7 @@
         <v>26.375</v>
       </c>
       <c r="X2" s="7">
-        <f>H2*N2</f>
-        <v>26.375</v>
+        <v>26.4</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.35">
@@ -19880,11 +19877,11 @@
         <v>219</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E4" s="17">
-        <f>6.4/64</f>
-        <v>0.1</v>
+        <f>6.4/256</f>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F4" s="4">
         <f t="shared" si="0"/>
@@ -19899,7 +19896,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="I4" s="18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>215</v>
@@ -19917,7 +19914,7 @@
         <v>1055</v>
       </c>
       <c r="O4" s="3">
-        <v>1065.6540405542701</v>
+        <v>1038.48230917147</v>
       </c>
       <c r="P4" s="8">
         <f>8*(N4/B4)^2</f>
@@ -19925,15 +19922,15 @@
       </c>
       <c r="Q4" s="8">
         <f>8*(O4/B4)^2</f>
-        <v>5.6780926707482096E-3</v>
+        <v>5.3922275323105423E-3</v>
       </c>
       <c r="R4" s="9">
         <f>(Q4-P4)/P4</f>
-        <v>2.0299215336261067E-2</v>
+        <v>-3.106802950328294E-2</v>
       </c>
       <c r="S4" s="7">
         <f>1700*O4/B4</f>
-        <v>45.29029672355648</v>
+        <v>44.135498139787479</v>
       </c>
       <c r="T4" s="3">
         <f>B4/4*P4</f>
@@ -19941,7 +19938,7 @@
       </c>
       <c r="U4" s="7">
         <f>E4*N4</f>
-        <v>105.5</v>
+        <v>26.375</v>
       </c>
       <c r="V4" s="7">
         <f>F4*N4</f>
@@ -19952,7 +19949,8 @@
         <v>26.375</v>
       </c>
       <c r="X4" s="7">
-        <v>26.4</v>
+        <f>H4*N4</f>
+        <v>26.375</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
cmpt_wallmodelbc works for channel
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mchao\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D71E91-E6F7-43B0-AC9D-E86F0C7B01BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF9AF34-CEF5-4557-B8F6-8605ED7A51F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="3" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="6" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="DUC_RETAU1000" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2009,7 +2010,7 @@
   <dimension ref="A1:X59"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4488,7 +4489,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B745900-CF34-4783-B8B3-D2DA1ADCC55F}">
   <dimension ref="A1:X29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S51" sqref="S51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -11698,8 +11701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE42F51E-90FA-449F-904F-669D9897EDC7}">
   <dimension ref="A1:X134"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E117" sqref="E117:F117"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="P112" sqref="P112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
bug in dw, dw(0:1,1:3) replaced by dw(6)
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mchao\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6019DD-4204-4E78-BDBE-7EBD4A267C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02FFDC0-6EAE-4FA0-BA78-876E67878BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="1" activeTab="2" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="781" activeTab="9" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
   <sheets>
     <sheet name="debug" sheetId="1" r:id="rId1"/>
@@ -22,8 +22,10 @@
     <sheet name="CHA_RETAU5200" sheetId="6" r:id="rId7"/>
     <sheet name="DUC_RETAU150" sheetId="11" r:id="rId8"/>
     <sheet name="DUC_RETAU1000" sheetId="12" r:id="rId9"/>
+    <sheet name="profile" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="234">
   <si>
     <t>channel, two walls</t>
   </si>
@@ -743,6 +745,33 @@
   </si>
   <si>
     <t>512×160×160</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>SMAG</t>
+  </si>
+  <si>
+    <t>DSMAG</t>
+  </si>
+  <si>
+    <t>SMAG-WM</t>
+  </si>
+  <si>
+    <t>DSMAG-WM</t>
+  </si>
+  <si>
+    <t>EXPLICIT</t>
+  </si>
+  <si>
+    <t>IMPLICIT3D</t>
+  </si>
+  <si>
+    <t>CPU(32)</t>
+  </si>
+  <si>
+    <t>cpu smag and dsmag can be divergent</t>
   </si>
 </sst>
 </file>
@@ -812,7 +841,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -879,6 +908,7 @@
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1970,12 +2000,270 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F0399A-8EF1-4A26-BF60-05A47F07A583}">
+  <dimension ref="A2:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.08984375" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3">
+        <v>1.49</v>
+      </c>
+      <c r="C3">
+        <v>0.11</v>
+      </c>
+      <c r="D3">
+        <f>B3/0.11*32</f>
+        <v>433.45454545454544</v>
+      </c>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D7" si="0">B4/0.11*32</f>
+        <v>674.90909090909088</v>
+      </c>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C5">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1192.7272727272725</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="C6">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>674.90909090909088</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C7">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1192.7272727272725</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="C11">
+        <v>0.18</v>
+      </c>
+      <c r="D11">
+        <f>B11/C11*32</f>
+        <v>387.5555555555556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" s="34">
+        <v>3.21</v>
+      </c>
+      <c r="C12">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:D21" si="1">B12/C12*32</f>
+        <v>501.07317073170736</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13">
+        <v>4.83</v>
+      </c>
+      <c r="C13">
+        <v>0.43</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>359.44186046511629</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>228</v>
+      </c>
+      <c r="C14">
+        <v>0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C15">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18" t="s">
+        <v>232</v>
+      </c>
+      <c r="C18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19">
+        <v>4.09</v>
+      </c>
+      <c r="C19">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>488.35820895522386</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>226</v>
+      </c>
+      <c r="B20">
+        <v>4.67</v>
+      </c>
+      <c r="C20">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>510.03412969283278</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>227</v>
+      </c>
+      <c r="B21">
+        <v>6.79</v>
+      </c>
+      <c r="C21">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>419.45945945945942</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>228</v>
+      </c>
+      <c r="C22">
+        <v>0.29299999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>229</v>
+      </c>
+      <c r="C23">
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B65B28-909F-4DCB-A7FC-99B4B3E29597}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2008,8 +2296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797B825A-8F5D-4559-BC02-F7413FCCDF08}">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19612,7 +19900,7 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
bug fixed, p1d(:) = 0._rp initialized in ave1d_channel
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mchao\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02FFDC0-6EAE-4FA0-BA78-876E67878BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFF6594-6650-43FF-81C9-E3ADC0DC66D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="781" activeTab="9" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="233">
   <si>
     <t>channel, two walls</t>
   </si>
@@ -769,9 +769,6 @@
   </si>
   <si>
     <t>CPU(32)</t>
-  </si>
-  <si>
-    <t>cpu smag and dsmag can be divergent</t>
   </si>
 </sst>
 </file>
@@ -2002,10 +1999,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F0399A-8EF1-4A26-BF60-05A47F07A583}">
-  <dimension ref="A2:H26"/>
+  <dimension ref="A2:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2135,14 +2132,14 @@
         <v>226</v>
       </c>
       <c r="B12" s="34">
-        <v>3.21</v>
+        <v>3.44</v>
       </c>
       <c r="C12">
         <v>0.20499999999999999</v>
       </c>
       <c r="D12">
         <f t="shared" ref="D12:D21" si="1">B12/C12*32</f>
-        <v>501.07317073170736</v>
+        <v>536.97560975609758</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -2150,14 +2147,14 @@
         <v>227</v>
       </c>
       <c r="B13">
-        <v>4.83</v>
+        <v>4.72</v>
       </c>
       <c r="C13">
         <v>0.43</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>359.44186046511629</v>
+        <v>351.25581395348837</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -2192,14 +2189,14 @@
         <v>147</v>
       </c>
       <c r="B19">
-        <v>4.09</v>
+        <v>4.18</v>
       </c>
       <c r="C19">
         <v>0.26800000000000002</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>488.35820895522386</v>
+        <v>499.10447761194024</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -2207,14 +2204,14 @@
         <v>226</v>
       </c>
       <c r="B20">
-        <v>4.67</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C20">
         <v>0.29299999999999998</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>510.03412969283278</v>
+        <v>535.15358361774747</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -2246,11 +2243,6 @@
       </c>
       <c r="C23">
         <v>0.51800000000000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
-        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fixed, ave1d,ave2d,out1d_chan.out2d_duct initialized with zero
</commit_message>
<xml_diff>
--- a/docs/note.xlsx
+++ b/docs/note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mchao\code\CaNS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFF6594-6650-43FF-81C9-E3ADC0DC66D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAB7EE9-8121-4A41-B2FD-10A1745BC480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="781" activeTab="9" xr2:uid="{01D2C22A-6FDC-4C8A-89EA-CFEF89D4AB13}"/>
   </bookViews>
@@ -25,7 +25,6 @@
     <sheet name="profile" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -838,7 +837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -905,7 +904,6 @@
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2002,7 +2000,7 @@
   <dimension ref="A2:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2131,7 +2129,7 @@
       <c r="A12" t="s">
         <v>226</v>
       </c>
-      <c r="B12" s="34">
+      <c r="B12">
         <v>3.44</v>
       </c>
       <c r="C12">

</xml_diff>